<commit_message>
Committing the test new update
</commit_message>
<xml_diff>
--- a/data/CRM_Testdata.xlsx
+++ b/data/CRM_Testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\vkamalak\git\OnPremise\Dynamics-CRM-Stage\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3314F2-52B1-4479-91EE-893A7DBB78E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA73FD5-CA8E-4B8F-BE9C-31487DB4A5C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="599" xr2:uid="{442E3441-3F3C-4A77-BB17-E93CAE512719}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1912" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2872" uniqueCount="482">
   <si>
     <t>UserName</t>
   </si>
@@ -1310,93 +1310,9 @@
     <t>2000531540</t>
   </si>
   <si>
-    <t>2000531679</t>
-  </si>
-  <si>
-    <t>2000531680</t>
-  </si>
-  <si>
-    <t>2000531681</t>
-  </si>
-  <si>
-    <t>2000531682</t>
-  </si>
-  <si>
-    <t>2000531685</t>
-  </si>
-  <si>
-    <t>2000531687</t>
-  </si>
-  <si>
-    <t>2000531688</t>
-  </si>
-  <si>
-    <t>2000531689</t>
-  </si>
-  <si>
-    <t>2000531692</t>
-  </si>
-  <si>
-    <t>2000531693</t>
-  </si>
-  <si>
-    <t>2000531696</t>
-  </si>
-  <si>
-    <t>551726561</t>
-  </si>
-  <si>
-    <t>hf1741188</t>
-  </si>
-  <si>
-    <t>2000531697</t>
-  </si>
-  <si>
-    <t>2000531698</t>
-  </si>
-  <si>
-    <t>2000531699</t>
-  </si>
-  <si>
-    <t>2000531700</t>
-  </si>
-  <si>
-    <t>2000531701</t>
-  </si>
-  <si>
-    <t>2000531702</t>
-  </si>
-  <si>
-    <t>2000531703</t>
-  </si>
-  <si>
     <t>2000531704</t>
   </si>
   <si>
-    <t>7000572471</t>
-  </si>
-  <si>
-    <t>7000572472</t>
-  </si>
-  <si>
-    <t>7000572473</t>
-  </si>
-  <si>
-    <t>7000572474</t>
-  </si>
-  <si>
-    <t>7000572475</t>
-  </si>
-  <si>
-    <t>7000572476</t>
-  </si>
-  <si>
-    <t>7000572477</t>
-  </si>
-  <si>
-    <t>http://c3dicrmv9app1/CRMDevV9/main.aspx#</t>
-  </si>
-  <si>
     <t>TFS ID_ 7112:Verify if primary account of a contact has been changed then other associated Contact account association should not get end dated/terminated</t>
   </si>
   <si>
@@ -1406,16 +1322,169 @@
     <t/>
   </si>
   <si>
+    <t>https://crmstage.premierinc.com/main.aspx#7815483</t>
+  </si>
+  <si>
+    <t>PASSED</t>
+  </si>
+  <si>
+    <t>2000533106</t>
+  </si>
+  <si>
+    <t>2000533107</t>
+  </si>
+  <si>
+    <t>2000533108</t>
+  </si>
+  <si>
+    <t>2000533109</t>
+  </si>
+  <si>
+    <t>2000533112</t>
+  </si>
+  <si>
+    <t>2000533114</t>
+  </si>
+  <si>
+    <t>2000533118</t>
+  </si>
+  <si>
+    <t>2000533120</t>
+  </si>
+  <si>
+    <t>2000533124</t>
+  </si>
+  <si>
+    <t>806388670</t>
+  </si>
+  <si>
+    <t>cf8233998</t>
+  </si>
+  <si>
+    <t>2000533125</t>
+  </si>
+  <si>
+    <t>2000533126</t>
+  </si>
+  <si>
+    <t>2000533127</t>
+  </si>
+  <si>
+    <t>2000533129</t>
+  </si>
+  <si>
+    <t>2000533130</t>
+  </si>
+  <si>
+    <t>2000533131</t>
+  </si>
+  <si>
+    <t>2000533132</t>
+  </si>
+  <si>
+    <t>7000572993</t>
+  </si>
+  <si>
+    <t>7000572994</t>
+  </si>
+  <si>
+    <t>7000572995</t>
+  </si>
+  <si>
+    <t>7000572996</t>
+  </si>
+  <si>
+    <t>7000572997</t>
+  </si>
+  <si>
+    <t>7000572998</t>
+  </si>
+  <si>
+    <t>7000572999</t>
+  </si>
+  <si>
+    <t>2000533147</t>
+  </si>
+  <si>
+    <t>2000533152</t>
+  </si>
+  <si>
+    <t>2022_05_30_04_34_45</t>
+  </si>
+  <si>
     <t>Failed</t>
   </si>
   <si>
-    <t>2022_04_13_03_36_07</t>
-  </si>
-  <si>
-    <t>2022_04_13_03_36_47</t>
-  </si>
-  <si>
-    <t>2022_04_19_11_08_52</t>
+    <t>2022_05_30_05_15_22</t>
+  </si>
+  <si>
+    <t>2000533156</t>
+  </si>
+  <si>
+    <t>2022_05_30_05_24_42</t>
+  </si>
+  <si>
+    <t>2000533157</t>
+  </si>
+  <si>
+    <t>2022_05_30_05_33_00</t>
+  </si>
+  <si>
+    <t>2000533160</t>
+  </si>
+  <si>
+    <t>2022_05_30_06_00_55</t>
+  </si>
+  <si>
+    <t>2000533162</t>
+  </si>
+  <si>
+    <t>2000533163</t>
+  </si>
+  <si>
+    <t>2022_05_30_06_09_11</t>
+  </si>
+  <si>
+    <t>2000533164</t>
+  </si>
+  <si>
+    <t>2000533165</t>
+  </si>
+  <si>
+    <t>2022_05_30_06_43_41</t>
+  </si>
+  <si>
+    <t>2000533166</t>
+  </si>
+  <si>
+    <t>2000533167</t>
+  </si>
+  <si>
+    <t>2022_05_30_06_56_05</t>
+  </si>
+  <si>
+    <t>2000533168</t>
+  </si>
+  <si>
+    <t>2022_05_30_07_14_51</t>
+  </si>
+  <si>
+    <t>2000533169</t>
+  </si>
+  <si>
+    <t>2022_05_30_07_24_57</t>
+  </si>
+  <si>
+    <t>2000533170</t>
+  </si>
+  <si>
+    <t>2022_05_30_07_43_14</t>
+  </si>
+  <si>
+    <t>2000533171</t>
+  </si>
+  <si>
+    <t>2022_05_30_08_04_09</t>
   </si>
 </sst>
 </file>
@@ -1576,7 +1645,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1621,23 +1690,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1756,8 +1814,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2079,10 +2135,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088699A3-39D2-44E6-8F71-47C2709580BF}">
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2135,7 +2191,7 @@
         <v>58</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D2" s="19" t="s">
         <v>9</v>
@@ -2144,16 +2200,16 @@
         <v>62</v>
       </c>
       <c r="F2" s="63" t="s">
-        <v>455</v>
+        <v>425</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>458</v>
+        <v>426</v>
       </c>
       <c r="H2" s="19" t="s">
-        <v>423</v>
+        <v>429</v>
       </c>
       <c r="I2" s="50" t="s">
-        <v>451</v>
+        <v>427</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2173,13 +2229,13 @@
         <v>62</v>
       </c>
       <c r="F3" s="63" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="I3" s="61"/>
     </row>
@@ -2200,13 +2256,13 @@
         <v>62</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H4" s="19" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="I4" s="19"/>
     </row>
@@ -2227,13 +2283,13 @@
         <v>62</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="I5" s="19"/>
     </row>
@@ -2254,10 +2310,10 @@
         <v>62</v>
       </c>
       <c r="F6" s="63" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
@@ -2279,10 +2335,10 @@
         <v>62</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
@@ -2304,13 +2360,13 @@
         <v>62</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>427</v>
+        <v>455</v>
       </c>
       <c r="I8" s="19"/>
     </row>
@@ -2331,10 +2387,10 @@
         <v>62</v>
       </c>
       <c r="F9" s="63" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
@@ -2356,13 +2412,13 @@
         <v>62</v>
       </c>
       <c r="F10" s="63" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>428</v>
+        <v>433</v>
       </c>
       <c r="I10" s="19"/>
     </row>
@@ -2383,13 +2439,13 @@
         <v>62</v>
       </c>
       <c r="F11" s="63" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G11" s="19" t="s">
+        <v>426</v>
+      </c>
+      <c r="H11" s="19" t="s">
         <v>454</v>
-      </c>
-      <c r="H11" s="19" t="s">
-        <v>429</v>
       </c>
       <c r="I11" s="19"/>
     </row>
@@ -2410,13 +2466,13 @@
         <v>62</v>
       </c>
       <c r="F12" s="63" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G12" s="19" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H12" s="19" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="I12" s="19"/>
     </row>
@@ -2437,10 +2493,10 @@
         <v>62</v>
       </c>
       <c r="F13" s="63" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G13" s="19" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H13" s="19"/>
       <c r="I13" s="19"/>
@@ -2462,10 +2518,10 @@
         <v>62</v>
       </c>
       <c r="F14" s="63" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G14" s="19" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H14" s="19"/>
       <c r="I14" s="19"/>
@@ -2487,13 +2543,13 @@
         <v>62</v>
       </c>
       <c r="F15" s="63" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H15" s="19" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="I15" s="19"/>
     </row>
@@ -2514,13 +2570,13 @@
         <v>62</v>
       </c>
       <c r="F16" s="63" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H16" s="19" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="I16" s="19"/>
     </row>
@@ -2541,10 +2597,10 @@
         <v>110</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G17" s="19" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="19"/>
@@ -2566,10 +2622,10 @@
         <v>110</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="19"/>
@@ -2591,10 +2647,10 @@
         <v>110</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G19" s="19" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H19" s="19"/>
       <c r="I19" s="19"/>
@@ -2616,10 +2672,10 @@
         <v>62</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G20" s="19" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H20" s="19"/>
       <c r="I20" s="19"/>
@@ -2641,13 +2697,13 @@
         <v>62</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G21" s="19" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H21" s="19" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="I21" s="19"/>
     </row>
@@ -2668,13 +2724,13 @@
         <v>62</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G22" s="19" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H22" s="19" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="I22" s="19"/>
     </row>
@@ -2695,13 +2751,13 @@
         <v>62</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G23" s="19" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H23" s="19" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="I23" s="19"/>
     </row>
@@ -2722,13 +2778,13 @@
         <v>62</v>
       </c>
       <c r="F24" s="19" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G24" s="19" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H24" s="19" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="I24" s="19"/>
     </row>
@@ -2749,13 +2805,13 @@
         <v>62</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G25" s="19" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H25" s="19" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="I25" s="19"/>
     </row>
@@ -2776,13 +2832,13 @@
         <v>62</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G26" s="19" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H26" s="19" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="I26" s="19"/>
     </row>
@@ -2803,13 +2859,13 @@
         <v>62</v>
       </c>
       <c r="F27" s="19" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G27" s="19" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H27" s="19" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="I27" s="19"/>
     </row>
@@ -2830,13 +2886,13 @@
         <v>62</v>
       </c>
       <c r="F28" s="19" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G28" s="19" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H28" s="65" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="I28" s="19"/>
     </row>
@@ -2857,10 +2913,10 @@
         <v>62</v>
       </c>
       <c r="F29" s="19" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G29" s="19" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H29" s="19"/>
       <c r="I29" s="19"/>
@@ -2873,7 +2929,7 @@
         <v>414</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D30" s="19" t="s">
         <v>9</v>
@@ -2882,19 +2938,19 @@
         <v>62</v>
       </c>
       <c r="F30" s="19" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="G30" s="19" t="s">
-        <v>454</v>
+        <v>481</v>
       </c>
       <c r="H30" s="19" t="s">
-        <v>443</v>
+        <v>480</v>
       </c>
       <c r="I30" s="19"/>
     </row>
     <row r="31" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="21">
-        <v>29</v>
+      <c r="A31" s="19">
+        <v>30</v>
       </c>
       <c r="B31" s="21" t="s">
         <v>51</v>
@@ -2909,17 +2965,17 @@
         <v>62</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G31" s="21" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H31" s="21"/>
       <c r="I31" s="22"/>
     </row>
     <row r="32" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="21">
-        <v>30</v>
+      <c r="A32" s="19">
+        <v>31</v>
       </c>
       <c r="B32" s="21" t="s">
         <v>127</v>
@@ -2934,17 +2990,17 @@
         <v>62</v>
       </c>
       <c r="F32" s="63" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G32" s="21" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H32" s="21"/>
       <c r="I32" s="22"/>
     </row>
     <row r="33" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="21">
-        <v>31</v>
+      <c r="A33" s="19">
+        <v>32</v>
       </c>
       <c r="B33" s="21" t="s">
         <v>132</v>
@@ -2959,17 +3015,17 @@
         <v>62</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G33" s="21" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H33" s="21"/>
       <c r="I33" s="22"/>
     </row>
     <row r="34" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="21">
-        <v>32</v>
+      <c r="A34" s="19">
+        <v>33</v>
       </c>
       <c r="B34" s="21" t="s">
         <v>139</v>
@@ -2984,17 +3040,17 @@
         <v>62</v>
       </c>
       <c r="F34" s="63" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G34" s="21" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H34" s="21"/>
       <c r="I34" s="22"/>
     </row>
     <row r="35" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="21">
-        <v>33</v>
+      <c r="A35" s="19">
+        <v>34</v>
       </c>
       <c r="B35" s="21" t="s">
         <v>144</v>
@@ -3009,17 +3065,17 @@
         <v>62</v>
       </c>
       <c r="F35" s="63" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G35" s="21" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H35" s="21"/>
       <c r="I35" s="22"/>
     </row>
     <row r="36" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="21">
-        <v>34</v>
+      <c r="A36" s="19">
+        <v>35</v>
       </c>
       <c r="B36" s="21" t="s">
         <v>149</v>
@@ -3034,17 +3090,17 @@
         <v>62</v>
       </c>
       <c r="F36" s="21" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G36" s="21" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H36" s="21"/>
       <c r="I36" s="22"/>
     </row>
     <row r="37" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="21">
-        <v>35</v>
+      <c r="A37" s="19">
+        <v>36</v>
       </c>
       <c r="B37" s="21" t="s">
         <v>153</v>
@@ -3059,17 +3115,17 @@
         <v>62</v>
       </c>
       <c r="F37" s="21" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G37" s="21" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H37" s="21"/>
       <c r="I37" s="22"/>
     </row>
     <row r="38" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="21">
-        <v>36</v>
+      <c r="A38" s="19">
+        <v>37</v>
       </c>
       <c r="B38" s="21" t="s">
         <v>158</v>
@@ -3084,17 +3140,17 @@
         <v>62</v>
       </c>
       <c r="F38" s="21" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G38" s="21" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H38" s="21"/>
       <c r="I38" s="22"/>
     </row>
     <row r="39" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="21">
-        <v>37</v>
+      <c r="A39" s="19">
+        <v>38</v>
       </c>
       <c r="B39" s="21" t="s">
         <v>161</v>
@@ -3109,17 +3165,17 @@
         <v>62</v>
       </c>
       <c r="F39" s="21" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G39" s="21" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H39" s="21"/>
       <c r="I39" s="22"/>
     </row>
     <row r="40" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="21">
-        <v>38</v>
+      <c r="A40" s="19">
+        <v>39</v>
       </c>
       <c r="B40" s="21" t="s">
         <v>164</v>
@@ -3134,17 +3190,17 @@
         <v>62</v>
       </c>
       <c r="F40" s="21" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G40" s="21" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H40" s="21"/>
       <c r="I40" s="22"/>
     </row>
     <row r="41" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="21">
-        <v>39</v>
+      <c r="A41" s="19">
+        <v>40</v>
       </c>
       <c r="B41" s="21" t="s">
         <v>169</v>
@@ -3159,17 +3215,17 @@
         <v>62</v>
       </c>
       <c r="F41" s="21" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G41" s="21" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H41" s="21"/>
       <c r="I41" s="22"/>
     </row>
     <row r="42" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="21">
-        <v>40</v>
+      <c r="A42" s="19">
+        <v>41</v>
       </c>
       <c r="B42" s="21" t="s">
         <v>176</v>
@@ -3184,17 +3240,17 @@
         <v>62</v>
       </c>
       <c r="F42" s="21" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G42" s="21" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H42" s="21"/>
       <c r="I42" s="22"/>
     </row>
     <row r="43" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="21">
-        <v>41</v>
+      <c r="A43" s="19">
+        <v>42</v>
       </c>
       <c r="B43" s="21" t="s">
         <v>183</v>
@@ -3209,17 +3265,17 @@
         <v>62</v>
       </c>
       <c r="F43" s="21" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G43" s="21" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H43" s="21"/>
       <c r="I43" s="22"/>
     </row>
     <row r="44" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="21">
-        <v>42</v>
+      <c r="A44" s="19">
+        <v>43</v>
       </c>
       <c r="B44" s="21" t="s">
         <v>378</v>
@@ -3234,17 +3290,17 @@
         <v>62</v>
       </c>
       <c r="F44" s="21" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G44" s="21" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H44" s="21"/>
       <c r="I44" s="22"/>
     </row>
     <row r="45" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="21">
-        <v>43</v>
+      <c r="A45" s="19">
+        <v>44</v>
       </c>
       <c r="B45" s="21" t="s">
         <v>268</v>
@@ -3259,17 +3315,17 @@
         <v>62</v>
       </c>
       <c r="F45" s="21" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G45" s="21" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H45" s="21"/>
       <c r="I45" s="22"/>
     </row>
     <row r="46" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="62">
-        <v>44</v>
+      <c r="A46" s="19">
+        <v>45</v>
       </c>
       <c r="B46" s="62" t="s">
         <v>307</v>
@@ -3284,19 +3340,19 @@
         <v>306</v>
       </c>
       <c r="F46" s="62" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G46" s="62" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H46" s="62" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="I46" s="62"/>
     </row>
     <row r="47" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="62">
-        <v>45</v>
+      <c r="A47" s="19">
+        <v>46</v>
       </c>
       <c r="B47" s="62" t="s">
         <v>311</v>
@@ -3311,19 +3367,19 @@
         <v>306</v>
       </c>
       <c r="F47" s="62" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G47" s="62" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H47" s="62" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="I47" s="62"/>
     </row>
     <row r="48" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="62">
-        <v>46</v>
+      <c r="A48" s="19">
+        <v>47</v>
       </c>
       <c r="B48" s="62" t="s">
         <v>310</v>
@@ -3338,19 +3394,19 @@
         <v>306</v>
       </c>
       <c r="F48" s="62" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G48" s="62" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H48" s="62" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="I48" s="62"/>
     </row>
     <row r="49" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="62">
-        <v>47</v>
+      <c r="A49" s="19">
+        <v>48</v>
       </c>
       <c r="B49" s="62" t="s">
         <v>325</v>
@@ -3365,19 +3421,19 @@
         <v>306</v>
       </c>
       <c r="F49" s="62" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G49" s="62" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H49" s="62" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="I49" s="62"/>
     </row>
     <row r="50" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="62">
-        <v>48</v>
+      <c r="A50" s="19">
+        <v>49</v>
       </c>
       <c r="B50" s="62" t="s">
         <v>335</v>
@@ -3392,19 +3448,19 @@
         <v>306</v>
       </c>
       <c r="F50" s="62" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G50" s="62" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H50" s="62" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="I50" s="62"/>
     </row>
     <row r="51" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="62">
-        <v>49</v>
+      <c r="A51" s="19">
+        <v>50</v>
       </c>
       <c r="B51" s="62" t="s">
         <v>334</v>
@@ -3419,17 +3475,17 @@
         <v>306</v>
       </c>
       <c r="F51" s="62" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G51" s="62" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H51" s="62"/>
       <c r="I51" s="62"/>
     </row>
     <row r="52" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="62">
-        <v>50</v>
+      <c r="A52" s="19">
+        <v>51</v>
       </c>
       <c r="B52" s="62" t="s">
         <v>331</v>
@@ -3444,17 +3500,17 @@
         <v>306</v>
       </c>
       <c r="F52" s="62" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G52" s="62" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H52" s="62"/>
       <c r="I52" s="62"/>
     </row>
     <row r="53" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="62">
-        <v>51</v>
+      <c r="A53" s="19">
+        <v>52</v>
       </c>
       <c r="B53" s="62" t="s">
         <v>341</v>
@@ -3469,19 +3525,19 @@
         <v>306</v>
       </c>
       <c r="F53" s="62" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="G53" s="62" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="H53" s="62" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="I53" s="62"/>
     </row>
     <row r="54" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="62">
-        <v>52</v>
+      <c r="A54" s="19">
+        <v>53</v>
       </c>
       <c r="B54" s="63" t="s">
         <v>342</v>
@@ -3496,38 +3552,15 @@
         <v>306</v>
       </c>
       <c r="F54" s="62" t="s">
+        <v>425</v>
+      </c>
+      <c r="G54" s="62" t="s">
+        <v>426</v>
+      </c>
+      <c r="H54" s="62" t="s">
         <v>453</v>
       </c>
-      <c r="G54" s="62" t="s">
-        <v>454</v>
-      </c>
-      <c r="H54" s="62" t="s">
-        <v>450</v>
-      </c>
       <c r="I54" s="62"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="66">
-        <v>53</v>
-      </c>
-      <c r="B55" s="63" t="s">
-        <v>452</v>
-      </c>
-      <c r="C55" s="67" t="s">
-        <v>56</v>
-      </c>
-      <c r="D55" s="66" t="s">
-        <v>9</v>
-      </c>
-      <c r="E55" s="62" t="s">
-        <v>306</v>
-      </c>
-      <c r="F55" s="66" t="s">
-        <v>455</v>
-      </c>
-      <c r="G55" t="s">
-        <v>457</v>
-      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:I54" xr:uid="{82E42E5A-9B39-4AEF-85C9-780A007CE908}"/>
@@ -3537,7 +3570,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{1B330AB7-A328-42B1-9088-FD495E692864}"/>
+    <hyperlink ref="I2" r:id="rId1" location="7815483" xr:uid="{1B330AB7-A328-42B1-9088-FD495E692864}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -7714,10 +7747,10 @@
         <v>57</v>
       </c>
       <c r="CN22" s="16" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="CO22" s="16" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c r="CP22" s="31" t="s">
         <v>57</v>
@@ -8766,7 +8799,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="63" t="s">
-        <v>452</v>
+        <v>424</v>
       </c>
       <c r="C31" s="26" t="s">
         <v>84</v>

</xml_diff>

<commit_message>
Committing Member Test cases
</commit_message>
<xml_diff>
--- a/data/CRM_Testdata.xlsx
+++ b/data/CRM_Testdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\vkamalak\git\OnPremise\Dynamics-CRM-Stage\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF20FA0-6930-46CB-9F1B-04134F278AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A52895-34A8-4E1D-9A8C-E4939E0BC7D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="599" activeTab="1" xr2:uid="{442E3441-3F3C-4A77-BB17-E93CAE512719}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1714" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2495" uniqueCount="510">
   <si>
     <t>UserName</t>
   </si>
@@ -1325,15 +1325,6 @@
     <t/>
   </si>
   <si>
-    <t>2000554807</t>
-  </si>
-  <si>
-    <t>2000554808</t>
-  </si>
-  <si>
-    <t>2000554810</t>
-  </si>
-  <si>
     <t>2000554812</t>
   </si>
   <si>
@@ -1367,9 +1358,6 @@
     <t>7000578829</t>
   </si>
   <si>
-    <t>2000554839</t>
-  </si>
-  <si>
     <t>2000554844</t>
   </si>
   <si>
@@ -1382,12 +1370,6 @@
     <t>bf9746162</t>
   </si>
   <si>
-    <t>2000555255</t>
-  </si>
-  <si>
-    <t>PASSED</t>
-  </si>
-  <si>
     <t>2000555263</t>
   </si>
   <si>
@@ -1412,19 +1394,181 @@
     <t>corp\crmtest10</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>2000555450</t>
-  </si>
-  <si>
-    <t>2022_10_19_06_02_50</t>
-  </si>
-  <si>
-    <t>2000555556</t>
-  </si>
-  <si>
-    <t>Mani sub 26OCT_</t>
+    <t>10/30/2022</t>
+  </si>
+  <si>
+    <t>2000555818</t>
+  </si>
+  <si>
+    <t>2000555819</t>
+  </si>
+  <si>
+    <t>2000555820</t>
+  </si>
+  <si>
+    <t>2000555823</t>
+  </si>
+  <si>
+    <t>TFS ID_45306:Verify Prospect accounts can not be published</t>
+  </si>
+  <si>
+    <t>45306_PublishProspectAccount</t>
+  </si>
+  <si>
+    <t>2000555831</t>
+  </si>
+  <si>
+    <t>You should not publish the prospect If you contact support, please provide the technical details.</t>
+  </si>
+  <si>
+    <t>TFS ID_45307:Verify if Accounts cannot be created directly in Terminated Status.</t>
+  </si>
+  <si>
+    <t>2000555837</t>
+  </si>
+  <si>
+    <t>Please do not create account with Terminated Account status If you contact support, please provide the technical details.</t>
+  </si>
+  <si>
+    <t>45307_CreateTerminateAccount</t>
+  </si>
+  <si>
+    <t>Please terminate the account by end dating the membership If you contact support, please provide the technical details.</t>
+  </si>
+  <si>
+    <t>2000316252</t>
+  </si>
+  <si>
+    <t>2000555870</t>
+  </si>
+  <si>
+    <t>45332_VerifyParticipationType</t>
+  </si>
+  <si>
+    <t>Cater</t>
+  </si>
+  <si>
+    <t>TFS ID_45332:Verify whether "Cater" is available in the "Participation Type" Field in Member Form and Member Entry Form.</t>
+  </si>
+  <si>
+    <t>TFS ID_45311:Verify whether child Account cannot be published if DP does not have entity code</t>
+  </si>
+  <si>
+    <t>1000190617</t>
+  </si>
+  <si>
+    <t>45311_SubAccWithoutEntity</t>
+  </si>
+  <si>
+    <t>You cannot publish the Member since Direct Parent has no Entity code If you contact support, please provide the technical details.</t>
+  </si>
+  <si>
+    <t>2000555900</t>
+  </si>
+  <si>
+    <t>TFS ID_45308:Verify user should not be allowed to change the account status to Active manually when Premier End date is present</t>
+  </si>
+  <si>
+    <t>1000031212</t>
+  </si>
+  <si>
+    <t>Please re-activate the account by creating the membership If you contact support, please provide the technical details.</t>
+  </si>
+  <si>
+    <t>TFS ID_45304:Verify if the State field in address only accept two characters or blank values, no numeric and/or special characters</t>
+  </si>
+  <si>
+    <t>TFS ID_45292:Verify whether user is able to "deactivate" Premier Membership in Published state when there is no other active Premier Membership.</t>
+  </si>
+  <si>
+    <t>1000003540</t>
+  </si>
+  <si>
+    <t>State/Province must be 2 Characters long or Empty</t>
+  </si>
+  <si>
+    <t>State/Province must contain only characters</t>
+  </si>
+  <si>
+    <t>Can't deactivate the premier membership since there is no other active premier membership</t>
+  </si>
+  <si>
+    <t>TFS ID_45309: Verify whether DP Exception Reason is not required, while creating new account from sub account entity</t>
+  </si>
+  <si>
+    <t>45309_CreateSubAccountwithoutDPException</t>
+  </si>
+  <si>
+    <t>2000555965</t>
+  </si>
+  <si>
+    <t>TFS ID_45321:Verify DP Relation Date is cleared if Is Top Parent Is Set to Yes</t>
+  </si>
+  <si>
+    <t>TFS ID_43707: Cloud: Verify Top Parent Relation should be OLM for Top parent</t>
+  </si>
+  <si>
+    <t>CreateTopParent</t>
+  </si>
+  <si>
+    <t>LOB Status</t>
+  </si>
+  <si>
+    <t>TFS ID_43702: 11223_Cloud: Verify corresponding LOB is getting deactivated when end dated membership is deactivated</t>
+  </si>
+  <si>
+    <t>Top Parent Relationship for Top Parent must be OLM If you contact support, please provide the technical details.</t>
+  </si>
+  <si>
+    <t>Aparna sub Nov3_</t>
+  </si>
+  <si>
+    <t>2000555522</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>5/4/2021</t>
+  </si>
+  <si>
+    <t>2000556059</t>
+  </si>
+  <si>
+    <t>11/5/2022</t>
+  </si>
+  <si>
+    <t>11/3/2022</t>
+  </si>
+  <si>
+    <t>2000556107</t>
+  </si>
+  <si>
+    <t>2022_11_03_09_51_54</t>
+  </si>
+  <si>
+    <t>TFS ID_44710:Verify when ship to account converted to main account, CP and FSP updated.</t>
+  </si>
+  <si>
+    <t>44710_LocationtoMember</t>
+  </si>
+  <si>
+    <t>2000556112</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>2022_11_04_11_16_30</t>
+  </si>
+  <si>
+    <t>2000556113</t>
+  </si>
+  <si>
+    <t>2000556114</t>
+  </si>
+  <si>
+    <t>2022_11_04_01_49_12</t>
   </si>
 </sst>
 </file>
@@ -1669,7 +1813,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1791,6 +1935,12 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2112,24 +2262,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088699A3-39D2-44E6-8F71-47C2709580BF}">
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="93.42578125" style="7" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11" style="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.5703125" style="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.5703125" style="7" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.140625" style="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.28515625" style="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.28515625" style="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="32" style="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="16384" width="9.140625" style="7" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="7" width="5.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="7" width="93.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="7" width="11.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="7" width="15.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="7" width="15.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="7" width="8.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="7" width="20.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="7" width="12.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="7" width="32.0" collapsed="true"/>
+    <col min="10" max="16384" style="7" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -2184,7 +2334,7 @@
         <v>427</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>428</v>
+        <v>458</v>
       </c>
       <c r="I2" s="46" t="s">
         <v>416</v>
@@ -2216,7 +2366,7 @@
         <v>427</v>
       </c>
       <c r="H3" t="s">
-        <v>429</v>
+        <v>452</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2242,7 +2392,7 @@
         <v>427</v>
       </c>
       <c r="H4" t="s">
-        <v>442</v>
+        <v>453</v>
       </c>
       <c r="J4" s="46" t="s">
         <v>425</v>
@@ -2271,7 +2421,7 @@
         <v>427</v>
       </c>
       <c r="H5" t="s">
-        <v>430</v>
+        <v>454</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2343,7 +2493,7 @@
         <v>427</v>
       </c>
       <c r="H8" t="s">
-        <v>447</v>
+        <v>455</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2392,7 +2542,7 @@
         <v>427</v>
       </c>
       <c r="H10" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2418,7 +2568,7 @@
         <v>427</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2444,7 +2594,7 @@
         <v>427</v>
       </c>
       <c r="H12" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2516,7 +2666,7 @@
         <v>427</v>
       </c>
       <c r="H15" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2542,7 +2692,7 @@
         <v>427</v>
       </c>
       <c r="H16" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="61" customFormat="1" x14ac:dyDescent="0.25">
@@ -2660,7 +2810,7 @@
         <v>427</v>
       </c>
       <c r="H21" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2686,7 +2836,7 @@
         <v>427</v>
       </c>
       <c r="H22" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2712,7 +2862,7 @@
         <v>427</v>
       </c>
       <c r="H23" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2738,7 +2888,7 @@
         <v>427</v>
       </c>
       <c r="H24" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2764,7 +2914,7 @@
         <v>427</v>
       </c>
       <c r="H25" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2790,7 +2940,7 @@
         <v>427</v>
       </c>
       <c r="H26" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2816,7 +2966,7 @@
         <v>427</v>
       </c>
       <c r="H27" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2842,7 +2992,7 @@
         <v>427</v>
       </c>
       <c r="H28" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="61" customFormat="1" x14ac:dyDescent="0.25">
@@ -2876,7 +3026,7 @@
         <v>411</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D30" s="60" t="s">
         <v>8</v>
@@ -2885,13 +3035,13 @@
         <v>109</v>
       </c>
       <c r="F30" s="60" t="s">
-        <v>448</v>
+        <v>426</v>
       </c>
       <c r="G30" t="s">
-        <v>459</v>
+        <v>427</v>
       </c>
       <c r="H30" t="s">
-        <v>458</v>
+        <v>497</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="67" customFormat="1" x14ac:dyDescent="0.25">
@@ -3292,7 +3442,7 @@
         <v>427</v>
       </c>
       <c r="H46" s="69" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="I46" s="69"/>
     </row>
@@ -3319,7 +3469,7 @@
         <v>427</v>
       </c>
       <c r="H47" s="69" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="I47" s="69"/>
     </row>
@@ -3346,7 +3496,7 @@
         <v>427</v>
       </c>
       <c r="H48" s="69" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="I48" s="69"/>
     </row>
@@ -3373,7 +3523,7 @@
         <v>427</v>
       </c>
       <c r="H49" s="69" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="I49" s="69"/>
     </row>
@@ -3400,7 +3550,7 @@
         <v>427</v>
       </c>
       <c r="H50" s="69" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="I50" s="69"/>
     </row>
@@ -3477,7 +3627,7 @@
         <v>427</v>
       </c>
       <c r="H53" s="69" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="I53" s="69"/>
     </row>
@@ -3504,13 +3654,307 @@
         <v>427</v>
       </c>
       <c r="H54" s="69" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="I54" s="69"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="7">
+        <v>54</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="C55" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D55" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="F55" s="18" t="s">
+        <v>426</v>
+      </c>
+      <c r="G55" t="s">
+        <v>427</v>
+      </c>
+      <c r="H55" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="7">
+        <v>55</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D56" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="F56" s="18" t="s">
+        <v>426</v>
+      </c>
+      <c r="G56" t="s">
+        <v>427</v>
+      </c>
+      <c r="H56" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="7">
+        <v>56</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D57" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="F57" s="18" t="s">
+        <v>426</v>
+      </c>
+      <c r="G57" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="7">
+        <v>57</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="C58" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D58" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="F58" s="18" t="s">
+        <v>426</v>
+      </c>
+      <c r="G58" t="s">
+        <v>427</v>
+      </c>
+      <c r="H58" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="7">
+        <v>58</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D59" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="F59" s="18" t="s">
+        <v>426</v>
+      </c>
+      <c r="G59" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="7">
+        <v>59</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="C60" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D60" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="F60" s="18" t="s">
+        <v>426</v>
+      </c>
+      <c r="G60" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="7">
+        <v>60</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="C61" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D61" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="F61" s="18" t="s">
+        <v>426</v>
+      </c>
+      <c r="G61" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="7">
+        <v>61</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="C62" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D62" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="F62" s="18" t="s">
+        <v>426</v>
+      </c>
+      <c r="G62" t="s">
+        <v>427</v>
+      </c>
+      <c r="H62" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="7">
+        <v>62</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>487</v>
+      </c>
+      <c r="C63" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D63" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="F63" s="18" t="s">
+        <v>426</v>
+      </c>
+      <c r="G63" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="7">
+        <v>63</v>
+      </c>
+      <c r="B64" s="73" t="s">
+        <v>488</v>
+      </c>
+      <c r="C64" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D64" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="F64" s="18" t="s">
+        <v>426</v>
+      </c>
+      <c r="G64" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="7">
+        <v>64</v>
+      </c>
+      <c r="B65" s="74" t="s">
+        <v>491</v>
+      </c>
+      <c r="C65" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D65" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E65" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="F65" s="18" t="s">
+        <v>426</v>
+      </c>
+      <c r="G65" t="s">
+        <v>427</v>
+      </c>
+      <c r="H65" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="7">
+        <v>65</v>
+      </c>
+      <c r="B66" s="74" t="s">
+        <v>502</v>
+      </c>
+      <c r="C66" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D66" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E66" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="F66" s="18" t="s">
+        <v>505</v>
+      </c>
+      <c r="G66" t="s">
+        <v>509</v>
+      </c>
+      <c r="H66" t="s">
+        <v>508</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C54" xr:uid="{A24E4840-CF83-45B5-8B9C-FAE6253DDB86}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C66" xr:uid="{A24E4840-CF83-45B5-8B9C-FAE6253DDB86}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3526,98 +3970,98 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9856292-E718-4F44-A2EB-03A51CA4C0E1}">
-  <dimension ref="A1:DC31"/>
+  <dimension ref="A1:DZ43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="102.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="12.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="69.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="11" width="36.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="20.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="20" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="15.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="16.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="14.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="20.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="21.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="27.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="18.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="10.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="4.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="8" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="7.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="8.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="12.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="19.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="24.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="24.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="9.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="17.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="22.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="9.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="21.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="26.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="30.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="23.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="41" width="23.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="7.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="22.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="24.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="8.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="16.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="6" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="20.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="20.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="26.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="24.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="27" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="25" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="29" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="56" width="15.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="25.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="15.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="17.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="14.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="11.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="62" max="62" width="17.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="63" max="63" width="12.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="64" max="64" width="15.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="65" max="65" width="19.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="66" max="66" width="19.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="67" max="67" width="14.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="68" max="68" width="14.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="69" max="69" width="10.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="70" max="70" width="19.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="71" max="71" width="12.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="72" max="72" width="9.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="73" max="73" width="14.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="74" max="74" width="32" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="75" max="75" width="16.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="76" max="82" width="9.140625" style="2" collapsed="1"/>
-    <col min="83" max="83" width="10" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="84" max="95" width="9.140625" style="2" collapsed="1"/>
-    <col min="96" max="96" width="28.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="97" max="97" width="22.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="98" max="98" width="26.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="99" max="99" width="26.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="100" max="100" width="12.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="101" max="101" width="12.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="102" max="102" width="22.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="103" max="103" width="18.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="104" max="104" width="18.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="105" max="105" width="18.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="106" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="5.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="102.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="14.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="10.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="11.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="12.85546875" collapsed="true"/>
+    <col min="7" max="8" customWidth="true" style="2" width="12.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="69.140625" collapsed="true"/>
+    <col min="10" max="11" customWidth="true" style="2" width="36.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="20.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="15.42578125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="16.7109375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="14.7109375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="2" width="20.140625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="2" width="21.7109375" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="2" width="27.140625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="2" width="18.5703125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="2" width="10.42578125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="2" width="4.42578125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="2" width="8.0" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="2" width="7.28515625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="2" width="8.28515625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="2" width="19.85546875" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="2" width="24.140625" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" style="2" width="24.140625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="2" width="9.85546875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="2" width="17.85546875" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="2" width="22.140625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" style="2" width="9.5703125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" style="2" width="21.85546875" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" style="2" width="26.28515625" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" style="2" width="30.42578125" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" style="2" width="23.28515625" collapsed="true"/>
+    <col min="39" max="41" customWidth="true" style="2" width="23.28515625" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" style="2" width="7.28515625" collapsed="true"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" style="2" width="22.28515625" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" style="2" width="24.5703125" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" style="2" width="8.85546875" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" style="2" width="16.7109375" collapsed="true"/>
+    <col min="47" max="47" bestFit="true" customWidth="true" style="2" width="6.0" collapsed="true"/>
+    <col min="48" max="48" bestFit="true" customWidth="true" style="2" width="20.5703125" collapsed="true"/>
+    <col min="49" max="49" bestFit="true" customWidth="true" style="2" width="20.28515625" collapsed="true"/>
+    <col min="50" max="50" bestFit="true" customWidth="true" style="2" width="26.42578125" collapsed="true"/>
+    <col min="51" max="51" bestFit="true" customWidth="true" style="2" width="24.28515625" collapsed="true"/>
+    <col min="52" max="52" bestFit="true" customWidth="true" style="2" width="27.0" collapsed="true"/>
+    <col min="53" max="53" bestFit="true" customWidth="true" style="2" width="25.0" collapsed="true"/>
+    <col min="54" max="54" bestFit="true" customWidth="true" style="2" width="29.0" collapsed="true"/>
+    <col min="55" max="56" bestFit="true" customWidth="true" style="2" width="15.140625" collapsed="true"/>
+    <col min="57" max="57" bestFit="true" customWidth="true" style="2" width="25.5703125" collapsed="true"/>
+    <col min="58" max="58" bestFit="true" customWidth="true" style="2" width="15.7109375" collapsed="true"/>
+    <col min="59" max="59" bestFit="true" customWidth="true" style="2" width="17.85546875" collapsed="true"/>
+    <col min="60" max="60" bestFit="true" customWidth="true" style="2" width="14.5703125" collapsed="true"/>
+    <col min="61" max="61" bestFit="true" customWidth="true" style="2" width="11.85546875" collapsed="true"/>
+    <col min="62" max="62" bestFit="true" customWidth="true" style="2" width="17.28515625" collapsed="true"/>
+    <col min="63" max="63" bestFit="true" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
+    <col min="64" max="64" bestFit="true" customWidth="true" style="2" width="15.28515625" collapsed="true"/>
+    <col min="65" max="65" bestFit="true" customWidth="true" style="2" width="19.85546875" collapsed="true"/>
+    <col min="66" max="66" bestFit="true" customWidth="true" style="2" width="19.42578125" collapsed="true"/>
+    <col min="67" max="67" bestFit="true" customWidth="true" style="2" width="14.42578125" collapsed="true"/>
+    <col min="68" max="68" bestFit="true" customWidth="true" style="2" width="14.7109375" collapsed="true"/>
+    <col min="69" max="69" bestFit="true" customWidth="true" style="2" width="10.7109375" collapsed="true"/>
+    <col min="70" max="70" bestFit="true" customWidth="true" style="2" width="19.42578125" collapsed="true"/>
+    <col min="71" max="71" bestFit="true" customWidth="true" style="2" width="12.28515625" collapsed="true"/>
+    <col min="72" max="72" bestFit="true" customWidth="true" style="2" width="9.28515625" collapsed="true"/>
+    <col min="73" max="73" bestFit="true" customWidth="true" style="2" width="14.140625" collapsed="true"/>
+    <col min="74" max="74" bestFit="true" customWidth="true" style="2" width="32.0" collapsed="true"/>
+    <col min="75" max="75" bestFit="true" customWidth="true" style="2" width="16.28515625" collapsed="true"/>
+    <col min="76" max="82" style="2" width="9.140625" collapsed="true"/>
+    <col min="83" max="83" bestFit="true" customWidth="true" style="2" width="10.0" collapsed="true"/>
+    <col min="84" max="95" style="2" width="9.140625" collapsed="true"/>
+    <col min="96" max="96" customWidth="true" style="2" width="28.28515625" collapsed="true"/>
+    <col min="97" max="97" bestFit="true" customWidth="true" style="2" width="22.140625" collapsed="true"/>
+    <col min="98" max="98" bestFit="true" customWidth="true" style="2" width="26.140625" collapsed="true"/>
+    <col min="99" max="99" customWidth="true" style="2" width="26.140625" collapsed="true"/>
+    <col min="100" max="100" bestFit="true" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
+    <col min="101" max="101" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
+    <col min="102" max="102" bestFit="true" customWidth="true" style="2" width="22.85546875" collapsed="true"/>
+    <col min="103" max="103" bestFit="true" customWidth="true" style="2" width="18.140625" collapsed="true"/>
+    <col min="104" max="104" customWidth="true" style="2" width="18.140625" collapsed="true"/>
+    <col min="105" max="105" bestFit="true" customWidth="true" style="2" width="18.28515625" collapsed="true"/>
+    <col min="106" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:107" x14ac:dyDescent="0.25">
@@ -4329,7 +4773,7 @@
         <v>293</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>424</v>
@@ -6681,7 +7125,7 @@
       <c r="DA16" s="23"/>
       <c r="DB16" s="23"/>
     </row>
-    <row r="17" spans="1:107" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:109" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="23">
         <v>16</v>
       </c>
@@ -6863,7 +7307,7 @@
       <c r="DA17" s="23"/>
       <c r="DB17" s="23"/>
     </row>
-    <row r="18" spans="1:107" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:109" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="23">
         <v>17</v>
       </c>
@@ -7045,7 +7489,7 @@
       <c r="DA18" s="23"/>
       <c r="DB18" s="23"/>
     </row>
-    <row r="19" spans="1:107" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A19" s="23">
         <v>18</v>
       </c>
@@ -7221,7 +7665,7 @@
       <c r="DA19" s="28"/>
       <c r="DB19" s="28"/>
     </row>
-    <row r="20" spans="1:107" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A20" s="23">
         <v>19</v>
       </c>
@@ -7351,7 +7795,7 @@
       <c r="DA20" s="28"/>
       <c r="DB20" s="28"/>
     </row>
-    <row r="21" spans="1:107" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:109" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="30">
         <v>20</v>
       </c>
@@ -7495,7 +7939,7 @@
       <c r="DA21" s="39"/>
       <c r="DB21" s="39"/>
     </row>
-    <row r="22" spans="1:107" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A22" s="23">
         <v>21</v>
       </c>
@@ -7736,10 +8180,10 @@
         <v>56</v>
       </c>
       <c r="CN22" s="15" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="CO22" s="15" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="CP22" s="28" t="s">
         <v>56</v>
@@ -7765,7 +8209,7 @@
       <c r="DA22" s="28"/>
       <c r="DB22" s="28"/>
     </row>
-    <row r="23" spans="1:107" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A23" s="23">
         <v>22</v>
       </c>
@@ -7893,7 +8337,7 @@
       <c r="DA23" s="28"/>
       <c r="DB23" s="28"/>
     </row>
-    <row r="24" spans="1:107" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A24" s="23">
         <v>23</v>
       </c>
@@ -8021,7 +8465,7 @@
       <c r="DA24" s="28"/>
       <c r="DB24" s="28"/>
     </row>
-    <row r="25" spans="1:107" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A25" s="23">
         <v>24</v>
       </c>
@@ -8149,7 +8593,7 @@
       <c r="DA25" s="28"/>
       <c r="DB25" s="28"/>
     </row>
-    <row r="26" spans="1:107" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A26" s="23">
         <v>25</v>
       </c>
@@ -8277,7 +8721,7 @@
       <c r="DA26" s="28"/>
       <c r="DB26" s="28"/>
     </row>
-    <row r="27" spans="1:107" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A27" s="23">
         <v>26</v>
       </c>
@@ -8407,7 +8851,7 @@
       <c r="DA27" s="28"/>
       <c r="DB27" s="28"/>
     </row>
-    <row r="28" spans="1:107" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A28" s="23">
         <v>27</v>
       </c>
@@ -8537,7 +8981,7 @@
       <c r="DA28" s="28"/>
       <c r="DB28" s="28"/>
     </row>
-    <row r="29" spans="1:107" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A29" s="23">
         <v>28</v>
       </c>
@@ -8681,7 +9125,7 @@
       <c r="DA29" s="28"/>
       <c r="DB29" s="28"/>
     </row>
-    <row r="30" spans="1:107" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -8695,7 +9139,7 @@
         <v>424</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>461</v>
+        <v>493</v>
       </c>
       <c r="M30" s="23" t="s">
         <v>4</v>
@@ -8725,13 +9169,13 @@
         <v>23</v>
       </c>
       <c r="AA30" s="58" t="s">
-        <v>460</v>
+        <v>494</v>
       </c>
       <c r="AB30" s="2" t="s">
         <v>84</v>
       </c>
       <c r="AC30" s="24" t="s">
-        <v>345</v>
+        <v>451</v>
       </c>
       <c r="AD30" s="24" t="s">
         <v>345</v>
@@ -8740,10 +9184,10 @@
         <v>98</v>
       </c>
       <c r="AF30" s="23" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="AG30" s="24" t="s">
-        <v>345</v>
+        <v>496</v>
       </c>
       <c r="AH30" s="23"/>
       <c r="AI30" s="23" t="s">
@@ -8780,10 +9224,10 @@
         <v>336</v>
       </c>
       <c r="DC30" s="58" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="31" spans="1:107" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="31" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -8796,6 +9240,1506 @@
       <c r="D31" s="23" t="s">
         <v>424</v>
       </c>
+    </row>
+    <row r="32" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>31</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>424</v>
+      </c>
+      <c r="I32" s="23" t="s">
+        <v>457</v>
+      </c>
+      <c r="J32" s="23" t="s">
+        <v>459</v>
+      </c>
+      <c r="K32" s="23"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="N32" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="O32" s="25" t="s">
+        <v>286</v>
+      </c>
+      <c r="P32" s="23"/>
+      <c r="Q32" s="23"/>
+      <c r="R32" s="23"/>
+      <c r="S32" s="23"/>
+      <c r="T32" s="23"/>
+      <c r="U32" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="V32" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="W32" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="X32" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y32" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z32" s="23">
+        <v>11010</v>
+      </c>
+      <c r="AA32" s="26" t="s">
+        <v>352</v>
+      </c>
+      <c r="AB32" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC32" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="AD32" s="24" t="s">
+        <v>420</v>
+      </c>
+      <c r="AE32" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="AF32" s="23" t="s">
+        <v>410</v>
+      </c>
+      <c r="AG32" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="AH32" s="23"/>
+      <c r="AI32" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ32" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK32" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL32" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="AM32" s="24"/>
+      <c r="AN32" s="24"/>
+      <c r="AO32" s="24"/>
+      <c r="AP32" s="23"/>
+      <c r="AQ32" s="23"/>
+      <c r="AR32" s="23"/>
+      <c r="AS32" s="23"/>
+      <c r="AT32" s="23"/>
+      <c r="AU32" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV32" s="23"/>
+      <c r="AW32" s="23"/>
+      <c r="AX32" s="23"/>
+      <c r="AY32" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AZ32" s="23" t="s">
+        <v>419</v>
+      </c>
+      <c r="BA32" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="BB32" s="23" t="s">
+        <v>419</v>
+      </c>
+      <c r="BC32" s="23" t="s">
+        <v>419</v>
+      </c>
+      <c r="BD32" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="BE32" s="23"/>
+      <c r="BF32" s="23" t="s">
+        <v>419</v>
+      </c>
+      <c r="BG32" s="23" t="s">
+        <v>351</v>
+      </c>
+      <c r="BH32" s="23"/>
+      <c r="BI32" s="23"/>
+      <c r="BJ32" s="23"/>
+      <c r="BK32" s="23"/>
+      <c r="BL32" s="23"/>
+      <c r="BM32" s="23"/>
+      <c r="BN32" s="23"/>
+      <c r="BO32" s="23"/>
+      <c r="BP32" s="23"/>
+      <c r="BQ32" s="23"/>
+      <c r="BR32" s="23"/>
+      <c r="BS32" s="23"/>
+      <c r="BT32" s="23"/>
+      <c r="BU32" s="23"/>
+      <c r="BV32" s="23"/>
+      <c r="BW32" s="23"/>
+      <c r="BX32" s="23"/>
+      <c r="BY32" s="23"/>
+      <c r="BZ32" s="23"/>
+      <c r="CA32" s="23"/>
+      <c r="CB32" s="23"/>
+      <c r="CC32" s="23"/>
+      <c r="CD32" s="23"/>
+      <c r="CE32" s="23"/>
+      <c r="CF32" s="23"/>
+      <c r="CG32" s="23"/>
+      <c r="CH32" s="23"/>
+      <c r="CI32" s="23"/>
+      <c r="CJ32" s="23"/>
+      <c r="CK32" s="23"/>
+      <c r="CL32" s="23"/>
+      <c r="CM32" s="23"/>
+      <c r="CN32" s="23"/>
+      <c r="CO32" s="23"/>
+      <c r="CP32" s="23"/>
+      <c r="CQ32" s="23"/>
+      <c r="CR32" s="23"/>
+      <c r="CS32" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="CT32" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="CU32" s="24"/>
+      <c r="CV32" s="23"/>
+      <c r="CW32" s="23"/>
+      <c r="CX32" s="23"/>
+      <c r="CY32" s="23" t="s">
+        <v>336</v>
+      </c>
+      <c r="CZ32" s="23"/>
+      <c r="DA32" s="23"/>
+      <c r="DB32" s="23"/>
+      <c r="DC32" s="6"/>
+      <c r="DD32" s="6"/>
+      <c r="DE32" s="6"/>
+    </row>
+    <row r="33" spans="1:130" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>424</v>
+      </c>
+      <c r="E33" s="58" t="s">
+        <v>465</v>
+      </c>
+      <c r="F33" s="58"/>
+      <c r="I33" s="23" t="s">
+        <v>463</v>
+      </c>
+      <c r="J33" s="23" t="s">
+        <v>462</v>
+      </c>
+      <c r="K33" s="23" t="s">
+        <v>464</v>
+      </c>
+      <c r="L33" s="24"/>
+      <c r="M33" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="N33" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="O33" s="25" t="s">
+        <v>286</v>
+      </c>
+      <c r="P33" s="23"/>
+      <c r="Q33" s="23"/>
+      <c r="R33" s="23"/>
+      <c r="S33" s="23"/>
+      <c r="T33" s="23"/>
+      <c r="U33" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="V33" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="W33" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="X33" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y33" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z33" s="23">
+        <v>11010</v>
+      </c>
+      <c r="AA33" s="26" t="s">
+        <v>352</v>
+      </c>
+      <c r="AB33" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC33" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="AD33" s="24" t="s">
+        <v>420</v>
+      </c>
+      <c r="AE33" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="AF33" s="23" t="s">
+        <v>410</v>
+      </c>
+      <c r="AG33" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="AH33" s="23"/>
+      <c r="AI33" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ33" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK33" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL33" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="AM33" s="24"/>
+      <c r="AN33" s="24"/>
+      <c r="AO33" s="24"/>
+      <c r="AP33" s="23"/>
+      <c r="AQ33" s="23"/>
+      <c r="AR33" s="23"/>
+      <c r="AS33" s="23"/>
+      <c r="AT33" s="23"/>
+      <c r="AU33" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV33" s="23"/>
+      <c r="AW33" s="23"/>
+      <c r="AX33" s="23"/>
+      <c r="AY33" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AZ33" s="23" t="s">
+        <v>419</v>
+      </c>
+      <c r="BA33" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="BB33" s="23" t="s">
+        <v>419</v>
+      </c>
+      <c r="BC33" s="23" t="s">
+        <v>419</v>
+      </c>
+      <c r="BD33" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="BE33" s="23"/>
+      <c r="BF33" s="23" t="s">
+        <v>419</v>
+      </c>
+      <c r="BG33" s="23" t="s">
+        <v>351</v>
+      </c>
+      <c r="BH33" s="23"/>
+      <c r="BI33" s="23"/>
+      <c r="BJ33" s="23"/>
+      <c r="BK33" s="25" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="34" spans="1:130" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" s="23" t="s">
+        <v>424</v>
+      </c>
+      <c r="E34" s="58" t="s">
+        <v>465</v>
+      </c>
+      <c r="I34" s="23" t="s">
+        <v>467</v>
+      </c>
+      <c r="J34" s="23"/>
+      <c r="K34" s="23"/>
+      <c r="L34" s="24"/>
+      <c r="M34" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="N34" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="O34" s="25" t="s">
+        <v>468</v>
+      </c>
+      <c r="P34" s="23"/>
+      <c r="Q34" s="23"/>
+      <c r="R34" s="23"/>
+      <c r="S34" s="23"/>
+      <c r="T34" s="23"/>
+      <c r="U34" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="V34" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="W34" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="X34" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y34" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z34" s="23">
+        <v>11010</v>
+      </c>
+      <c r="AA34" s="26" t="s">
+        <v>352</v>
+      </c>
+      <c r="AB34" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC34" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="AD34" s="24" t="s">
+        <v>420</v>
+      </c>
+      <c r="AE34" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="AF34" s="23" t="s">
+        <v>410</v>
+      </c>
+      <c r="AG34" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="AH34" s="23"/>
+      <c r="AI34" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ34" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK34" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL34" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="AM34" s="24"/>
+      <c r="AN34" s="24"/>
+      <c r="AO34" s="24"/>
+      <c r="AP34" s="23"/>
+      <c r="AQ34" s="23"/>
+      <c r="AR34" s="23"/>
+      <c r="AS34" s="23"/>
+      <c r="AT34" s="23"/>
+      <c r="AU34" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV34" s="23"/>
+      <c r="AW34" s="23"/>
+      <c r="AX34" s="23"/>
+      <c r="AY34" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AZ34" s="23" t="s">
+        <v>419</v>
+      </c>
+      <c r="BA34" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="BB34" s="23" t="s">
+        <v>419</v>
+      </c>
+      <c r="BC34" s="23" t="s">
+        <v>419</v>
+      </c>
+      <c r="BD34" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="BE34" s="23"/>
+      <c r="BF34" s="23" t="s">
+        <v>419</v>
+      </c>
+      <c r="BG34" s="23" t="s">
+        <v>351</v>
+      </c>
+      <c r="BH34" s="23"/>
+      <c r="BI34" s="23"/>
+      <c r="BJ34" s="23"/>
+      <c r="BK34" s="25" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="35" spans="1:130" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="23">
+        <v>34</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="C35" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="23" t="s">
+        <v>424</v>
+      </c>
+      <c r="E35" s="26" t="s">
+        <v>471</v>
+      </c>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="23" t="s">
+        <v>472</v>
+      </c>
+      <c r="J35" s="23" t="s">
+        <v>473</v>
+      </c>
+      <c r="K35" s="23"/>
+      <c r="L35" s="24"/>
+      <c r="M35" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="N35" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="O35" s="25" t="s">
+        <v>286</v>
+      </c>
+      <c r="P35" s="23"/>
+      <c r="Q35" s="23"/>
+      <c r="R35" s="23"/>
+      <c r="S35" s="23"/>
+      <c r="T35" s="23"/>
+      <c r="U35" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="V35" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="W35" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="X35" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y35" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z35" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA35" s="26" t="s">
+        <v>352</v>
+      </c>
+      <c r="AB35" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC35" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="AD35" s="24" t="s">
+        <v>420</v>
+      </c>
+      <c r="AE35" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="AF35" s="23" t="s">
+        <v>410</v>
+      </c>
+      <c r="AG35" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="AH35" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="AI35" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ35" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK35" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL35" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="AM35" s="24"/>
+      <c r="AN35" s="24"/>
+      <c r="AO35" s="24"/>
+      <c r="AP35" s="23"/>
+      <c r="AQ35" s="23"/>
+      <c r="AR35" s="23"/>
+      <c r="AS35" s="23"/>
+      <c r="AT35" s="23"/>
+      <c r="AU35" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV35" s="23"/>
+      <c r="AW35" s="23"/>
+      <c r="AX35" s="23"/>
+      <c r="AY35" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AZ35" s="23" t="s">
+        <v>419</v>
+      </c>
+      <c r="BA35" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="BB35" s="23" t="s">
+        <v>419</v>
+      </c>
+      <c r="BC35" s="23" t="s">
+        <v>419</v>
+      </c>
+      <c r="BD35" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="BE35" s="23"/>
+      <c r="BF35" s="23" t="s">
+        <v>419</v>
+      </c>
+      <c r="BG35" s="23" t="s">
+        <v>351</v>
+      </c>
+      <c r="BH35" s="23"/>
+      <c r="BI35" s="23"/>
+      <c r="BJ35" s="23"/>
+      <c r="BK35" s="23"/>
+      <c r="BL35" s="23"/>
+      <c r="BM35" s="23"/>
+      <c r="BN35" s="23"/>
+      <c r="BO35" s="23"/>
+      <c r="BP35" s="23"/>
+      <c r="BQ35" s="23"/>
+      <c r="BR35" s="23"/>
+      <c r="BS35" s="23"/>
+      <c r="BT35" s="23"/>
+      <c r="BU35" s="23"/>
+      <c r="BV35" s="23"/>
+      <c r="BW35" s="23"/>
+      <c r="BX35" s="23"/>
+      <c r="BY35" s="23"/>
+      <c r="BZ35" s="23"/>
+      <c r="CA35" s="23"/>
+      <c r="CB35" s="23"/>
+      <c r="CC35" s="23"/>
+      <c r="CD35" s="23"/>
+      <c r="CE35" s="23"/>
+      <c r="CF35" s="23"/>
+      <c r="CG35" s="23"/>
+      <c r="CH35" s="23"/>
+      <c r="CI35" s="23"/>
+      <c r="CJ35" s="23"/>
+      <c r="CK35" s="23"/>
+      <c r="CL35" s="23"/>
+      <c r="CM35" s="23"/>
+      <c r="CN35" s="23"/>
+      <c r="CO35" s="23"/>
+      <c r="CP35" s="23"/>
+      <c r="CQ35" s="23"/>
+      <c r="CR35" s="23"/>
+      <c r="CS35" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="CT35" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="CU35" s="24"/>
+      <c r="CV35" s="23"/>
+      <c r="CW35" s="23"/>
+      <c r="CX35" s="23"/>
+      <c r="CY35" s="23" t="s">
+        <v>336</v>
+      </c>
+      <c r="CZ35" s="23"/>
+      <c r="DA35" s="23"/>
+      <c r="DB35" s="23"/>
+    </row>
+    <row r="36" spans="1:130" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="C36" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="23" t="s">
+        <v>424</v>
+      </c>
+      <c r="E36" s="58" t="s">
+        <v>476</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="37" spans="1:130" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="C37" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37" s="23" t="s">
+        <v>424</v>
+      </c>
+      <c r="E37" s="58" t="s">
+        <v>465</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="38" spans="1:130" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>37</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="C38" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D38" s="23" t="s">
+        <v>424</v>
+      </c>
+      <c r="E38" s="58" t="s">
+        <v>480</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="39" spans="1:130" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>38</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="C39" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="23" t="s">
+        <v>424</v>
+      </c>
+      <c r="E39" s="58" t="s">
+        <v>480</v>
+      </c>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
+      <c r="H39" s="23"/>
+      <c r="I39" s="23" t="s">
+        <v>485</v>
+      </c>
+      <c r="J39" s="23"/>
+      <c r="K39" s="23"/>
+      <c r="L39" s="24"/>
+      <c r="M39" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="N39" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="O39" s="25" t="s">
+        <v>286</v>
+      </c>
+      <c r="P39" s="23"/>
+      <c r="Q39" s="23"/>
+      <c r="R39" s="23"/>
+      <c r="S39" s="23"/>
+      <c r="T39" s="23"/>
+      <c r="U39" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="V39" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="W39" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="X39" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y39" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z39" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA39" s="26" t="s">
+        <v>352</v>
+      </c>
+      <c r="AB39" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC39" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="AD39" s="24" t="s">
+        <v>420</v>
+      </c>
+      <c r="AE39" s="23"/>
+      <c r="AF39" s="23" t="s">
+        <v>410</v>
+      </c>
+      <c r="AG39" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="AH39" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="AI39" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ39" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK39" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL39" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="AM39" s="24"/>
+      <c r="AN39" s="24"/>
+      <c r="AO39" s="24"/>
+      <c r="AP39" s="23"/>
+      <c r="AQ39" s="23"/>
+      <c r="AR39" s="23"/>
+      <c r="AS39" s="23"/>
+      <c r="AT39" s="23"/>
+      <c r="AU39" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV39" s="23"/>
+      <c r="AW39" s="23"/>
+      <c r="AX39" s="23"/>
+      <c r="AY39" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AZ39" s="23" t="s">
+        <v>419</v>
+      </c>
+      <c r="BA39" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="BB39" s="23" t="s">
+        <v>419</v>
+      </c>
+      <c r="BC39" s="23" t="s">
+        <v>419</v>
+      </c>
+      <c r="BD39" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="BE39" s="23"/>
+      <c r="BF39" s="23" t="s">
+        <v>419</v>
+      </c>
+      <c r="BG39" s="23" t="s">
+        <v>351</v>
+      </c>
+      <c r="BH39" s="23"/>
+      <c r="BI39" s="23"/>
+      <c r="BJ39" s="23"/>
+      <c r="BK39" s="23"/>
+      <c r="BL39" s="23"/>
+      <c r="BM39" s="23"/>
+      <c r="BN39" s="23"/>
+      <c r="BO39" s="23"/>
+      <c r="BP39" s="23"/>
+      <c r="BQ39" s="23"/>
+      <c r="BR39" s="23"/>
+      <c r="BS39" s="23"/>
+      <c r="BT39" s="23"/>
+      <c r="BU39" s="23"/>
+      <c r="BV39" s="23"/>
+      <c r="BW39" s="23"/>
+      <c r="BX39" s="23"/>
+      <c r="BY39" s="23"/>
+      <c r="BZ39" s="23"/>
+      <c r="CA39" s="23"/>
+      <c r="CB39" s="23"/>
+      <c r="CC39" s="23"/>
+      <c r="CD39" s="23"/>
+      <c r="CE39" s="23"/>
+      <c r="CF39" s="23"/>
+      <c r="CG39" s="23"/>
+      <c r="CH39" s="23"/>
+      <c r="CI39" s="23"/>
+      <c r="CJ39" s="23"/>
+      <c r="CK39" s="23"/>
+      <c r="CL39" s="23"/>
+      <c r="CM39" s="23"/>
+      <c r="CN39" s="23"/>
+      <c r="CO39" s="23"/>
+      <c r="CP39" s="23"/>
+      <c r="CQ39" s="23"/>
+      <c r="CR39" s="23"/>
+      <c r="CS39" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="CT39" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="CU39" s="24"/>
+      <c r="CV39" s="23"/>
+      <c r="CW39" s="23"/>
+      <c r="CX39" s="23"/>
+      <c r="CY39" s="23" t="s">
+        <v>336</v>
+      </c>
+      <c r="CZ39" s="23"/>
+      <c r="DA39" s="23"/>
+      <c r="DB39" s="23"/>
+      <c r="DC39" s="6"/>
+      <c r="DD39" s="6"/>
+      <c r="DE39" s="6"/>
+      <c r="DF39" s="6"/>
+      <c r="DG39" s="6"/>
+      <c r="DH39" s="6"/>
+      <c r="DI39" s="6"/>
+      <c r="DJ39" s="6"/>
+      <c r="DK39" s="6"/>
+      <c r="DL39" s="6"/>
+      <c r="DM39" s="6"/>
+      <c r="DN39" s="6"/>
+      <c r="DO39" s="6"/>
+      <c r="DP39" s="6"/>
+      <c r="DQ39" s="6"/>
+      <c r="DR39" s="6"/>
+      <c r="DS39" s="6"/>
+      <c r="DT39" s="6"/>
+      <c r="DU39" s="6"/>
+      <c r="DV39" s="6"/>
+      <c r="DW39" s="6"/>
+      <c r="DX39" s="6"/>
+      <c r="DY39" s="6"/>
+      <c r="DZ39" s="6"/>
+    </row>
+    <row r="40" spans="1:130" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>39</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>487</v>
+      </c>
+      <c r="C40" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" s="23" t="s">
+        <v>424</v>
+      </c>
+      <c r="E40" s="58" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="41" spans="1:130" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="23">
+        <v>40</v>
+      </c>
+      <c r="B41" s="73" t="s">
+        <v>488</v>
+      </c>
+      <c r="C41" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="D41" s="23" t="s">
+        <v>424</v>
+      </c>
+      <c r="E41" s="23"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="23"/>
+      <c r="H41" s="23"/>
+      <c r="I41" s="23" t="s">
+        <v>489</v>
+      </c>
+      <c r="J41" s="23" t="s">
+        <v>492</v>
+      </c>
+      <c r="K41" s="23"/>
+      <c r="L41" s="24"/>
+      <c r="M41" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="N41" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="O41" s="25" t="s">
+        <v>286</v>
+      </c>
+      <c r="P41" s="23"/>
+      <c r="Q41" s="23"/>
+      <c r="R41" s="23"/>
+      <c r="S41" s="23"/>
+      <c r="T41" s="23"/>
+      <c r="U41" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="V41" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="W41" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="X41" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y41" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z41" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA41" s="26"/>
+      <c r="AB41" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC41" s="23"/>
+      <c r="AD41" s="24" t="s">
+        <v>420</v>
+      </c>
+      <c r="AE41" s="23"/>
+      <c r="AF41" s="23" t="s">
+        <v>409</v>
+      </c>
+      <c r="AG41" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="AH41" s="23"/>
+      <c r="AI41" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ41" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK41" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL41" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="AM41" s="24"/>
+      <c r="AN41" s="24"/>
+      <c r="AO41" s="24"/>
+      <c r="AP41" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="AQ41" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="AR41" s="24">
+        <v>44259</v>
+      </c>
+      <c r="AS41" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="AT41" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="AU41" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="AV41" s="35" t="s">
+        <v>406</v>
+      </c>
+      <c r="AW41" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="AX41" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="AY41" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="AZ41" s="23"/>
+      <c r="BA41" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="BB41" s="23"/>
+      <c r="BC41" s="23"/>
+      <c r="BD41" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="BE41" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="BF41" s="23" t="s">
+        <v>419</v>
+      </c>
+      <c r="BG41" s="23" t="s">
+        <v>351</v>
+      </c>
+      <c r="BH41" s="23"/>
+      <c r="BI41" s="23"/>
+      <c r="BJ41" s="23"/>
+      <c r="BK41" s="23"/>
+      <c r="BL41" s="23"/>
+      <c r="BM41" s="23"/>
+      <c r="BN41" s="23"/>
+      <c r="BO41" s="23"/>
+      <c r="BP41" s="23"/>
+      <c r="BQ41" s="23"/>
+      <c r="BR41" s="23"/>
+      <c r="BS41" s="23"/>
+      <c r="BT41" s="23"/>
+      <c r="BU41" s="23"/>
+      <c r="BV41" s="23"/>
+      <c r="BW41" s="23"/>
+      <c r="BX41" s="23"/>
+      <c r="BY41" s="23"/>
+      <c r="BZ41" s="23"/>
+      <c r="CA41" s="23"/>
+      <c r="CB41" s="23"/>
+      <c r="CC41" s="23"/>
+      <c r="CD41" s="23"/>
+      <c r="CE41" s="23"/>
+      <c r="CF41" s="23"/>
+      <c r="CG41" s="23"/>
+      <c r="CH41" s="23"/>
+      <c r="CI41" s="23"/>
+      <c r="CJ41" s="23"/>
+      <c r="CK41" s="23"/>
+      <c r="CL41" s="23"/>
+      <c r="CM41" s="23"/>
+      <c r="CN41" s="23"/>
+      <c r="CO41" s="23"/>
+      <c r="CP41" s="23"/>
+      <c r="CQ41" s="23"/>
+      <c r="CR41" s="23"/>
+      <c r="CS41" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="CT41" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="CU41" s="24"/>
+      <c r="CV41" s="23"/>
+      <c r="CW41" s="23"/>
+      <c r="CX41" s="23"/>
+      <c r="CY41" s="23" t="s">
+        <v>336</v>
+      </c>
+      <c r="CZ41" s="23"/>
+      <c r="DA41" s="23"/>
+      <c r="DB41" s="23"/>
+    </row>
+    <row r="42" spans="1:130" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="23">
+        <v>41</v>
+      </c>
+      <c r="B42" s="74" t="s">
+        <v>491</v>
+      </c>
+      <c r="C42" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D42" s="23" t="s">
+        <v>424</v>
+      </c>
+      <c r="E42" s="28"/>
+      <c r="F42" s="28"/>
+      <c r="G42" s="28"/>
+      <c r="H42" s="28"/>
+      <c r="I42" s="28" t="s">
+        <v>490</v>
+      </c>
+      <c r="J42" s="28"/>
+      <c r="K42" s="28"/>
+      <c r="L42" s="28"/>
+      <c r="M42" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="N42" s="24">
+        <v>44868</v>
+      </c>
+      <c r="O42" s="25" t="s">
+        <v>347</v>
+      </c>
+      <c r="P42" s="28"/>
+      <c r="Q42" s="28"/>
+      <c r="R42" s="28"/>
+      <c r="S42" s="28"/>
+      <c r="T42" s="28"/>
+      <c r="U42" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="V42" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="W42" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="X42" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y42" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z42" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA42" s="26" t="s">
+        <v>352</v>
+      </c>
+      <c r="AB42" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC42" s="24">
+        <v>44868</v>
+      </c>
+      <c r="AD42" s="24">
+        <v>44868</v>
+      </c>
+      <c r="AE42" s="28"/>
+      <c r="AF42" s="23" t="s">
+        <v>410</v>
+      </c>
+      <c r="AG42" s="24">
+        <v>44868</v>
+      </c>
+      <c r="AH42" s="28"/>
+      <c r="AI42" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ42" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK42" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL42" s="24">
+        <v>44868</v>
+      </c>
+      <c r="AM42" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="AN42" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="AO42" s="24">
+        <v>44868</v>
+      </c>
+      <c r="AP42" s="28"/>
+      <c r="AQ42" s="28"/>
+      <c r="AR42" s="28"/>
+      <c r="AS42" s="28"/>
+      <c r="AT42" s="28"/>
+      <c r="AU42" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV42" s="29" t="s">
+        <v>407</v>
+      </c>
+      <c r="AW42" s="23" t="s">
+        <v>421</v>
+      </c>
+      <c r="AX42" s="28"/>
+      <c r="AY42" s="28"/>
+      <c r="AZ42" s="23" t="s">
+        <v>419</v>
+      </c>
+      <c r="BA42" s="28"/>
+      <c r="BB42" s="23" t="s">
+        <v>419</v>
+      </c>
+      <c r="BC42" s="23" t="s">
+        <v>419</v>
+      </c>
+      <c r="BD42" s="28"/>
+      <c r="BE42" s="28"/>
+      <c r="BF42" s="23" t="s">
+        <v>419</v>
+      </c>
+      <c r="BG42" s="23" t="s">
+        <v>351</v>
+      </c>
+      <c r="BH42" s="28"/>
+      <c r="BI42" s="28"/>
+      <c r="BJ42" s="28"/>
+      <c r="BK42" s="28"/>
+      <c r="BL42" s="28"/>
+      <c r="BM42" s="28"/>
+      <c r="BN42" s="28"/>
+      <c r="BO42" s="28"/>
+      <c r="BP42" s="28"/>
+      <c r="BQ42" s="28"/>
+      <c r="BR42" s="28"/>
+      <c r="BS42" s="28"/>
+      <c r="BT42" s="28"/>
+      <c r="BU42" s="28"/>
+      <c r="BV42" s="28"/>
+      <c r="BW42" s="28"/>
+      <c r="BX42" s="28"/>
+      <c r="BY42" s="28"/>
+      <c r="BZ42" s="28"/>
+      <c r="CA42" s="28"/>
+      <c r="CB42" s="28"/>
+      <c r="CC42" s="28"/>
+      <c r="CD42" s="28"/>
+      <c r="CE42" s="28"/>
+      <c r="CF42" s="28"/>
+      <c r="CG42" s="28"/>
+      <c r="CH42" s="28"/>
+      <c r="CI42" s="28"/>
+      <c r="CJ42" s="28"/>
+      <c r="CK42" s="28"/>
+      <c r="CL42" s="28"/>
+      <c r="CM42" s="28"/>
+      <c r="CN42" s="28"/>
+      <c r="CO42" s="28"/>
+      <c r="CP42" s="28"/>
+      <c r="CQ42" s="28"/>
+      <c r="CR42" s="28"/>
+      <c r="CS42" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="CT42" s="24" t="s">
+        <v>499</v>
+      </c>
+      <c r="CU42" s="24" t="s">
+        <v>499</v>
+      </c>
+      <c r="CV42" s="25" t="s">
+        <v>263</v>
+      </c>
+      <c r="CW42" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="CX42" s="28"/>
+      <c r="CY42" s="23" t="s">
+        <v>336</v>
+      </c>
+      <c r="CZ42" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="DA42" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="DB42" s="28" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="43" spans="1:130" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="23">
+        <v>42</v>
+      </c>
+      <c r="B43" s="74" t="s">
+        <v>502</v>
+      </c>
+      <c r="C43" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D43" s="23" t="s">
+        <v>424</v>
+      </c>
+      <c r="E43" s="23"/>
+      <c r="F43" s="23"/>
+      <c r="G43" s="23"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23" t="s">
+        <v>503</v>
+      </c>
+      <c r="J43" s="23"/>
+      <c r="K43" s="23"/>
+      <c r="L43" s="24"/>
+      <c r="M43" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="N43" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="O43" s="25" t="s">
+        <v>286</v>
+      </c>
+      <c r="P43" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q43" s="23"/>
+      <c r="R43" s="23"/>
+      <c r="S43" s="23"/>
+      <c r="T43" s="23"/>
+      <c r="U43" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="V43" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="W43" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="X43" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y43" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z43" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA43" s="26" t="s">
+        <v>352</v>
+      </c>
+      <c r="AB43" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC43" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="AD43" s="24" t="s">
+        <v>420</v>
+      </c>
+      <c r="AE43" s="23"/>
+      <c r="AF43" s="23" t="s">
+        <v>410</v>
+      </c>
+      <c r="AG43" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="AH43" s="23"/>
+      <c r="AI43" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ43" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK43" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL43" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="AM43" s="24"/>
+      <c r="AN43" s="24"/>
+      <c r="AO43" s="24"/>
+      <c r="AP43" s="23"/>
+      <c r="AQ43" s="23"/>
+      <c r="AR43" s="23"/>
+      <c r="AS43" s="23"/>
+      <c r="AT43" s="23"/>
+      <c r="AU43" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV43" s="23"/>
+      <c r="AW43" s="23"/>
+      <c r="AX43" s="24"/>
+      <c r="AY43" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AZ43" s="23" t="s">
+        <v>419</v>
+      </c>
+      <c r="BA43" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="BB43" s="23" t="s">
+        <v>419</v>
+      </c>
+      <c r="BC43" s="23" t="s">
+        <v>419</v>
+      </c>
+      <c r="BD43" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="BE43" s="23"/>
+      <c r="BF43" s="23" t="s">
+        <v>419</v>
+      </c>
+      <c r="BG43" s="23" t="s">
+        <v>351</v>
+      </c>
+      <c r="BH43" s="23"/>
+      <c r="BI43" s="23"/>
+      <c r="BJ43" s="23"/>
+      <c r="BK43" s="23"/>
+      <c r="BL43" s="23"/>
+      <c r="BM43" s="23"/>
+      <c r="BN43" s="23"/>
+      <c r="BO43" s="23"/>
+      <c r="BP43" s="23"/>
+      <c r="BQ43" s="23"/>
+      <c r="BR43" s="23"/>
+      <c r="BS43" s="23"/>
+      <c r="BT43" s="23"/>
+      <c r="BU43" s="23"/>
+      <c r="BV43" s="23"/>
+      <c r="BW43" s="23"/>
+      <c r="BX43" s="23"/>
+      <c r="BY43" s="23"/>
+      <c r="BZ43" s="23"/>
+      <c r="CA43" s="23"/>
+      <c r="CB43" s="23"/>
+      <c r="CC43" s="23"/>
+      <c r="CD43" s="23"/>
+      <c r="CE43" s="23"/>
+      <c r="CF43" s="23"/>
+      <c r="CG43" s="23"/>
+      <c r="CH43" s="23"/>
+      <c r="CI43" s="23"/>
+      <c r="CJ43" s="23"/>
+      <c r="CK43" s="23"/>
+      <c r="CL43" s="23"/>
+      <c r="CM43" s="23"/>
+      <c r="CN43" s="23"/>
+      <c r="CO43" s="23"/>
+      <c r="CP43" s="23"/>
+      <c r="CQ43" s="23"/>
+      <c r="CR43" s="23"/>
+      <c r="CS43" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="CT43" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="CU43" s="24"/>
+      <c r="CV43" s="23"/>
+      <c r="CW43" s="23"/>
+      <c r="CX43" s="23"/>
+      <c r="CY43" s="23" t="s">
+        <v>336</v>
+      </c>
+      <c r="CZ43" s="23"/>
+      <c r="DA43" s="23"/>
+      <c r="DB43" s="23"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -8817,57 +10761,57 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="114" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="82.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="34.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="33" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="9.5703125" customWidth="1" collapsed="1"/>
-    <col min="35" max="36" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="4.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="5.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="6.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="114.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="82.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="34.85546875" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="31" max="33" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="35" max="36" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="4.140625" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" width="5.7109375" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" width="6.7109375" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="47" max="47" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="48" max="48" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="49" max="49" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="50" max="50" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="51" max="51" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="52" max="52" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="53" max="53" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="54" max="54" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:55" x14ac:dyDescent="0.25">
@@ -10406,25 +12350,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="113.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="65.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="73.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="113.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="65.42578125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="73.85546875" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
@@ -11017,15 +12961,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006150CD2B74865543AE839454BD4B5DC6" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a2ee5e546ec1836f671c2a05bfe6bfc8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0be14d6d-d8a1-45f7-9f98-2db40f8691c4" xmlns:ns3="567c5c99-f8da-409a-bc28-51b94ad9a241" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e7ff770c31624934d8e1a633c6fbe95" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -11259,6 +13194,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -11269,16 +13213,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB0B3A61-2E64-4CE7-BDD4-6ECB945D22FD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64F77A26-17A6-43DF-A115-F9EC24E62EB0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11298,6 +13232,16 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB0B3A61-2E64-4CE7-BDD4-6ECB945D22FD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E980A1B9-8C22-45F7-8344-5E520FA354EB}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Committing 43703 and 44710
</commit_message>
<xml_diff>
--- a/data/CRM_Testdata.xlsx
+++ b/data/CRM_Testdata.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2495" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2881" uniqueCount="511">
   <si>
     <t>UserName</t>
   </si>
@@ -1569,6 +1569,9 @@
   </si>
   <si>
     <t>2022_11_04_01_49_12</t>
+  </si>
+  <si>
+    <t>2022_11_04_03_17_09</t>
   </si>
 </sst>
 </file>
@@ -3946,7 +3949,7 @@
         <v>505</v>
       </c>
       <c r="G66" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="H66" t="s">
         <v>508</v>

</xml_diff>

<commit_message>
Committing On Prem Automation test cases
</commit_message>
<xml_diff>
--- a/data/CRM_Testdata.xlsx
+++ b/data/CRM_Testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\vkamalak\git\OnPremise\Dynamics-CRM-Stage\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\vkamalak\git\Dynamics-CRM-Stage\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC82571-9FA3-4216-885B-8EE28B980FFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5630F0DF-7592-4210-9CFB-3C859D086C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="599" xr2:uid="{442E3441-3F3C-4A77-BB17-E93CAE512719}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="599" xr2:uid="{442E3441-3F3C-4A77-BB17-E93CAE512719}"/>
   </bookViews>
   <sheets>
     <sheet name="Driver" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2395" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2415" uniqueCount="537">
   <si>
     <t>UserName</t>
   </si>
@@ -1325,18 +1325,9 @@
     <t/>
   </si>
   <si>
-    <t>2000554812</t>
-  </si>
-  <si>
     <t>2000554813</t>
   </si>
   <si>
-    <t>2000554814</t>
-  </si>
-  <si>
-    <t>2000554818</t>
-  </si>
-  <si>
     <t>7000578823</t>
   </si>
   <si>
@@ -1358,39 +1349,6 @@
     <t>7000578829</t>
   </si>
   <si>
-    <t>2000554844</t>
-  </si>
-  <si>
-    <t>2000554848</t>
-  </si>
-  <si>
-    <t>284867136</t>
-  </si>
-  <si>
-    <t>bf9746162</t>
-  </si>
-  <si>
-    <t>2000555263</t>
-  </si>
-  <si>
-    <t>2000555264</t>
-  </si>
-  <si>
-    <t>2000555265</t>
-  </si>
-  <si>
-    <t>2000555266</t>
-  </si>
-  <si>
-    <t>2000555267</t>
-  </si>
-  <si>
-    <t>2000555268</t>
-  </si>
-  <si>
-    <t>2000555269</t>
-  </si>
-  <si>
     <t>corp\crmtest10</t>
   </si>
   <si>
@@ -1400,24 +1358,15 @@
     <t>2000555818</t>
   </si>
   <si>
-    <t>2000555819</t>
-  </si>
-  <si>
     <t>2000555820</t>
   </si>
   <si>
-    <t>2000555823</t>
-  </si>
-  <si>
     <t>TFS ID_45306:Verify Prospect accounts can not be published</t>
   </si>
   <si>
     <t>45306_PublishProspectAccount</t>
   </si>
   <si>
-    <t>2000555831</t>
-  </si>
-  <si>
     <t>You should not publish the prospect If you contact support, please provide the technical details.</t>
   </si>
   <si>
@@ -1520,21 +1469,9 @@
     <t>Top Parent Relationship for Top Parent must be OLM If you contact support, please provide the technical details.</t>
   </si>
   <si>
-    <t>Aparna sub Nov3_</t>
-  </si>
-  <si>
-    <t>2000555522</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
     <t>5/4/2021</t>
   </si>
   <si>
-    <t>2000556059</t>
-  </si>
-  <si>
     <t>11/5/2022</t>
   </si>
   <si>
@@ -1634,13 +1571,85 @@
     <t>2000556237</t>
   </si>
   <si>
-    <t>2000556238</t>
+    <t>2000556506</t>
+  </si>
+  <si>
+    <t>2000556507</t>
+  </si>
+  <si>
+    <t>2000556509</t>
+  </si>
+  <si>
+    <t>2000556511</t>
+  </si>
+  <si>
+    <t>2000556512</t>
+  </si>
+  <si>
+    <t>2000556515</t>
+  </si>
+  <si>
+    <t>2000556516</t>
+  </si>
+  <si>
+    <t>2000556519</t>
+  </si>
+  <si>
+    <t>849987128</t>
+  </si>
+  <si>
+    <t>rf7459476</t>
+  </si>
+  <si>
+    <t>2000556520</t>
+  </si>
+  <si>
+    <t>2000556521</t>
+  </si>
+  <si>
+    <t>2000556522</t>
+  </si>
+  <si>
+    <t>2000556523</t>
+  </si>
+  <si>
+    <t>2000556524</t>
+  </si>
+  <si>
+    <t>2000556525</t>
+  </si>
+  <si>
+    <t>2000556526</t>
+  </si>
+  <si>
+    <t>TFS ID_43705: 11231 Cloud: Verify warning message is NOT displayed when there is any DP change of an account with only location type children</t>
+  </si>
+  <si>
+    <t>2000108670</t>
+  </si>
+  <si>
+    <t>Mani Sub 14Nov_</t>
+  </si>
+  <si>
+    <t>1000109619</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>2000556551</t>
+  </si>
+  <si>
+    <t>2000556557</t>
+  </si>
+  <si>
+    <t>TFS ID_43706: 11232: Cloud: Verify warning message is displayed when there is any DP change of an account with children (non location type)</t>
   </si>
   <si>
     <t>Failed</t>
   </si>
   <si>
-    <t>2022_11_11_03_22_26</t>
+    <t>2022_11_15_12_25_28</t>
   </si>
 </sst>
 </file>
@@ -1767,7 +1776,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1834,6 +1843,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -1885,7 +1900,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2016,6 +2031,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2337,9 +2354,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088699A3-39D2-44E6-8F71-47C2709580BF}">
-  <dimension ref="A1:J77"/>
+  <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2392,7 +2411,7 @@
         <v>57</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>8</v>
@@ -2407,7 +2426,7 @@
         <v>427</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>458</v>
+        <v>510</v>
       </c>
       <c r="I2" s="46" t="s">
         <v>416</v>
@@ -2420,11 +2439,11 @@
       <c r="A3" s="18">
         <v>2</v>
       </c>
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="76" t="s">
         <v>58</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>8</v>
@@ -2439,18 +2458,18 @@
         <v>427</v>
       </c>
       <c r="H3" t="s">
-        <v>452</v>
+        <v>438</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18">
         <v>3</v>
       </c>
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="76" t="s">
         <v>60</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>8</v>
@@ -2465,7 +2484,7 @@
         <v>427</v>
       </c>
       <c r="H4" t="s">
-        <v>453</v>
+        <v>511</v>
       </c>
       <c r="J4" s="46" t="s">
         <v>425</v>
@@ -2475,11 +2494,11 @@
       <c r="A5" s="18">
         <v>4</v>
       </c>
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="76" t="s">
         <v>59</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D5" s="18" t="s">
         <v>8</v>
@@ -2494,7 +2513,7 @@
         <v>427</v>
       </c>
       <c r="H5" t="s">
-        <v>454</v>
+        <v>439</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2505,7 +2524,7 @@
         <v>70</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D6" s="18" t="s">
         <v>8</v>
@@ -2524,11 +2543,11 @@
       <c r="A7" s="18">
         <v>6</v>
       </c>
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="76" t="s">
         <v>71</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>8</v>
@@ -2551,7 +2570,7 @@
         <v>73</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>8</v>
@@ -2566,7 +2585,7 @@
         <v>427</v>
       </c>
       <c r="H8" t="s">
-        <v>455</v>
+        <v>512</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2577,7 +2596,7 @@
         <v>74</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>8</v>
@@ -2600,7 +2619,7 @@
         <v>92</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>8</v>
@@ -2615,18 +2634,18 @@
         <v>427</v>
       </c>
       <c r="H10" t="s">
-        <v>428</v>
+        <v>513</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18">
         <v>10</v>
       </c>
-      <c r="B11" s="70" t="s">
+      <c r="B11" s="76" t="s">
         <v>95</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>8</v>
@@ -2641,7 +2660,7 @@
         <v>427</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2652,7 +2671,7 @@
         <v>94</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>8</v>
@@ -2667,7 +2686,7 @@
         <v>427</v>
       </c>
       <c r="H12" t="s">
-        <v>430</v>
+        <v>514</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2678,7 +2697,7 @@
         <v>99</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D13" s="18" t="s">
         <v>8</v>
@@ -2701,7 +2720,7 @@
         <v>361</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>8</v>
@@ -2724,7 +2743,7 @@
         <v>90</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>8</v>
@@ -2739,7 +2758,7 @@
         <v>427</v>
       </c>
       <c r="H15" t="s">
-        <v>439</v>
+        <v>515</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2750,7 +2769,7 @@
         <v>89</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>8</v>
@@ -2765,7 +2784,7 @@
         <v>427</v>
       </c>
       <c r="H16" t="s">
-        <v>431</v>
+        <v>516</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="61" customFormat="1" x14ac:dyDescent="0.25">
@@ -2776,7 +2795,7 @@
         <v>188</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D17" s="61" t="s">
         <v>8</v>
@@ -2799,7 +2818,7 @@
         <v>100</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>8</v>
@@ -2822,7 +2841,7 @@
         <v>108</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>8</v>
@@ -2845,7 +2864,7 @@
         <v>362</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>8</v>
@@ -2868,7 +2887,7 @@
         <v>346</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D21" s="18" t="s">
         <v>8</v>
@@ -2883,7 +2902,7 @@
         <v>427</v>
       </c>
       <c r="H21" t="s">
-        <v>440</v>
+        <v>517</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2894,7 +2913,7 @@
         <v>258</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>8</v>
@@ -2909,7 +2928,7 @@
         <v>427</v>
       </c>
       <c r="H22" t="s">
-        <v>443</v>
+        <v>520</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2920,7 +2939,7 @@
         <v>257</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>8</v>
@@ -2935,7 +2954,7 @@
         <v>427</v>
       </c>
       <c r="H23" t="s">
-        <v>444</v>
+        <v>521</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2946,7 +2965,7 @@
         <v>247</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D24" s="18" t="s">
         <v>8</v>
@@ -2961,7 +2980,7 @@
         <v>427</v>
       </c>
       <c r="H24" t="s">
-        <v>445</v>
+        <v>522</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2972,7 +2991,7 @@
         <v>259</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>8</v>
@@ -2987,7 +3006,7 @@
         <v>427</v>
       </c>
       <c r="H25" t="s">
-        <v>446</v>
+        <v>523</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2998,7 +3017,7 @@
         <v>260</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>8</v>
@@ -3013,7 +3032,7 @@
         <v>427</v>
       </c>
       <c r="H26" t="s">
-        <v>447</v>
+        <v>524</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -3024,7 +3043,7 @@
         <v>261</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D27" s="18" t="s">
         <v>8</v>
@@ -3039,7 +3058,7 @@
         <v>427</v>
       </c>
       <c r="H27" t="s">
-        <v>448</v>
+        <v>525</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -3050,7 +3069,7 @@
         <v>265</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D28" s="18" t="s">
         <v>8</v>
@@ -3065,18 +3084,18 @@
         <v>427</v>
       </c>
       <c r="H28" t="s">
-        <v>449</v>
+        <v>526</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="61" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="61">
         <v>28</v>
       </c>
-      <c r="B29" s="61" t="s">
+      <c r="B29" s="76" t="s">
         <v>293</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D29" s="61" t="s">
         <v>8</v>
@@ -3099,7 +3118,7 @@
         <v>411</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D30" s="60" t="s">
         <v>8</v>
@@ -3114,7 +3133,7 @@
         <v>427</v>
       </c>
       <c r="H30" t="s">
-        <v>497</v>
+        <v>532</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="67" customFormat="1" x14ac:dyDescent="0.25">
@@ -3396,7 +3415,7 @@
       <c r="A42" s="64">
         <v>41</v>
       </c>
-      <c r="B42" s="65" t="s">
+      <c r="B42" s="77" t="s">
         <v>175</v>
       </c>
       <c r="C42" s="7" t="s">
@@ -3515,7 +3534,7 @@
         <v>427</v>
       </c>
       <c r="H46" s="69" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I46" s="69"/>
     </row>
@@ -3542,7 +3561,7 @@
         <v>427</v>
       </c>
       <c r="H47" s="69" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="I47" s="69"/>
     </row>
@@ -3569,7 +3588,7 @@
         <v>427</v>
       </c>
       <c r="H48" s="69" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="I48" s="69"/>
     </row>
@@ -3596,7 +3615,7 @@
         <v>427</v>
       </c>
       <c r="H49" s="69" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="I49" s="69"/>
     </row>
@@ -3623,7 +3642,7 @@
         <v>427</v>
       </c>
       <c r="H50" s="69" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="I50" s="69"/>
     </row>
@@ -3700,7 +3719,7 @@
         <v>427</v>
       </c>
       <c r="H53" s="69" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="I53" s="69"/>
     </row>
@@ -3727,7 +3746,7 @@
         <v>427</v>
       </c>
       <c r="H54" s="69" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="I54" s="69"/>
     </row>
@@ -3736,10 +3755,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>456</v>
+        <v>440</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D55" s="18" t="s">
         <v>8</v>
@@ -3754,7 +3773,7 @@
         <v>427</v>
       </c>
       <c r="H55" t="s">
-        <v>466</v>
+        <v>449</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -3762,10 +3781,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>460</v>
+        <v>443</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D56" s="18" t="s">
         <v>8</v>
@@ -3780,7 +3799,7 @@
         <v>427</v>
       </c>
       <c r="H56" t="s">
-        <v>461</v>
+        <v>444</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -3788,10 +3807,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>469</v>
+        <v>452</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D57" s="18" t="s">
         <v>8</v>
@@ -3811,10 +3830,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>470</v>
+        <v>453</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D58" s="18" t="s">
         <v>8</v>
@@ -3829,7 +3848,7 @@
         <v>427</v>
       </c>
       <c r="H58" t="s">
-        <v>474</v>
+        <v>457</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -3837,10 +3856,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>475</v>
+        <v>458</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D59" s="18" t="s">
         <v>8</v>
@@ -3860,10 +3879,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>478</v>
+        <v>461</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D60" s="18" t="s">
         <v>8</v>
@@ -3883,10 +3902,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>479</v>
+        <v>462</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D61" s="18" t="s">
         <v>8</v>
@@ -3906,10 +3925,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>484</v>
+        <v>467</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D62" s="18" t="s">
         <v>8</v>
@@ -3924,7 +3943,7 @@
         <v>427</v>
       </c>
       <c r="H62" t="s">
-        <v>486</v>
+        <v>469</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -3932,10 +3951,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>487</v>
+        <v>470</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D63" s="18" t="s">
         <v>8</v>
@@ -3955,10 +3974,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="73" t="s">
-        <v>488</v>
+        <v>471</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D64" s="18" t="s">
         <v>8</v>
@@ -3978,10 +3997,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="74" t="s">
-        <v>491</v>
+        <v>474</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D65" s="18" t="s">
         <v>8</v>
@@ -3996,7 +4015,7 @@
         <v>427</v>
       </c>
       <c r="H65" t="s">
-        <v>500</v>
+        <v>479</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -4004,10 +4023,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="74" t="s">
-        <v>501</v>
+        <v>480</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D66" s="18" t="s">
         <v>8</v>
@@ -4022,7 +4041,7 @@
         <v>427</v>
       </c>
       <c r="H66" t="s">
-        <v>504</v>
+        <v>483</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -4030,10 +4049,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>503</v>
+        <v>482</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D67" s="18" t="s">
         <v>8</v>
@@ -4053,10 +4072,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>505</v>
+        <v>484</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D68" s="18" t="s">
         <v>8</v>
@@ -4071,7 +4090,7 @@
         <v>427</v>
       </c>
       <c r="H68" t="s">
-        <v>507</v>
+        <v>486</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -4079,10 +4098,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>511</v>
+        <v>490</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D69" s="18" t="s">
         <v>8</v>
@@ -4097,7 +4116,7 @@
         <v>427</v>
       </c>
       <c r="H69" t="s">
-        <v>515</v>
+        <v>494</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -4105,10 +4124,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>510</v>
+        <v>489</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D70" s="18" t="s">
         <v>8</v>
@@ -4128,10 +4147,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>516</v>
+        <v>495</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D71" s="18" t="s">
         <v>8</v>
@@ -4151,10 +4170,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>517</v>
+        <v>496</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D72" s="18" t="s">
         <v>8</v>
@@ -4174,10 +4193,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>518</v>
+        <v>497</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D73" s="18" t="s">
         <v>8</v>
@@ -4197,10 +4216,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="75" t="s">
-        <v>521</v>
+        <v>500</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D74" s="18" t="s">
         <v>8</v>
@@ -4220,10 +4239,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="27" t="s">
-        <v>524</v>
+        <v>503</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D75" s="7" t="s">
         <v>8</v>
@@ -4243,10 +4262,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="23" t="s">
-        <v>525</v>
+        <v>504</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D76" s="7" t="s">
         <v>8</v>
@@ -4261,7 +4280,7 @@
         <v>427</v>
       </c>
       <c r="H76" t="s">
-        <v>530</v>
+        <v>509</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -4269,7 +4288,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>527</v>
+        <v>506</v>
       </c>
       <c r="C77" s="7" t="s">
         <v>56</v>
@@ -4281,13 +4300,59 @@
         <v>109</v>
       </c>
       <c r="F77" s="18" t="s">
-        <v>532</v>
+        <v>426</v>
       </c>
       <c r="G77" t="s">
+        <v>427</v>
+      </c>
+      <c r="H77" t="s">
         <v>533</v>
       </c>
-      <c r="H77" t="s">
-        <v>531</v>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="7">
+        <v>77</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>527</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D78" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E78" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="F78" s="18" t="s">
+        <v>426</v>
+      </c>
+      <c r="G78" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="7">
+        <v>78</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>534</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D79" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E79" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="F79" s="18" t="s">
+        <v>535</v>
+      </c>
+      <c r="G79" t="s">
+        <v>536</v>
       </c>
     </row>
   </sheetData>
@@ -4303,10 +4368,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9856292-E718-4F44-A2EB-03A51CA4C0E1}">
-  <dimension ref="A1:DZ54"/>
+  <dimension ref="A1:DZ56"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView topLeftCell="C39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4720,7 +4785,7 @@
         <v>412</v>
       </c>
       <c r="DD1" s="2" t="s">
-        <v>519</v>
+        <v>498</v>
       </c>
     </row>
     <row r="2" spans="1:108" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -5109,7 +5174,7 @@
         <v>293</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>450</v>
+        <v>436</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>424</v>
@@ -8516,10 +8581,10 @@
         <v>56</v>
       </c>
       <c r="CN22" s="15" t="s">
-        <v>442</v>
+        <v>519</v>
       </c>
       <c r="CO22" s="15" t="s">
-        <v>441</v>
+        <v>518</v>
       </c>
       <c r="CP22" s="28" t="s">
         <v>56</v>
@@ -9475,7 +9540,7 @@
         <v>424</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>493</v>
+        <v>529</v>
       </c>
       <c r="M30" s="23" t="s">
         <v>4</v>
@@ -9505,13 +9570,13 @@
         <v>23</v>
       </c>
       <c r="AA30" s="58" t="s">
-        <v>494</v>
+        <v>530</v>
       </c>
       <c r="AB30" s="2" t="s">
         <v>84</v>
       </c>
       <c r="AC30" s="24" t="s">
-        <v>451</v>
+        <v>437</v>
       </c>
       <c r="AD30" s="24" t="s">
         <v>345</v>
@@ -9520,10 +9585,10 @@
         <v>98</v>
       </c>
       <c r="AF30" s="23" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="AG30" s="24" t="s">
-        <v>496</v>
+        <v>476</v>
       </c>
       <c r="AH30" s="23"/>
       <c r="AI30" s="23" t="s">
@@ -9560,7 +9625,7 @@
         <v>336</v>
       </c>
       <c r="DC30" s="58" t="s">
-        <v>495</v>
+        <v>531</v>
       </c>
     </row>
     <row r="31" spans="1:109" x14ac:dyDescent="0.25">
@@ -9582,7 +9647,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>456</v>
+        <v>440</v>
       </c>
       <c r="C32" s="23" t="s">
         <v>83</v>
@@ -9591,10 +9656,10 @@
         <v>424</v>
       </c>
       <c r="I32" s="23" t="s">
-        <v>457</v>
+        <v>441</v>
       </c>
       <c r="J32" s="23" t="s">
-        <v>459</v>
+        <v>442</v>
       </c>
       <c r="K32" s="23"/>
       <c r="L32" s="24"/>
@@ -9765,7 +9830,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>460</v>
+        <v>443</v>
       </c>
       <c r="C33" s="23" t="s">
         <v>83</v>
@@ -9774,17 +9839,17 @@
         <v>424</v>
       </c>
       <c r="E33" s="58" t="s">
-        <v>465</v>
+        <v>448</v>
       </c>
       <c r="F33" s="58"/>
       <c r="I33" s="23" t="s">
-        <v>463</v>
+        <v>446</v>
       </c>
       <c r="J33" s="23" t="s">
-        <v>462</v>
+        <v>445</v>
       </c>
       <c r="K33" s="23" t="s">
-        <v>464</v>
+        <v>447</v>
       </c>
       <c r="L33" s="24"/>
       <c r="M33" s="23" t="s">
@@ -9904,7 +9969,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>469</v>
+        <v>452</v>
       </c>
       <c r="C34" s="23" t="s">
         <v>83</v>
@@ -9913,10 +9978,10 @@
         <v>424</v>
       </c>
       <c r="E34" s="58" t="s">
-        <v>465</v>
+        <v>448</v>
       </c>
       <c r="I34" s="23" t="s">
-        <v>467</v>
+        <v>450</v>
       </c>
       <c r="J34" s="23"/>
       <c r="K34" s="23"/>
@@ -9928,7 +9993,7 @@
         <v>345</v>
       </c>
       <c r="O34" s="25" t="s">
-        <v>468</v>
+        <v>451</v>
       </c>
       <c r="P34" s="23"/>
       <c r="Q34" s="23"/>
@@ -10038,7 +10103,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>470</v>
+        <v>453</v>
       </c>
       <c r="C35" s="23" t="s">
         <v>27</v>
@@ -10047,16 +10112,16 @@
         <v>424</v>
       </c>
       <c r="E35" s="26" t="s">
-        <v>471</v>
+        <v>454</v>
       </c>
       <c r="F35" s="23"/>
       <c r="G35" s="23"/>
       <c r="H35" s="23"/>
       <c r="I35" s="23" t="s">
-        <v>472</v>
+        <v>455</v>
       </c>
       <c r="J35" s="23" t="s">
-        <v>473</v>
+        <v>456</v>
       </c>
       <c r="K35" s="23"/>
       <c r="L35" s="24"/>
@@ -10226,7 +10291,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>475</v>
+        <v>458</v>
       </c>
       <c r="C36" s="23" t="s">
         <v>27</v>
@@ -10235,10 +10300,10 @@
         <v>424</v>
       </c>
       <c r="E36" s="58" t="s">
-        <v>476</v>
+        <v>459</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>477</v>
+        <v>460</v>
       </c>
     </row>
     <row r="37" spans="1:130" x14ac:dyDescent="0.25">
@@ -10246,7 +10311,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>478</v>
+        <v>461</v>
       </c>
       <c r="C37" s="23" t="s">
         <v>27</v>
@@ -10255,13 +10320,13 @@
         <v>424</v>
       </c>
       <c r="E37" s="58" t="s">
+        <v>448</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="K37" s="2" t="s">
         <v>465</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="38" spans="1:130" x14ac:dyDescent="0.25">
@@ -10269,7 +10334,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>479</v>
+        <v>462</v>
       </c>
       <c r="C38" s="23" t="s">
         <v>27</v>
@@ -10278,10 +10343,10 @@
         <v>424</v>
       </c>
       <c r="E38" s="58" t="s">
-        <v>480</v>
+        <v>463</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>483</v>
+        <v>466</v>
       </c>
     </row>
     <row r="39" spans="1:130" x14ac:dyDescent="0.25">
@@ -10289,7 +10354,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>484</v>
+        <v>467</v>
       </c>
       <c r="C39" s="23" t="s">
         <v>27</v>
@@ -10298,13 +10363,13 @@
         <v>424</v>
       </c>
       <c r="E39" s="58" t="s">
-        <v>480</v>
+        <v>463</v>
       </c>
       <c r="F39" s="23"/>
       <c r="G39" s="23"/>
       <c r="H39" s="23"/>
       <c r="I39" s="23" t="s">
-        <v>485</v>
+        <v>468</v>
       </c>
       <c r="J39" s="23"/>
       <c r="K39" s="23"/>
@@ -10497,7 +10562,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>487</v>
+        <v>470</v>
       </c>
       <c r="C40" s="23" t="s">
         <v>27</v>
@@ -10506,7 +10571,7 @@
         <v>424</v>
       </c>
       <c r="E40" s="58" t="s">
-        <v>480</v>
+        <v>463</v>
       </c>
     </row>
     <row r="41" spans="1:130" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -10514,7 +10579,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="73" t="s">
-        <v>488</v>
+        <v>471</v>
       </c>
       <c r="C41" s="23" t="s">
         <v>83</v>
@@ -10527,10 +10592,10 @@
       <c r="G41" s="23"/>
       <c r="H41" s="23"/>
       <c r="I41" s="23" t="s">
-        <v>489</v>
+        <v>472</v>
       </c>
       <c r="J41" s="23" t="s">
-        <v>492</v>
+        <v>475</v>
       </c>
       <c r="K41" s="23"/>
       <c r="L41" s="24"/>
@@ -10704,7 +10769,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="74" t="s">
-        <v>491</v>
+        <v>474</v>
       </c>
       <c r="C42" s="23" t="s">
         <v>27</v>
@@ -10717,7 +10782,7 @@
       <c r="G42" s="28"/>
       <c r="H42" s="28"/>
       <c r="I42" s="28" t="s">
-        <v>490</v>
+        <v>473</v>
       </c>
       <c r="J42" s="28"/>
       <c r="K42" s="28"/>
@@ -10870,10 +10935,10 @@
         <v>334</v>
       </c>
       <c r="CT42" s="24" t="s">
-        <v>499</v>
+        <v>478</v>
       </c>
       <c r="CU42" s="24" t="s">
-        <v>499</v>
+        <v>478</v>
       </c>
       <c r="CV42" s="25" t="s">
         <v>263</v>
@@ -10889,7 +10954,7 @@
         <v>76</v>
       </c>
       <c r="DA42" s="24" t="s">
-        <v>498</v>
+        <v>477</v>
       </c>
       <c r="DB42" s="28" t="s">
         <v>365</v>
@@ -10900,7 +10965,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="74" t="s">
-        <v>501</v>
+        <v>480</v>
       </c>
       <c r="C43" s="23" t="s">
         <v>27</v>
@@ -10913,7 +10978,7 @@
       <c r="G43" s="23"/>
       <c r="H43" s="23"/>
       <c r="I43" s="23" t="s">
-        <v>502</v>
+        <v>481</v>
       </c>
       <c r="J43" s="23"/>
       <c r="K43" s="23"/>
@@ -11082,7 +11147,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>503</v>
+        <v>482</v>
       </c>
       <c r="C44" s="23" t="s">
         <v>27</v>
@@ -11096,7 +11161,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>505</v>
+        <v>484</v>
       </c>
       <c r="C45" s="23" t="s">
         <v>27</v>
@@ -11109,7 +11174,7 @@
       <c r="G45" s="23"/>
       <c r="H45" s="23"/>
       <c r="I45" s="23" t="s">
-        <v>506</v>
+        <v>485</v>
       </c>
       <c r="J45" s="23"/>
       <c r="K45" s="23"/>
@@ -11275,7 +11340,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>511</v>
+        <v>490</v>
       </c>
       <c r="C46" s="23" t="s">
         <v>27</v>
@@ -11288,10 +11353,10 @@
       <c r="G46" s="23"/>
       <c r="H46" s="23"/>
       <c r="I46" s="23" t="s">
-        <v>508</v>
+        <v>487</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>509</v>
+        <v>488</v>
       </c>
       <c r="K46" s="23"/>
       <c r="L46" s="24"/>
@@ -11459,7 +11524,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>510</v>
+        <v>489</v>
       </c>
       <c r="C47" s="23" t="s">
         <v>27</v>
@@ -11468,16 +11533,16 @@
         <v>424</v>
       </c>
       <c r="E47" s="58" t="s">
-        <v>512</v>
+        <v>491</v>
       </c>
       <c r="F47" s="58" t="s">
-        <v>513</v>
+        <v>492</v>
       </c>
       <c r="G47" s="58" t="s">
-        <v>465</v>
+        <v>448</v>
       </c>
       <c r="H47" s="58" t="s">
-        <v>514</v>
+        <v>493</v>
       </c>
     </row>
     <row r="48" spans="1:130" x14ac:dyDescent="0.25">
@@ -11485,7 +11550,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>516</v>
+        <v>495</v>
       </c>
       <c r="C48" s="23" t="s">
         <v>27</v>
@@ -11494,7 +11559,7 @@
         <v>424</v>
       </c>
       <c r="E48" s="58" t="s">
-        <v>512</v>
+        <v>491</v>
       </c>
     </row>
     <row r="49" spans="1:108" x14ac:dyDescent="0.25">
@@ -11502,7 +11567,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>517</v>
+        <v>496</v>
       </c>
       <c r="C49" s="23" t="s">
         <v>27</v>
@@ -11511,7 +11576,7 @@
         <v>424</v>
       </c>
       <c r="E49" s="58" t="s">
-        <v>512</v>
+        <v>491</v>
       </c>
     </row>
     <row r="50" spans="1:108" x14ac:dyDescent="0.25">
@@ -11519,7 +11584,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>518</v>
+        <v>497</v>
       </c>
       <c r="C50" s="23" t="s">
         <v>27</v>
@@ -11529,7 +11594,7 @@
       </c>
       <c r="E50" s="58"/>
       <c r="DD50" s="58" t="s">
-        <v>520</v>
+        <v>499</v>
       </c>
     </row>
     <row r="51" spans="1:108" ht="30" x14ac:dyDescent="0.25">
@@ -11537,7 +11602,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="75" t="s">
-        <v>521</v>
+        <v>500</v>
       </c>
       <c r="C51" s="23" t="s">
         <v>27</v>
@@ -11546,10 +11611,10 @@
         <v>424</v>
       </c>
       <c r="E51" s="58" t="s">
-        <v>523</v>
+        <v>502</v>
       </c>
       <c r="F51" s="58" t="s">
-        <v>522</v>
+        <v>501</v>
       </c>
     </row>
     <row r="52" spans="1:108" x14ac:dyDescent="0.25">
@@ -11557,7 +11622,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="27" t="s">
-        <v>524</v>
+        <v>503</v>
       </c>
       <c r="C52" s="23" t="s">
         <v>27</v>
@@ -11753,7 +11818,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>525</v>
+        <v>504</v>
       </c>
       <c r="C53" s="23" t="s">
         <v>83</v>
@@ -11766,7 +11831,7 @@
       <c r="G53" s="23"/>
       <c r="H53" s="23"/>
       <c r="I53" s="23" t="s">
-        <v>526</v>
+        <v>505</v>
       </c>
       <c r="J53" s="23"/>
       <c r="K53" s="23"/>
@@ -11943,7 +12008,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>527</v>
+        <v>506</v>
       </c>
       <c r="C54" s="23" t="s">
         <v>27</v>
@@ -11952,13 +12017,13 @@
         <v>424</v>
       </c>
       <c r="E54" s="26" t="s">
-        <v>528</v>
+        <v>507</v>
       </c>
       <c r="F54" s="23"/>
       <c r="G54" s="23"/>
       <c r="H54" s="23"/>
       <c r="I54" s="23" t="s">
-        <v>529</v>
+        <v>508</v>
       </c>
       <c r="J54" s="23"/>
       <c r="K54" s="23"/>
@@ -12120,6 +12185,40 @@
       </c>
       <c r="CZ54" s="23"/>
       <c r="DA54" s="23"/>
+    </row>
+    <row r="55" spans="1:108" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>54</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>527</v>
+      </c>
+      <c r="C55" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D55" s="23" t="s">
+        <v>424</v>
+      </c>
+      <c r="E55" s="58" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="56" spans="1:108" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>55</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>534</v>
+      </c>
+      <c r="C56" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D56" s="23" t="s">
+        <v>424</v>
+      </c>
+      <c r="E56" s="58" t="s">
+        <v>507</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -14341,6 +14440,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006150CD2B74865543AE839454BD4B5DC6" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a2ee5e546ec1836f671c2a05bfe6bfc8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0be14d6d-d8a1-45f7-9f98-2db40f8691c4" xmlns:ns3="567c5c99-f8da-409a-bc28-51b94ad9a241" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e7ff770c31624934d8e1a633c6fbe95" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -14574,25 +14691,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB0B3A61-2E64-4CE7-BDD4-6ECB945D22FD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E980A1B9-8C22-45F7-8344-5E520FA354EB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64F77A26-17A6-43DF-A115-F9EC24E62EB0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14610,22 +14727,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E980A1B9-8C22-45F7-8344-5E520FA354EB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB0B3A61-2E64-4CE7-BDD4-6ECB945D22FD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Committing new Test cases
</commit_message>
<xml_diff>
--- a/data/CRM_Testdata.xlsx
+++ b/data/CRM_Testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\vkamalak\git\Dynamics-CRM-Stage\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC17EDF-EDAD-4B73-A99B-E67811D8361F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C686CE-B2EF-416B-B4A5-2DE787B7EAAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="599" xr2:uid="{442E3441-3F3C-4A77-BB17-E93CAE512719}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2415" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2415" uniqueCount="540">
   <si>
     <t>UserName</t>
   </si>
@@ -1325,9 +1325,6 @@
     <t/>
   </si>
   <si>
-    <t>2000554813</t>
-  </si>
-  <si>
     <t>7000578823</t>
   </si>
   <si>
@@ -1355,12 +1352,6 @@
     <t>10/30/2022</t>
   </si>
   <si>
-    <t>2000555818</t>
-  </si>
-  <si>
-    <t>2000555820</t>
-  </si>
-  <si>
     <t>TFS ID_45306:Verify Prospect accounts can not be published</t>
   </si>
   <si>
@@ -1448,9 +1439,6 @@
     <t>45309_CreateSubAccountwithoutDPException</t>
   </si>
   <si>
-    <t>2000555965</t>
-  </si>
-  <si>
     <t>TFS ID_45321:Verify DP Relation Date is cleared if Is Top Parent Is Set to Yes</t>
   </si>
   <si>
@@ -1568,9 +1556,6 @@
     <t>11228_VerifyDraftStatus</t>
   </si>
   <si>
-    <t>2000556237</t>
-  </si>
-  <si>
     <t>2000556507</t>
   </si>
   <si>
@@ -1643,13 +1628,37 @@
     <t>TFS ID_43706: 11232: Cloud: Verify warning message is displayed when there is any DP change of an account with children (non location type)</t>
   </si>
   <si>
-    <t>2000556583</t>
-  </si>
-  <si>
     <t>PASSED</t>
   </si>
   <si>
-    <t>2022_11_15_02_50_42</t>
+    <t>2000556599</t>
+  </si>
+  <si>
+    <t>2000556636</t>
+  </si>
+  <si>
+    <t>1000155542</t>
+  </si>
+  <si>
+    <t>2000556653</t>
+  </si>
+  <si>
+    <t>2000556662</t>
+  </si>
+  <si>
+    <t>2022_11_16_10_35_31</t>
+  </si>
+  <si>
+    <t>2000556663</t>
+  </si>
+  <si>
+    <t>2022_11_16_10_39_48</t>
+  </si>
+  <si>
+    <t>2000556664</t>
+  </si>
+  <si>
+    <t>2022_11_16_10_43_53</t>
   </si>
 </sst>
 </file>
@@ -2356,8 +2365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088699A3-39D2-44E6-8F71-47C2709580BF}">
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C29"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2411,7 +2420,7 @@
         <v>57</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>8</v>
@@ -2426,7 +2435,7 @@
         <v>427</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="I2" s="46" t="s">
         <v>416</v>
@@ -2443,7 +2452,7 @@
         <v>58</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>8</v>
@@ -2452,13 +2461,13 @@
         <v>109</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>426</v>
+        <v>529</v>
       </c>
       <c r="G3" t="s">
-        <v>427</v>
+        <v>535</v>
       </c>
       <c r="H3" t="s">
-        <v>438</v>
+        <v>534</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2469,7 +2478,7 @@
         <v>60</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>8</v>
@@ -2484,7 +2493,7 @@
         <v>427</v>
       </c>
       <c r="H4" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="J4" s="46" t="s">
         <v>425</v>
@@ -2498,7 +2507,7 @@
         <v>59</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D5" s="18" t="s">
         <v>8</v>
@@ -2507,13 +2516,13 @@
         <v>109</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>426</v>
+        <v>529</v>
       </c>
       <c r="G5" t="s">
-        <v>427</v>
+        <v>537</v>
       </c>
       <c r="H5" t="s">
-        <v>439</v>
+        <v>536</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2524,7 +2533,7 @@
         <v>70</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D6" s="18" t="s">
         <v>8</v>
@@ -2547,7 +2556,7 @@
         <v>71</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>8</v>
@@ -2570,7 +2579,7 @@
         <v>73</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>8</v>
@@ -2585,7 +2594,7 @@
         <v>427</v>
       </c>
       <c r="H8" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2596,7 +2605,7 @@
         <v>74</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>8</v>
@@ -2619,7 +2628,7 @@
         <v>92</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>8</v>
@@ -2634,7 +2643,7 @@
         <v>427</v>
       </c>
       <c r="H10" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2645,7 +2654,7 @@
         <v>95</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>8</v>
@@ -2654,13 +2663,13 @@
         <v>109</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>426</v>
+        <v>529</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>427</v>
+        <v>539</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>428</v>
+        <v>538</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2671,7 +2680,7 @@
         <v>94</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>8</v>
@@ -2686,7 +2695,7 @@
         <v>427</v>
       </c>
       <c r="H12" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2697,7 +2706,7 @@
         <v>99</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D13" s="18" t="s">
         <v>8</v>
@@ -2720,7 +2729,7 @@
         <v>361</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>8</v>
@@ -2743,7 +2752,7 @@
         <v>90</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>8</v>
@@ -2758,7 +2767,7 @@
         <v>427</v>
       </c>
       <c r="H15" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2769,7 +2778,7 @@
         <v>89</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>8</v>
@@ -2784,7 +2793,7 @@
         <v>427</v>
       </c>
       <c r="H16" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="61" customFormat="1" x14ac:dyDescent="0.25">
@@ -2795,7 +2804,7 @@
         <v>188</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D17" s="61" t="s">
         <v>8</v>
@@ -2818,7 +2827,7 @@
         <v>100</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>8</v>
@@ -2841,7 +2850,7 @@
         <v>108</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>8</v>
@@ -2864,7 +2873,7 @@
         <v>362</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>8</v>
@@ -2887,7 +2896,7 @@
         <v>346</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D21" s="18" t="s">
         <v>8</v>
@@ -2902,7 +2911,7 @@
         <v>427</v>
       </c>
       <c r="H21" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2913,7 +2922,7 @@
         <v>258</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>8</v>
@@ -2928,7 +2937,7 @@
         <v>427</v>
       </c>
       <c r="H22" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2939,7 +2948,7 @@
         <v>257</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>8</v>
@@ -2954,7 +2963,7 @@
         <v>427</v>
       </c>
       <c r="H23" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2965,7 +2974,7 @@
         <v>247</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D24" s="18" t="s">
         <v>8</v>
@@ -2980,7 +2989,7 @@
         <v>427</v>
       </c>
       <c r="H24" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2991,7 +3000,7 @@
         <v>259</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>8</v>
@@ -3006,7 +3015,7 @@
         <v>427</v>
       </c>
       <c r="H25" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -3017,7 +3026,7 @@
         <v>260</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>8</v>
@@ -3032,7 +3041,7 @@
         <v>427</v>
       </c>
       <c r="H26" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -3043,7 +3052,7 @@
         <v>261</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D27" s="18" t="s">
         <v>8</v>
@@ -3058,7 +3067,7 @@
         <v>427</v>
       </c>
       <c r="H27" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -3069,7 +3078,7 @@
         <v>265</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D28" s="18" t="s">
         <v>8</v>
@@ -3084,7 +3093,7 @@
         <v>427</v>
       </c>
       <c r="H28" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="61" customFormat="1" x14ac:dyDescent="0.25">
@@ -3095,7 +3104,7 @@
         <v>293</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D29" s="61" t="s">
         <v>8</v>
@@ -3133,7 +3142,7 @@
         <v>427</v>
       </c>
       <c r="H30" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="67" customFormat="1" x14ac:dyDescent="0.25">
@@ -3534,7 +3543,7 @@
         <v>427</v>
       </c>
       <c r="H46" s="69" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="I46" s="69"/>
     </row>
@@ -3561,7 +3570,7 @@
         <v>427</v>
       </c>
       <c r="H47" s="69" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="I47" s="69"/>
     </row>
@@ -3588,7 +3597,7 @@
         <v>427</v>
       </c>
       <c r="H48" s="69" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="I48" s="69"/>
     </row>
@@ -3615,7 +3624,7 @@
         <v>427</v>
       </c>
       <c r="H49" s="69" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="I49" s="69"/>
     </row>
@@ -3642,7 +3651,7 @@
         <v>427</v>
       </c>
       <c r="H50" s="69" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I50" s="69"/>
     </row>
@@ -3719,7 +3728,7 @@
         <v>427</v>
       </c>
       <c r="H53" s="69" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="I53" s="69"/>
     </row>
@@ -3746,7 +3755,7 @@
         <v>427</v>
       </c>
       <c r="H54" s="69" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="I54" s="69"/>
     </row>
@@ -3755,10 +3764,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D55" s="18" t="s">
         <v>8</v>
@@ -3773,7 +3782,7 @@
         <v>427</v>
       </c>
       <c r="H55" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -3781,10 +3790,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D56" s="18" t="s">
         <v>8</v>
@@ -3799,7 +3808,7 @@
         <v>427</v>
       </c>
       <c r="H56" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -3807,10 +3816,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D57" s="18" t="s">
         <v>8</v>
@@ -3830,10 +3839,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D58" s="18" t="s">
         <v>8</v>
@@ -3848,7 +3857,7 @@
         <v>427</v>
       </c>
       <c r="H58" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -3856,10 +3865,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D59" s="18" t="s">
         <v>8</v>
@@ -3879,10 +3888,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D60" s="18" t="s">
         <v>8</v>
@@ -3902,10 +3911,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D61" s="18" t="s">
         <v>8</v>
@@ -3925,10 +3934,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D62" s="18" t="s">
         <v>8</v>
@@ -3943,7 +3952,7 @@
         <v>427</v>
       </c>
       <c r="H62" t="s">
-        <v>469</v>
+        <v>533</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -3951,10 +3960,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D63" s="18" t="s">
         <v>8</v>
@@ -3974,10 +3983,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="73" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D64" s="18" t="s">
         <v>8</v>
@@ -3997,10 +4006,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="74" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D65" s="18" t="s">
         <v>8</v>
@@ -4015,7 +4024,7 @@
         <v>427</v>
       </c>
       <c r="H65" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -4023,10 +4032,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="74" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D66" s="18" t="s">
         <v>8</v>
@@ -4041,7 +4050,7 @@
         <v>427</v>
       </c>
       <c r="H66" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -4049,10 +4058,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D67" s="18" t="s">
         <v>8</v>
@@ -4072,10 +4081,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D68" s="18" t="s">
         <v>8</v>
@@ -4090,7 +4099,7 @@
         <v>427</v>
       </c>
       <c r="H68" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -4098,10 +4107,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D69" s="18" t="s">
         <v>8</v>
@@ -4116,7 +4125,7 @@
         <v>427</v>
       </c>
       <c r="H69" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -4124,10 +4133,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D70" s="18" t="s">
         <v>8</v>
@@ -4147,10 +4156,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D71" s="18" t="s">
         <v>8</v>
@@ -4170,10 +4179,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D72" s="18" t="s">
         <v>8</v>
@@ -4193,10 +4202,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D73" s="18" t="s">
         <v>8</v>
@@ -4216,10 +4225,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="75" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D74" s="18" t="s">
         <v>8</v>
@@ -4239,10 +4248,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="27" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D75" s="7" t="s">
         <v>8</v>
@@ -4262,10 +4271,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="23" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D76" s="7" t="s">
         <v>8</v>
@@ -4280,7 +4289,7 @@
         <v>427</v>
       </c>
       <c r="H76" t="s">
-        <v>509</v>
+        <v>531</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -4288,10 +4297,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D77" s="7" t="s">
         <v>8</v>
@@ -4306,7 +4315,7 @@
         <v>427</v>
       </c>
       <c r="H77" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -4314,10 +4323,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D78" s="7" t="s">
         <v>8</v>
@@ -4337,10 +4346,10 @@
         <v>78</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D79" s="7" t="s">
         <v>8</v>
@@ -4349,10 +4358,10 @@
         <v>109</v>
       </c>
       <c r="F79" s="18" t="s">
-        <v>535</v>
+        <v>426</v>
       </c>
       <c r="G79" t="s">
-        <v>536</v>
+        <v>427</v>
       </c>
     </row>
   </sheetData>
@@ -4370,9 +4379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9856292-E718-4F44-A2EB-03A51CA4C0E1}">
   <dimension ref="A1:DZ56"/>
   <sheetViews>
-    <sheetView topLeftCell="C39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4785,7 +4792,7 @@
         <v>412</v>
       </c>
       <c r="DD1" s="2" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="2" spans="1:108" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -5174,7 +5181,7 @@
         <v>293</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>424</v>
@@ -8581,10 +8588,10 @@
         <v>56</v>
       </c>
       <c r="CN22" s="15" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="CO22" s="15" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="CP22" s="28" t="s">
         <v>56</v>
@@ -9540,7 +9547,7 @@
         <v>424</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="M30" s="23" t="s">
         <v>4</v>
@@ -9570,13 +9577,13 @@
         <v>23</v>
       </c>
       <c r="AA30" s="58" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="AB30" s="2" t="s">
         <v>84</v>
       </c>
       <c r="AC30" s="24" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="AD30" s="24" t="s">
         <v>345</v>
@@ -9588,7 +9595,7 @@
         <v>409</v>
       </c>
       <c r="AG30" s="24" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="AH30" s="23"/>
       <c r="AI30" s="23" t="s">
@@ -9625,7 +9632,7 @@
         <v>336</v>
       </c>
       <c r="DC30" s="58" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
     </row>
     <row r="31" spans="1:109" x14ac:dyDescent="0.25">
@@ -9647,7 +9654,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="C32" s="23" t="s">
         <v>83</v>
@@ -9656,10 +9663,10 @@
         <v>424</v>
       </c>
       <c r="I32" s="23" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="J32" s="23" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="K32" s="23"/>
       <c r="L32" s="24"/>
@@ -9830,7 +9837,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="C33" s="23" t="s">
         <v>83</v>
@@ -9839,17 +9846,17 @@
         <v>424</v>
       </c>
       <c r="E33" s="58" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="F33" s="58"/>
       <c r="I33" s="23" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="J33" s="23" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="K33" s="23" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="L33" s="24"/>
       <c r="M33" s="23" t="s">
@@ -9969,7 +9976,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="C34" s="23" t="s">
         <v>83</v>
@@ -9978,10 +9985,10 @@
         <v>424</v>
       </c>
       <c r="E34" s="58" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="I34" s="23" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="J34" s="23"/>
       <c r="K34" s="23"/>
@@ -9993,7 +10000,7 @@
         <v>345</v>
       </c>
       <c r="O34" s="25" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="P34" s="23"/>
       <c r="Q34" s="23"/>
@@ -10103,7 +10110,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C35" s="23" t="s">
         <v>27</v>
@@ -10112,16 +10119,16 @@
         <v>424</v>
       </c>
       <c r="E35" s="26" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="F35" s="23"/>
       <c r="G35" s="23"/>
       <c r="H35" s="23"/>
       <c r="I35" s="23" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="J35" s="23" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="K35" s="23"/>
       <c r="L35" s="24"/>
@@ -10291,7 +10298,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="C36" s="23" t="s">
         <v>27</v>
@@ -10300,10 +10307,10 @@
         <v>424</v>
       </c>
       <c r="E36" s="58" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="37" spans="1:130" x14ac:dyDescent="0.25">
@@ -10311,7 +10318,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="C37" s="23" t="s">
         <v>27</v>
@@ -10320,13 +10327,13 @@
         <v>424</v>
       </c>
       <c r="E37" s="58" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="38" spans="1:130" x14ac:dyDescent="0.25">
@@ -10334,7 +10341,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="C38" s="23" t="s">
         <v>27</v>
@@ -10343,10 +10350,10 @@
         <v>424</v>
       </c>
       <c r="E38" s="58" t="s">
+        <v>460</v>
+      </c>
+      <c r="J38" s="2" t="s">
         <v>463</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="39" spans="1:130" x14ac:dyDescent="0.25">
@@ -10354,7 +10361,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="C39" s="23" t="s">
         <v>27</v>
@@ -10363,13 +10370,13 @@
         <v>424</v>
       </c>
       <c r="E39" s="58" t="s">
-        <v>463</v>
+        <v>532</v>
       </c>
       <c r="F39" s="23"/>
       <c r="G39" s="23"/>
       <c r="H39" s="23"/>
       <c r="I39" s="23" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="J39" s="23"/>
       <c r="K39" s="23"/>
@@ -10562,7 +10569,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="C40" s="23" t="s">
         <v>27</v>
@@ -10571,7 +10578,7 @@
         <v>424</v>
       </c>
       <c r="E40" s="58" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="41" spans="1:130" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -10579,7 +10586,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="73" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="C41" s="23" t="s">
         <v>83</v>
@@ -10592,10 +10599,10 @@
       <c r="G41" s="23"/>
       <c r="H41" s="23"/>
       <c r="I41" s="23" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="J41" s="23" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="K41" s="23"/>
       <c r="L41" s="24"/>
@@ -10769,7 +10776,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="74" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="C42" s="23" t="s">
         <v>27</v>
@@ -10782,7 +10789,7 @@
       <c r="G42" s="28"/>
       <c r="H42" s="28"/>
       <c r="I42" s="28" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="J42" s="28"/>
       <c r="K42" s="28"/>
@@ -10935,10 +10942,10 @@
         <v>334</v>
       </c>
       <c r="CT42" s="24" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="CU42" s="24" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="CV42" s="25" t="s">
         <v>263</v>
@@ -10954,7 +10961,7 @@
         <v>76</v>
       </c>
       <c r="DA42" s="24" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="DB42" s="28" t="s">
         <v>365</v>
@@ -10965,7 +10972,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="74" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="C43" s="23" t="s">
         <v>27</v>
@@ -10978,7 +10985,7 @@
       <c r="G43" s="23"/>
       <c r="H43" s="23"/>
       <c r="I43" s="23" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="J43" s="23"/>
       <c r="K43" s="23"/>
@@ -11147,7 +11154,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="C44" s="23" t="s">
         <v>27</v>
@@ -11161,7 +11168,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="C45" s="23" t="s">
         <v>27</v>
@@ -11174,7 +11181,7 @@
       <c r="G45" s="23"/>
       <c r="H45" s="23"/>
       <c r="I45" s="23" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="J45" s="23"/>
       <c r="K45" s="23"/>
@@ -11340,7 +11347,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="C46" s="23" t="s">
         <v>27</v>
@@ -11353,10 +11360,10 @@
       <c r="G46" s="23"/>
       <c r="H46" s="23"/>
       <c r="I46" s="23" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="K46" s="23"/>
       <c r="L46" s="24"/>
@@ -11524,7 +11531,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="C47" s="23" t="s">
         <v>27</v>
@@ -11533,16 +11540,16 @@
         <v>424</v>
       </c>
       <c r="E47" s="58" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="F47" s="58" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="G47" s="58" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="H47" s="58" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
     </row>
     <row r="48" spans="1:130" x14ac:dyDescent="0.25">
@@ -11550,7 +11557,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="C48" s="23" t="s">
         <v>27</v>
@@ -11559,7 +11566,7 @@
         <v>424</v>
       </c>
       <c r="E48" s="58" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
     </row>
     <row r="49" spans="1:108" x14ac:dyDescent="0.25">
@@ -11567,7 +11574,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="C49" s="23" t="s">
         <v>27</v>
@@ -11576,7 +11583,7 @@
         <v>424</v>
       </c>
       <c r="E49" s="58" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
     </row>
     <row r="50" spans="1:108" x14ac:dyDescent="0.25">
@@ -11584,7 +11591,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="C50" s="23" t="s">
         <v>27</v>
@@ -11594,7 +11601,7 @@
       </c>
       <c r="E50" s="58"/>
       <c r="DD50" s="58" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
     </row>
     <row r="51" spans="1:108" ht="30" x14ac:dyDescent="0.25">
@@ -11602,7 +11609,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="75" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C51" s="23" t="s">
         <v>27</v>
@@ -11611,10 +11618,10 @@
         <v>424</v>
       </c>
       <c r="E51" s="58" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="F51" s="58" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="52" spans="1:108" x14ac:dyDescent="0.25">
@@ -11622,7 +11629,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="27" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="C52" s="23" t="s">
         <v>27</v>
@@ -11818,7 +11825,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="C53" s="23" t="s">
         <v>83</v>
@@ -11831,7 +11838,7 @@
       <c r="G53" s="23"/>
       <c r="H53" s="23"/>
       <c r="I53" s="23" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="J53" s="23"/>
       <c r="K53" s="23"/>
@@ -12008,7 +12015,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="C54" s="23" t="s">
         <v>27</v>
@@ -12017,13 +12024,13 @@
         <v>424</v>
       </c>
       <c r="E54" s="26" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="F54" s="23"/>
       <c r="G54" s="23"/>
       <c r="H54" s="23"/>
       <c r="I54" s="23" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="J54" s="23"/>
       <c r="K54" s="23"/>
@@ -12191,7 +12198,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="C55" s="23" t="s">
         <v>27</v>
@@ -12200,7 +12207,7 @@
         <v>424</v>
       </c>
       <c r="E55" s="58" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
     </row>
     <row r="56" spans="1:108" x14ac:dyDescent="0.25">
@@ -12208,7 +12215,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="C56" s="23" t="s">
         <v>27</v>
@@ -12217,7 +12224,7 @@
         <v>424</v>
       </c>
       <c r="E56" s="58" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
     </row>
   </sheetData>
@@ -14440,6 +14447,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006150CD2B74865543AE839454BD4B5DC6" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a2ee5e546ec1836f671c2a05bfe6bfc8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0be14d6d-d8a1-45f7-9f98-2db40f8691c4" xmlns:ns3="567c5c99-f8da-409a-bc28-51b94ad9a241" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e7ff770c31624934d8e1a633c6fbe95" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -14673,25 +14698,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB0B3A61-2E64-4CE7-BDD4-6ECB945D22FD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E980A1B9-8C22-45F7-8344-5E520FA354EB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64F77A26-17A6-43DF-A115-F9EC24E62EB0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14709,22 +14734,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E980A1B9-8C22-45F7-8344-5E520FA354EB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB0B3A61-2E64-4CE7-BDD4-6ECB945D22FD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updating Run Mode for Supplier 20 cases batch run
</commit_message>
<xml_diff>
--- a/data/CRM_Testdata.xlsx
+++ b/data/CRM_Testdata.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\vkamalak\git\Dynamics-CRM-Stage\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\fahmed2\git\Dynamics-CRM-Stage\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70595C44-617F-4A9C-8780-A5F8A5AA594D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7B6473-365E-44EE-B1CE-F2B674912B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="599" activeTab="1" xr2:uid="{442E3441-3F3C-4A77-BB17-E93CAE512719}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="599" xr2:uid="{442E3441-3F3C-4A77-BB17-E93CAE512719}"/>
   </bookViews>
   <sheets>
     <sheet name="Driver" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2784" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2616" uniqueCount="557">
   <si>
     <t>UserName</t>
   </si>
@@ -1698,9 +1698,6 @@
   </si>
   <si>
     <t>1000074769</t>
-  </si>
-  <si>
-    <t>2022_11_22_04_47_08</t>
   </si>
   <si>
     <t>44754_MemberEntryProspectFirst</t>
@@ -2419,22 +2416,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088699A3-39D2-44E6-8F71-47C2709580BF}">
   <dimension ref="A1:J85"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="7" width="5.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="7" width="93.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="7" width="11.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="7" width="15.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="7" width="15.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="7" width="8.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="7" width="20.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="7" width="12.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="7" width="32.0" collapsed="true"/>
-    <col min="10" max="16384" style="7" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="5.140625" style="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="93.42578125" style="7" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11" style="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.5703125" style="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.5703125" style="7" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.140625" style="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.28515625" style="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.28515625" style="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="32" style="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="16384" width="9.140625" style="7" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -3207,7 +3204,7 @@
         <v>50</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D31" s="65" t="s">
         <v>47</v>
@@ -3232,7 +3229,7 @@
         <v>126</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D32" s="65" t="s">
         <v>47</v>
@@ -3257,7 +3254,7 @@
         <v>131</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D33" s="65" t="s">
         <v>47</v>
@@ -3282,7 +3279,7 @@
         <v>138</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D34" s="65" t="s">
         <v>47</v>
@@ -3307,7 +3304,7 @@
         <v>143</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D35" s="65" t="s">
         <v>47</v>
@@ -3332,7 +3329,7 @@
         <v>148</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D36" s="65" t="s">
         <v>47</v>
@@ -3357,7 +3354,7 @@
         <v>152</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D37" s="65" t="s">
         <v>47</v>
@@ -3382,7 +3379,7 @@
         <v>157</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D38" s="65" t="s">
         <v>47</v>
@@ -3407,7 +3404,7 @@
         <v>160</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D39" s="65" t="s">
         <v>47</v>
@@ -3432,7 +3429,7 @@
         <v>163</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D40" s="65" t="s">
         <v>47</v>
@@ -3457,7 +3454,7 @@
         <v>168</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D41" s="65" t="s">
         <v>47</v>
@@ -3482,7 +3479,7 @@
         <v>175</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D42" s="65" t="s">
         <v>47</v>
@@ -3507,7 +3504,7 @@
         <v>182</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D43" s="65" t="s">
         <v>47</v>
@@ -3532,7 +3529,7 @@
         <v>375</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D44" s="65" t="s">
         <v>47</v>
@@ -3557,7 +3554,7 @@
         <v>267</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D45" s="65" t="s">
         <v>47</v>
@@ -3582,7 +3579,7 @@
         <v>305</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D46" s="69" t="s">
         <v>303</v>
@@ -3609,7 +3606,7 @@
         <v>309</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D47" s="69" t="s">
         <v>303</v>
@@ -3636,7 +3633,7 @@
         <v>308</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D48" s="69" t="s">
         <v>303</v>
@@ -3663,7 +3660,7 @@
         <v>323</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D49" s="69" t="s">
         <v>303</v>
@@ -3690,7 +3687,7 @@
         <v>333</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D50" s="69" t="s">
         <v>303</v>
@@ -4550,7 +4547,7 @@
         <v>551</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D85" s="7" t="s">
         <v>8</v>
@@ -4559,13 +4556,13 @@
         <v>109</v>
       </c>
       <c r="F85" s="18" t="s">
+        <v>555</v>
+      </c>
+      <c r="G85" t="s">
         <v>556</v>
       </c>
-      <c r="G85" t="s">
-        <v>557</v>
-      </c>
       <c r="H85" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
   </sheetData>
@@ -4583,97 +4580,97 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9856292-E718-4F44-A2EB-03A51CA4C0E1}">
   <dimension ref="A1:EM62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="5.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="102.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="14.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="14.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="10.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="11.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="12.85546875" collapsed="true"/>
-    <col min="8" max="9" customWidth="true" style="2" width="12.85546875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="69.140625" collapsed="true"/>
-    <col min="11" max="12" customWidth="true" style="2" width="36.5703125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="20.0" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="15.42578125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="16.7109375" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="2" width="14.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="2" width="20.140625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="2" width="21.7109375" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="2" width="27.140625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="2" width="18.5703125" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="2" width="10.42578125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="2" width="4.42578125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="2" width="8.0" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="2" width="7.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="2" width="8.28515625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="2" width="19.85546875" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="2" width="24.140625" collapsed="true"/>
-    <col min="31" max="31" customWidth="true" style="2" width="24.140625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="2" width="9.85546875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="2" width="17.85546875" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="2" width="22.140625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="2" width="9.5703125" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" style="2" width="21.85546875" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" style="2" width="26.28515625" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" style="2" width="30.42578125" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" style="2" width="23.28515625" collapsed="true"/>
-    <col min="40" max="42" customWidth="true" style="2" width="23.28515625" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" style="2" width="7.28515625" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" style="2" width="22.28515625" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" style="2" width="24.5703125" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" style="2" width="8.85546875" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" style="2" width="16.7109375" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" style="2" width="6.0" collapsed="true"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" style="2" width="20.5703125" collapsed="true"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" style="2" width="20.28515625" collapsed="true"/>
-    <col min="51" max="51" bestFit="true" customWidth="true" style="2" width="26.42578125" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" style="2" width="24.28515625" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" style="2" width="27.0" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" style="2" width="25.0" collapsed="true"/>
-    <col min="55" max="55" bestFit="true" customWidth="true" style="2" width="29.0" collapsed="true"/>
-    <col min="56" max="57" bestFit="true" customWidth="true" style="2" width="15.140625" collapsed="true"/>
-    <col min="58" max="58" bestFit="true" customWidth="true" style="2" width="25.5703125" collapsed="true"/>
-    <col min="59" max="59" bestFit="true" customWidth="true" style="2" width="15.7109375" collapsed="true"/>
-    <col min="60" max="60" bestFit="true" customWidth="true" style="2" width="17.85546875" collapsed="true"/>
-    <col min="61" max="61" bestFit="true" customWidth="true" style="2" width="14.5703125" collapsed="true"/>
-    <col min="62" max="62" bestFit="true" customWidth="true" style="2" width="11.85546875" collapsed="true"/>
-    <col min="63" max="63" bestFit="true" customWidth="true" style="2" width="17.28515625" collapsed="true"/>
-    <col min="64" max="64" bestFit="true" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
-    <col min="65" max="65" bestFit="true" customWidth="true" style="2" width="15.28515625" collapsed="true"/>
-    <col min="66" max="66" bestFit="true" customWidth="true" style="2" width="19.85546875" collapsed="true"/>
-    <col min="67" max="67" bestFit="true" customWidth="true" style="2" width="19.42578125" collapsed="true"/>
-    <col min="68" max="68" bestFit="true" customWidth="true" style="2" width="14.42578125" collapsed="true"/>
-    <col min="69" max="69" bestFit="true" customWidth="true" style="2" width="14.7109375" collapsed="true"/>
-    <col min="70" max="70" bestFit="true" customWidth="true" style="2" width="10.7109375" collapsed="true"/>
-    <col min="71" max="71" bestFit="true" customWidth="true" style="2" width="19.42578125" collapsed="true"/>
-    <col min="72" max="72" bestFit="true" customWidth="true" style="2" width="12.28515625" collapsed="true"/>
-    <col min="73" max="73" bestFit="true" customWidth="true" style="2" width="9.28515625" collapsed="true"/>
-    <col min="74" max="74" bestFit="true" customWidth="true" style="2" width="14.140625" collapsed="true"/>
-    <col min="75" max="75" bestFit="true" customWidth="true" style="2" width="32.0" collapsed="true"/>
-    <col min="76" max="76" bestFit="true" customWidth="true" style="2" width="16.28515625" collapsed="true"/>
-    <col min="77" max="83" style="2" width="9.140625" collapsed="true"/>
-    <col min="84" max="84" bestFit="true" customWidth="true" style="2" width="10.0" collapsed="true"/>
-    <col min="85" max="96" style="2" width="9.140625" collapsed="true"/>
-    <col min="97" max="97" customWidth="true" style="2" width="28.28515625" collapsed="true"/>
-    <col min="98" max="98" bestFit="true" customWidth="true" style="2" width="22.140625" collapsed="true"/>
-    <col min="99" max="99" bestFit="true" customWidth="true" style="2" width="26.140625" collapsed="true"/>
-    <col min="100" max="100" customWidth="true" style="2" width="26.140625" collapsed="true"/>
-    <col min="101" max="101" bestFit="true" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
-    <col min="102" max="102" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
-    <col min="103" max="103" bestFit="true" customWidth="true" style="2" width="22.85546875" collapsed="true"/>
-    <col min="104" max="104" bestFit="true" customWidth="true" style="2" width="18.140625" collapsed="true"/>
-    <col min="105" max="105" customWidth="true" style="2" width="18.140625" collapsed="true"/>
-    <col min="106" max="106" bestFit="true" customWidth="true" style="2" width="18.28515625" collapsed="true"/>
-    <col min="107" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="5.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="102.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="12.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="69.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="12" width="36.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="20.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="20" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="15.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="16.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="14.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="20.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="21.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="27.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="18.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="10.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="4.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="8" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="7.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="8.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="12.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="19.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="24.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="24.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="9.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="17.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="22.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="9.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="21.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="26.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="30.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="23.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="42" width="23.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="7.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="22.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="24.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="8.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="16.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="6" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="20.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="20.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="24.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="27" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="25" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="29" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="57" width="15.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="25.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="15.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="17.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="14.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="62" max="62" width="11.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="63" max="63" width="17.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="64" max="64" width="12.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="65" max="65" width="15.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="66" max="66" width="19.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="67" max="67" width="19.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="68" max="68" width="14.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="69" max="69" width="14.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="70" max="70" width="10.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="71" max="71" width="19.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="72" max="72" width="12.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="73" max="73" width="9.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="74" max="74" width="14.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="75" max="75" width="32" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="76" max="76" width="16.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="77" max="83" width="9.140625" style="2" collapsed="1"/>
+    <col min="84" max="84" width="10" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="85" max="96" width="9.140625" style="2" collapsed="1"/>
+    <col min="97" max="97" width="28.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="98" max="98" width="22.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="99" max="99" width="26.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="100" max="100" width="26.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="101" max="101" width="12.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="102" max="102" width="12.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="103" max="103" width="22.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="104" max="104" width="18.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="105" max="105" width="18.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="106" max="106" width="18.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="107" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:109" x14ac:dyDescent="0.25">
@@ -13090,7 +13087,7 @@
         <v>552</v>
       </c>
       <c r="J62" s="23" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="K62" s="23"/>
       <c r="L62" s="23"/>
@@ -13300,63 +13297,63 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D073B921-24DF-4F78-BD1E-1984D65F897D}">
   <dimension ref="A1:BC17"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="V13" sqref="V13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="114.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="82.42578125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="24.5703125" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="34.85546875" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="31" max="33" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="34" max="34" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="35" max="36" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="4.140625" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" width="5.7109375" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="6.7109375" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="51" max="51" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="114" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="82.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="34.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.5703125" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="33" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="9.5703125" customWidth="1" collapsed="1"/>
+    <col min="35" max="36" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="4.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="5.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="6.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:55" x14ac:dyDescent="0.25">
@@ -14895,25 +14892,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="113.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="65.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="73.85546875" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="113.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="65.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="73.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
@@ -15506,6 +15503,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006150CD2B74865543AE839454BD4B5DC6" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a2ee5e546ec1836f671c2a05bfe6bfc8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0be14d6d-d8a1-45f7-9f98-2db40f8691c4" xmlns:ns3="567c5c99-f8da-409a-bc28-51b94ad9a241" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e7ff770c31624934d8e1a633c6fbe95" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -15739,25 +15754,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E980A1B9-8C22-45F7-8344-5E520FA354EB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB0B3A61-2E64-4CE7-BDD4-6ECB945D22FD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64F77A26-17A6-43DF-A115-F9EC24E62EB0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15775,22 +15790,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB0B3A61-2E64-4CE7-BDD4-6ECB945D22FD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E980A1B9-8C22-45F7-8344-5E520FA354EB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Data sheet update for batch run -Supplier
</commit_message>
<xml_diff>
--- a/data/CRM_Testdata.xlsx
+++ b/data/CRM_Testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\fahmed2\git\Dynamics-CRM-Stage\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7B6473-365E-44EE-B1CE-F2B674912B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC19244-7233-4B2E-ABB2-40EA0B0D3C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="599" xr2:uid="{442E3441-3F3C-4A77-BB17-E93CAE512719}"/>
   </bookViews>
@@ -2416,8 +2416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088699A3-39D2-44E6-8F71-47C2709580BF}">
   <dimension ref="A1:J85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3714,7 +3714,7 @@
         <v>332</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D51" s="69" t="s">
         <v>303</v>
@@ -15503,24 +15503,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006150CD2B74865543AE839454BD4B5DC6" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a2ee5e546ec1836f671c2a05bfe6bfc8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0be14d6d-d8a1-45f7-9f98-2db40f8691c4" xmlns:ns3="567c5c99-f8da-409a-bc28-51b94ad9a241" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e7ff770c31624934d8e1a633c6fbe95" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -15754,25 +15736,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E980A1B9-8C22-45F7-8344-5E520FA354EB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB0B3A61-2E64-4CE7-BDD4-6ECB945D22FD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64F77A26-17A6-43DF-A115-F9EC24E62EB0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15790,4 +15772,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB0B3A61-2E64-4CE7-BDD4-6ECB945D22FD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E980A1B9-8C22-45F7-8344-5E520FA354EB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Member 28 , Contact 3 Run- Test Data Update
</commit_message>
<xml_diff>
--- a/data/CRM_Testdata.xlsx
+++ b/data/CRM_Testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\fahmed2\git\Dynamics-CRM-Stage\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC19244-7233-4B2E-ABB2-40EA0B0D3C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30D5A53-F910-43AC-A97B-EAA71A050DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="599" xr2:uid="{442E3441-3F3C-4A77-BB17-E93CAE512719}"/>
   </bookViews>
@@ -2417,7 +2417,7 @@
   <dimension ref="A1:J85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2471,7 +2471,7 @@
         <v>57</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>8</v>
@@ -2503,7 +2503,7 @@
         <v>58</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>8</v>
@@ -2529,7 +2529,7 @@
         <v>60</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>8</v>
@@ -2558,7 +2558,7 @@
         <v>59</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" s="18" t="s">
         <v>8</v>
@@ -2584,7 +2584,7 @@
         <v>70</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" s="18" t="s">
         <v>8</v>
@@ -2607,7 +2607,7 @@
         <v>71</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>8</v>
@@ -2630,7 +2630,7 @@
         <v>73</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>8</v>
@@ -2656,7 +2656,7 @@
         <v>74</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>8</v>
@@ -2679,7 +2679,7 @@
         <v>92</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>8</v>
@@ -2705,7 +2705,7 @@
         <v>95</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>8</v>
@@ -2731,7 +2731,7 @@
         <v>94</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>8</v>
@@ -2757,7 +2757,7 @@
         <v>99</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" s="18" t="s">
         <v>8</v>
@@ -2780,7 +2780,7 @@
         <v>361</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>8</v>
@@ -2803,7 +2803,7 @@
         <v>90</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>8</v>
@@ -2829,7 +2829,7 @@
         <v>89</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>8</v>
@@ -2855,7 +2855,7 @@
         <v>188</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D17" s="61" t="s">
         <v>8</v>
@@ -2878,7 +2878,7 @@
         <v>100</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>8</v>
@@ -2901,7 +2901,7 @@
         <v>108</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>8</v>
@@ -2924,7 +2924,7 @@
         <v>362</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>8</v>
@@ -2947,7 +2947,7 @@
         <v>346</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D21" s="18" t="s">
         <v>8</v>
@@ -2973,7 +2973,7 @@
         <v>258</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>8</v>
@@ -2999,7 +2999,7 @@
         <v>257</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>8</v>
@@ -3025,7 +3025,7 @@
         <v>247</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D24" s="18" t="s">
         <v>8</v>
@@ -3051,7 +3051,7 @@
         <v>259</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>8</v>
@@ -3077,7 +3077,7 @@
         <v>260</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>8</v>
@@ -3103,7 +3103,7 @@
         <v>261</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D27" s="18" t="s">
         <v>8</v>
@@ -3129,7 +3129,7 @@
         <v>265</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D28" s="18" t="s">
         <v>8</v>
@@ -3155,7 +3155,7 @@
         <v>293</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D29" s="61" t="s">
         <v>8</v>
@@ -3204,7 +3204,7 @@
         <v>50</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D31" s="65" t="s">
         <v>47</v>
@@ -3229,7 +3229,7 @@
         <v>126</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D32" s="65" t="s">
         <v>47</v>
@@ -3254,7 +3254,7 @@
         <v>131</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D33" s="65" t="s">
         <v>47</v>
@@ -3279,7 +3279,7 @@
         <v>138</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D34" s="65" t="s">
         <v>47</v>
@@ -3304,7 +3304,7 @@
         <v>143</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D35" s="65" t="s">
         <v>47</v>
@@ -3329,7 +3329,7 @@
         <v>148</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D36" s="65" t="s">
         <v>47</v>
@@ -3354,7 +3354,7 @@
         <v>152</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D37" s="65" t="s">
         <v>47</v>
@@ -3379,7 +3379,7 @@
         <v>157</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D38" s="65" t="s">
         <v>47</v>
@@ -3404,7 +3404,7 @@
         <v>160</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D39" s="65" t="s">
         <v>47</v>
@@ -3429,7 +3429,7 @@
         <v>163</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D40" s="65" t="s">
         <v>47</v>
@@ -3454,7 +3454,7 @@
         <v>168</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D41" s="65" t="s">
         <v>47</v>
@@ -3479,7 +3479,7 @@
         <v>175</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D42" s="65" t="s">
         <v>47</v>
@@ -3504,7 +3504,7 @@
         <v>182</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D43" s="65" t="s">
         <v>47</v>
@@ -3529,7 +3529,7 @@
         <v>375</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D44" s="65" t="s">
         <v>47</v>
@@ -3554,7 +3554,7 @@
         <v>267</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D45" s="65" t="s">
         <v>47</v>
@@ -3579,7 +3579,7 @@
         <v>305</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D46" s="69" t="s">
         <v>303</v>
@@ -3606,7 +3606,7 @@
         <v>309</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D47" s="69" t="s">
         <v>303</v>
@@ -3633,7 +3633,7 @@
         <v>308</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D48" s="69" t="s">
         <v>303</v>
@@ -3660,7 +3660,7 @@
         <v>323</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D49" s="69" t="s">
         <v>303</v>
@@ -3687,7 +3687,7 @@
         <v>333</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D50" s="69" t="s">
         <v>303</v>
@@ -3714,7 +3714,7 @@
         <v>332</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D51" s="69" t="s">
         <v>303</v>
@@ -3739,7 +3739,7 @@
         <v>329</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D52" s="69" t="s">
         <v>303</v>
@@ -3764,7 +3764,7 @@
         <v>339</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D53" s="69" t="s">
         <v>303</v>
@@ -3791,7 +3791,7 @@
         <v>340</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D54" s="69" t="s">
         <v>303</v>
@@ -15503,6 +15503,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006150CD2B74865543AE839454BD4B5DC6" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a2ee5e546ec1836f671c2a05bfe6bfc8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0be14d6d-d8a1-45f7-9f98-2db40f8691c4" xmlns:ns3="567c5c99-f8da-409a-bc28-51b94ad9a241" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e7ff770c31624934d8e1a633c6fbe95" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -15736,25 +15754,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E980A1B9-8C22-45F7-8344-5E520FA354EB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB0B3A61-2E64-4CE7-BDD4-6ECB945D22FD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64F77A26-17A6-43DF-A115-F9EC24E62EB0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15772,22 +15790,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB0B3A61-2E64-4CE7-BDD4-6ECB945D22FD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E980A1B9-8C22-45F7-8344-5E520FA354EB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Last batch run -Member 31 cases
</commit_message>
<xml_diff>
--- a/data/CRM_Testdata.xlsx
+++ b/data/CRM_Testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\fahmed2\git\Dynamics-CRM-Stage\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30D5A53-F910-43AC-A97B-EAA71A050DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5442054-E5CD-4962-8B57-2D41F8931A82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="599" xr2:uid="{442E3441-3F3C-4A77-BB17-E93CAE512719}"/>
   </bookViews>
@@ -1836,7 +1836,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1882,30 +1882,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1960,7 +1936,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2079,9 +2055,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2091,8 +2064,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2416,8 +2395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088699A3-39D2-44E6-8F71-47C2709580BF}">
   <dimension ref="A1:J85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2467,11 +2446,11 @@
       <c r="A2" s="18">
         <v>1</v>
       </c>
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="18" t="s">
         <v>57</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>8</v>
@@ -2499,11 +2478,11 @@
       <c r="A3" s="18">
         <v>2</v>
       </c>
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="18" t="s">
         <v>58</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>8</v>
@@ -2525,11 +2504,11 @@
       <c r="A4" s="18">
         <v>3</v>
       </c>
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="18" t="s">
         <v>60</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>8</v>
@@ -2554,11 +2533,11 @@
       <c r="A5" s="18">
         <v>4</v>
       </c>
-      <c r="B5" s="76" t="s">
+      <c r="B5" s="18" t="s">
         <v>59</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D5" s="18" t="s">
         <v>8</v>
@@ -2580,11 +2559,11 @@
       <c r="A6" s="18">
         <v>5</v>
       </c>
-      <c r="B6" s="71" t="s">
+      <c r="B6" s="18" t="s">
         <v>70</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D6" s="18" t="s">
         <v>8</v>
@@ -2603,11 +2582,11 @@
       <c r="A7" s="18">
         <v>6</v>
       </c>
-      <c r="B7" s="76" t="s">
+      <c r="B7" s="18" t="s">
         <v>71</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>8</v>
@@ -2626,11 +2605,11 @@
       <c r="A8" s="18">
         <v>7</v>
       </c>
-      <c r="B8" s="72" t="s">
+      <c r="B8" s="18" t="s">
         <v>73</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>8</v>
@@ -2652,11 +2631,11 @@
       <c r="A9" s="18">
         <v>8</v>
       </c>
-      <c r="B9" s="71" t="s">
+      <c r="B9" s="18" t="s">
         <v>74</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>8</v>
@@ -2675,11 +2654,11 @@
       <c r="A10" s="18">
         <v>9</v>
       </c>
-      <c r="B10" s="70" t="s">
+      <c r="B10" s="18" t="s">
         <v>92</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>8</v>
@@ -2701,11 +2680,11 @@
       <c r="A11" s="18">
         <v>10</v>
       </c>
-      <c r="B11" s="76" t="s">
+      <c r="B11" s="18" t="s">
         <v>95</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>8</v>
@@ -2727,11 +2706,11 @@
       <c r="A12" s="18">
         <v>11</v>
       </c>
-      <c r="B12" s="70" t="s">
+      <c r="B12" s="18" t="s">
         <v>94</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>8</v>
@@ -2753,11 +2732,11 @@
       <c r="A13" s="18">
         <v>12</v>
       </c>
-      <c r="B13" s="70" t="s">
+      <c r="B13" s="18" t="s">
         <v>99</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D13" s="18" t="s">
         <v>8</v>
@@ -2780,7 +2759,7 @@
         <v>361</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>8</v>
@@ -2799,11 +2778,11 @@
       <c r="A15" s="18">
         <v>14</v>
       </c>
-      <c r="B15" s="72" t="s">
+      <c r="B15" s="18" t="s">
         <v>90</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>8</v>
@@ -2825,11 +2804,11 @@
       <c r="A16" s="18">
         <v>15</v>
       </c>
-      <c r="B16" s="70" t="s">
+      <c r="B16" s="18" t="s">
         <v>89</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>8</v>
@@ -2851,11 +2830,11 @@
       <c r="A17" s="61">
         <v>16</v>
       </c>
-      <c r="B17" s="72" t="s">
+      <c r="B17" s="18" t="s">
         <v>188</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D17" s="61" t="s">
         <v>8</v>
@@ -2874,11 +2853,11 @@
       <c r="A18" s="18">
         <v>17</v>
       </c>
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="18" t="s">
         <v>100</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>8</v>
@@ -2897,11 +2876,11 @@
       <c r="A19" s="18">
         <v>18</v>
       </c>
-      <c r="B19" s="72" t="s">
+      <c r="B19" s="18" t="s">
         <v>108</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>8</v>
@@ -2920,11 +2899,11 @@
       <c r="A20" s="18">
         <v>19</v>
       </c>
-      <c r="B20" s="72" t="s">
+      <c r="B20" s="18" t="s">
         <v>362</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>8</v>
@@ -2943,11 +2922,11 @@
       <c r="A21" s="18">
         <v>20</v>
       </c>
-      <c r="B21" s="72" t="s">
+      <c r="B21" s="18" t="s">
         <v>346</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D21" s="18" t="s">
         <v>8</v>
@@ -2969,11 +2948,11 @@
       <c r="A22" s="18">
         <v>21</v>
       </c>
-      <c r="B22" s="71" t="s">
+      <c r="B22" s="18" t="s">
         <v>258</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>8</v>
@@ -2995,11 +2974,11 @@
       <c r="A23" s="18">
         <v>22</v>
       </c>
-      <c r="B23" s="71" t="s">
+      <c r="B23" s="18" t="s">
         <v>257</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>8</v>
@@ -3021,11 +3000,11 @@
       <c r="A24" s="18">
         <v>23</v>
       </c>
-      <c r="B24" s="71" t="s">
+      <c r="B24" s="18" t="s">
         <v>247</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D24" s="18" t="s">
         <v>8</v>
@@ -3047,11 +3026,11 @@
       <c r="A25" s="18">
         <v>24</v>
       </c>
-      <c r="B25" s="71" t="s">
+      <c r="B25" s="18" t="s">
         <v>259</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>8</v>
@@ -3073,11 +3052,11 @@
       <c r="A26" s="18">
         <v>25</v>
       </c>
-      <c r="B26" s="71" t="s">
+      <c r="B26" s="18" t="s">
         <v>260</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>8</v>
@@ -3099,11 +3078,11 @@
       <c r="A27" s="18">
         <v>26</v>
       </c>
-      <c r="B27" s="71" t="s">
+      <c r="B27" s="18" t="s">
         <v>261</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D27" s="18" t="s">
         <v>8</v>
@@ -3129,7 +3108,7 @@
         <v>265</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D28" s="18" t="s">
         <v>8</v>
@@ -3151,11 +3130,11 @@
       <c r="A29" s="61">
         <v>28</v>
       </c>
-      <c r="B29" s="76" t="s">
+      <c r="B29" s="18" t="s">
         <v>293</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D29" s="61" t="s">
         <v>8</v>
@@ -3174,7 +3153,7 @@
       <c r="A30" s="60">
         <v>29</v>
       </c>
-      <c r="B30" s="60" t="s">
+      <c r="B30" s="18" t="s">
         <v>411</v>
       </c>
       <c r="C30" s="7" t="s">
@@ -3200,7 +3179,7 @@
       <c r="A31" s="64">
         <v>30</v>
       </c>
-      <c r="B31" s="65" t="s">
+      <c r="B31" s="73" t="s">
         <v>50</v>
       </c>
       <c r="C31" s="7" t="s">
@@ -3225,7 +3204,7 @@
       <c r="A32" s="64">
         <v>31</v>
       </c>
-      <c r="B32" s="65" t="s">
+      <c r="B32" s="73" t="s">
         <v>126</v>
       </c>
       <c r="C32" s="7" t="s">
@@ -3250,7 +3229,7 @@
       <c r="A33" s="64">
         <v>32</v>
       </c>
-      <c r="B33" s="65" t="s">
+      <c r="B33" s="73" t="s">
         <v>131</v>
       </c>
       <c r="C33" s="7" t="s">
@@ -3275,7 +3254,7 @@
       <c r="A34" s="64">
         <v>33</v>
       </c>
-      <c r="B34" s="65" t="s">
+      <c r="B34" s="73" t="s">
         <v>138</v>
       </c>
       <c r="C34" s="7" t="s">
@@ -3300,7 +3279,7 @@
       <c r="A35" s="64">
         <v>34</v>
       </c>
-      <c r="B35" s="65" t="s">
+      <c r="B35" s="73" t="s">
         <v>143</v>
       </c>
       <c r="C35" s="7" t="s">
@@ -3325,7 +3304,7 @@
       <c r="A36" s="64">
         <v>35</v>
       </c>
-      <c r="B36" s="65" t="s">
+      <c r="B36" s="73" t="s">
         <v>148</v>
       </c>
       <c r="C36" s="7" t="s">
@@ -3350,7 +3329,7 @@
       <c r="A37" s="64">
         <v>36</v>
       </c>
-      <c r="B37" s="65" t="s">
+      <c r="B37" s="73" t="s">
         <v>152</v>
       </c>
       <c r="C37" s="7" t="s">
@@ -3375,7 +3354,7 @@
       <c r="A38" s="64">
         <v>37</v>
       </c>
-      <c r="B38" s="65" t="s">
+      <c r="B38" s="73" t="s">
         <v>157</v>
       </c>
       <c r="C38" s="7" t="s">
@@ -3400,7 +3379,7 @@
       <c r="A39" s="64">
         <v>38</v>
       </c>
-      <c r="B39" s="65" t="s">
+      <c r="B39" s="73" t="s">
         <v>160</v>
       </c>
       <c r="C39" s="7" t="s">
@@ -3425,7 +3404,7 @@
       <c r="A40" s="64">
         <v>39</v>
       </c>
-      <c r="B40" s="65" t="s">
+      <c r="B40" s="73" t="s">
         <v>163</v>
       </c>
       <c r="C40" s="7" t="s">
@@ -3450,7 +3429,7 @@
       <c r="A41" s="64">
         <v>40</v>
       </c>
-      <c r="B41" s="65" t="s">
+      <c r="B41" s="73" t="s">
         <v>168</v>
       </c>
       <c r="C41" s="7" t="s">
@@ -3475,7 +3454,7 @@
       <c r="A42" s="64">
         <v>41</v>
       </c>
-      <c r="B42" s="77" t="s">
+      <c r="B42" s="73" t="s">
         <v>175</v>
       </c>
       <c r="C42" s="7" t="s">
@@ -3500,7 +3479,7 @@
       <c r="A43" s="64">
         <v>42</v>
       </c>
-      <c r="B43" s="65" t="s">
+      <c r="B43" s="73" t="s">
         <v>182</v>
       </c>
       <c r="C43" s="7" t="s">
@@ -3525,7 +3504,7 @@
       <c r="A44" s="64">
         <v>43</v>
       </c>
-      <c r="B44" s="65" t="s">
+      <c r="B44" s="73" t="s">
         <v>375</v>
       </c>
       <c r="C44" s="7" t="s">
@@ -3550,7 +3529,7 @@
       <c r="A45" s="64">
         <v>44</v>
       </c>
-      <c r="B45" s="65" t="s">
+      <c r="B45" s="73" t="s">
         <v>267</v>
       </c>
       <c r="C45" s="7" t="s">
@@ -3575,7 +3554,7 @@
       <c r="A46" s="64">
         <v>45</v>
       </c>
-      <c r="B46" s="69" t="s">
+      <c r="B46" s="74" t="s">
         <v>305</v>
       </c>
       <c r="C46" s="7" t="s">
@@ -3602,7 +3581,7 @@
       <c r="A47" s="64">
         <v>46</v>
       </c>
-      <c r="B47" s="69" t="s">
+      <c r="B47" s="74" t="s">
         <v>309</v>
       </c>
       <c r="C47" s="7" t="s">
@@ -3629,7 +3608,7 @@
       <c r="A48" s="64">
         <v>47</v>
       </c>
-      <c r="B48" s="69" t="s">
+      <c r="B48" s="74" t="s">
         <v>308</v>
       </c>
       <c r="C48" s="7" t="s">
@@ -3656,7 +3635,7 @@
       <c r="A49" s="64">
         <v>48</v>
       </c>
-      <c r="B49" s="69" t="s">
+      <c r="B49" s="74" t="s">
         <v>323</v>
       </c>
       <c r="C49" s="7" t="s">
@@ -3683,7 +3662,7 @@
       <c r="A50" s="64">
         <v>49</v>
       </c>
-      <c r="B50" s="69" t="s">
+      <c r="B50" s="74" t="s">
         <v>333</v>
       </c>
       <c r="C50" s="7" t="s">
@@ -3710,7 +3689,7 @@
       <c r="A51" s="64">
         <v>50</v>
       </c>
-      <c r="B51" s="69" t="s">
+      <c r="B51" s="74" t="s">
         <v>332</v>
       </c>
       <c r="C51" s="7" t="s">
@@ -3735,11 +3714,11 @@
       <c r="A52" s="64">
         <v>51</v>
       </c>
-      <c r="B52" s="69" t="s">
+      <c r="B52" s="74" t="s">
         <v>329</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D52" s="69" t="s">
         <v>303</v>
@@ -3760,11 +3739,11 @@
       <c r="A53" s="64">
         <v>52</v>
       </c>
-      <c r="B53" s="69" t="s">
+      <c r="B53" s="74" t="s">
         <v>339</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D53" s="69" t="s">
         <v>303</v>
@@ -3787,11 +3766,11 @@
       <c r="A54" s="64">
         <v>53</v>
       </c>
-      <c r="B54" s="68" t="s">
+      <c r="B54" s="57" t="s">
         <v>340</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D54" s="69" t="s">
         <v>303</v>
@@ -3818,7 +3797,7 @@
         <v>437</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D55" s="18" t="s">
         <v>8</v>
@@ -3840,11 +3819,11 @@
       <c r="A56" s="7">
         <v>55</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="14" t="s">
         <v>440</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D56" s="18" t="s">
         <v>8</v>
@@ -3870,7 +3849,7 @@
         <v>449</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D57" s="18" t="s">
         <v>8</v>
@@ -3893,7 +3872,7 @@
         <v>450</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D58" s="18" t="s">
         <v>8</v>
@@ -3915,11 +3894,11 @@
       <c r="A59" s="7">
         <v>58</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="14" t="s">
         <v>455</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D59" s="18" t="s">
         <v>8</v>
@@ -3938,11 +3917,11 @@
       <c r="A60" s="7">
         <v>59</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="14" t="s">
         <v>458</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D60" s="18" t="s">
         <v>8</v>
@@ -3965,7 +3944,7 @@
         <v>459</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D61" s="18" t="s">
         <v>8</v>
@@ -3984,11 +3963,11 @@
       <c r="A62" s="7">
         <v>61</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B62" s="14" t="s">
         <v>464</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D62" s="18" t="s">
         <v>8</v>
@@ -4014,7 +3993,7 @@
         <v>466</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D63" s="18" t="s">
         <v>8</v>
@@ -4033,11 +4012,11 @@
       <c r="A64" s="7">
         <v>63</v>
       </c>
-      <c r="B64" s="73" t="s">
+      <c r="B64" s="70" t="s">
         <v>467</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D64" s="18" t="s">
         <v>8</v>
@@ -4056,11 +4035,11 @@
       <c r="A65" s="7">
         <v>64</v>
       </c>
-      <c r="B65" s="74" t="s">
+      <c r="B65" s="75" t="s">
         <v>470</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D65" s="18" t="s">
         <v>8</v>
@@ -4082,11 +4061,11 @@
       <c r="A66" s="7">
         <v>65</v>
       </c>
-      <c r="B66" s="74" t="s">
+      <c r="B66" s="75" t="s">
         <v>476</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D66" s="18" t="s">
         <v>8</v>
@@ -4112,7 +4091,7 @@
         <v>478</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D67" s="18" t="s">
         <v>8</v>
@@ -4135,7 +4114,7 @@
         <v>480</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D68" s="18" t="s">
         <v>8</v>
@@ -4161,7 +4140,7 @@
         <v>486</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D69" s="18" t="s">
         <v>8</v>
@@ -4187,7 +4166,7 @@
         <v>485</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D70" s="18" t="s">
         <v>8</v>
@@ -4210,7 +4189,7 @@
         <v>491</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D71" s="18" t="s">
         <v>8</v>
@@ -4233,7 +4212,7 @@
         <v>492</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D72" s="18" t="s">
         <v>8</v>
@@ -4256,7 +4235,7 @@
         <v>493</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D73" s="18" t="s">
         <v>8</v>
@@ -4275,11 +4254,11 @@
       <c r="A74" s="7">
         <v>73</v>
       </c>
-      <c r="B74" s="75" t="s">
+      <c r="B74" s="76" t="s">
         <v>496</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D74" s="18" t="s">
         <v>8</v>
@@ -4302,7 +4281,7 @@
         <v>499</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D75" s="7" t="s">
         <v>8</v>
@@ -4321,11 +4300,11 @@
       <c r="A76" s="7">
         <v>75</v>
       </c>
-      <c r="B76" s="23" t="s">
+      <c r="B76" s="30" t="s">
         <v>500</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D76" s="7" t="s">
         <v>8</v>
@@ -4347,11 +4326,11 @@
       <c r="A77" s="7">
         <v>76</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B77" s="14" t="s">
         <v>502</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D77" s="7" t="s">
         <v>8</v>
@@ -4377,7 +4356,7 @@
         <v>521</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D78" s="7" t="s">
         <v>8</v>
@@ -4400,7 +4379,7 @@
         <v>528</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D79" s="7" t="s">
         <v>8</v>
@@ -4423,7 +4402,7 @@
         <v>536</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D80" s="7" t="s">
         <v>8</v>
@@ -4445,11 +4424,11 @@
       <c r="A81" s="7">
         <v>80</v>
       </c>
-      <c r="B81" s="74" t="s">
+      <c r="B81" s="75" t="s">
         <v>538</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D81" s="7" t="s">
         <v>8</v>
@@ -4472,7 +4451,7 @@
         <v>541</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D82" s="7" t="s">
         <v>8</v>
@@ -4498,7 +4477,7 @@
         <v>543</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D83" s="7" t="s">
         <v>8</v>
@@ -4521,7 +4500,7 @@
         <v>546</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D84" s="7" t="s">
         <v>8</v>
@@ -4547,7 +4526,7 @@
         <v>551</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D85" s="7" t="s">
         <v>8</v>
@@ -10831,7 +10810,7 @@
       <c r="A41" s="23">
         <v>40</v>
       </c>
-      <c r="B41" s="73" t="s">
+      <c r="B41" s="70" t="s">
         <v>467</v>
       </c>
       <c r="C41" s="23" t="s">
@@ -11022,7 +11001,7 @@
       <c r="A42" s="23">
         <v>41</v>
       </c>
-      <c r="B42" s="74" t="s">
+      <c r="B42" s="71" t="s">
         <v>470</v>
       </c>
       <c r="C42" s="23" t="s">
@@ -11219,7 +11198,7 @@
       <c r="A43" s="23">
         <v>42</v>
       </c>
-      <c r="B43" s="74" t="s">
+      <c r="B43" s="71" t="s">
         <v>476</v>
       </c>
       <c r="C43" s="23" t="s">
@@ -11864,7 +11843,7 @@
       <c r="A51" s="2">
         <v>50</v>
       </c>
-      <c r="B51" s="75" t="s">
+      <c r="B51" s="72" t="s">
         <v>496</v>
       </c>
       <c r="C51" s="23" t="s">
@@ -12652,7 +12631,7 @@
       <c r="A58" s="2">
         <v>57</v>
       </c>
-      <c r="B58" s="74" t="s">
+      <c r="B58" s="71" t="s">
         <v>538</v>
       </c>
       <c r="C58" s="23" t="s">
@@ -15503,24 +15482,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006150CD2B74865543AE839454BD4B5DC6" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a2ee5e546ec1836f671c2a05bfe6bfc8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0be14d6d-d8a1-45f7-9f98-2db40f8691c4" xmlns:ns3="567c5c99-f8da-409a-bc28-51b94ad9a241" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e7ff770c31624934d8e1a633c6fbe95" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -15754,25 +15715,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E980A1B9-8C22-45F7-8344-5E520FA354EB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB0B3A61-2E64-4CE7-BDD4-6ECB945D22FD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64F77A26-17A6-43DF-A115-F9EC24E62EB0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15790,4 +15751,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB0B3A61-2E64-4CE7-BDD4-6ECB945D22FD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E980A1B9-8C22-45F7-8344-5E520FA354EB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Committing Updated test cases
</commit_message>
<xml_diff>
--- a/data/CRM_Testdata.xlsx
+++ b/data/CRM_Testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\vkamalak\git\Dynamics-CRM-Stage\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC4D21A-409B-440C-B579-148A1C880C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDC353F-C4E0-411C-89AA-AE5206A6EA43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="599" activeTab="2" xr2:uid="{442E3441-3F3C-4A77-BB17-E93CAE512719}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="599" xr2:uid="{442E3441-3F3C-4A77-BB17-E93CAE512719}"/>
   </bookViews>
   <sheets>
     <sheet name="Driver" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3254" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3263" uniqueCount="651">
   <si>
     <t>UserName</t>
   </si>
@@ -1541,24 +1541,6 @@
     <t>11228_VerifyDraftStatus</t>
   </si>
   <si>
-    <t>2000556507</t>
-  </si>
-  <si>
-    <t>2000556509</t>
-  </si>
-  <si>
-    <t>2000556511</t>
-  </si>
-  <si>
-    <t>2000556512</t>
-  </si>
-  <si>
-    <t>2000556515</t>
-  </si>
-  <si>
-    <t>2000556516</t>
-  </si>
-  <si>
     <t>2000556519</t>
   </si>
   <si>
@@ -1610,21 +1592,9 @@
     <t>TFS ID_43706: 11232: Cloud: Verify warning message is displayed when there is any DP change of an account with children (non location type)</t>
   </si>
   <si>
-    <t>2000556599</t>
-  </si>
-  <si>
     <t>1000155542</t>
   </si>
   <si>
-    <t>2000556662</t>
-  </si>
-  <si>
-    <t>2000556663</t>
-  </si>
-  <si>
-    <t>2000556664</t>
-  </si>
-  <si>
     <t>TFS ID_45285:Verify whether the TPR is getting saved properly when DP change to different hierarchy</t>
   </si>
   <si>
@@ -1772,13 +1742,256 @@
     <t>2000133513</t>
   </si>
   <si>
-    <t>2022_11_29_11_53_36</t>
+    <t>TFS ID_43987:Test Case 9314 : Verify active supplier can not have DP without EIN</t>
+  </si>
+  <si>
+    <t>TFS ID_43986:Test Case 9315 :Verify terminated supplier can not have DP without EIN</t>
+  </si>
+  <si>
+    <t>1000001373</t>
+  </si>
+  <si>
+    <t>1000000245</t>
+  </si>
+  <si>
+    <t>TFS ID_45287:Validate Top Parent Relationship Date Change</t>
+  </si>
+  <si>
+    <t>TFS ID_44009:Test Case 8519 :Verify whether user should be able to update Premier Start date for the "Supplier" via Membership Entity</t>
+  </si>
+  <si>
+    <t>2000141822</t>
+  </si>
+  <si>
+    <t>TFS ID_43982:Test Case 9633 : Verify whether user should not get any script error on add any Supplier Diversity</t>
+  </si>
+  <si>
+    <t>DiversityValue</t>
+  </si>
+  <si>
+    <t>Minority Owned</t>
+  </si>
+  <si>
+    <t>CertifyingAgency</t>
+  </si>
+  <si>
+    <t>TFS ID_44011:Automation Test Case 8310 :Cloud : Verify the Premier End Date is removed from the Supplier Form when the accounts is reactivated</t>
+  </si>
+  <si>
+    <t>TFS ID_43980:Test Case 11064 :Verify when a Supplier is end dated, the End Reason  defaults to 'Change' automatically</t>
+  </si>
+  <si>
+    <t>TFS ID_44008:Test Case 8771 :Supplier Form - DP &amp; TP Search Look up should have only Supplier Accounts</t>
+  </si>
+  <si>
+    <t>43980 Verify End Reason</t>
+  </si>
+  <si>
+    <t>44011 Activate terminated supplier</t>
+  </si>
+  <si>
+    <t>2000171160</t>
+  </si>
+  <si>
+    <t>44008 Location DP</t>
+  </si>
+  <si>
+    <t>TFS ID_44013:Automation Test Case 6064 :Cloud: #Members field should be available in Member Form and removed from Supplier Form</t>
   </si>
   <si>
     <t>PASSED</t>
   </si>
   <si>
-    <t>2022_11_29_12_02_29</t>
+    <t>TFS ID_440131:Automation Test Case 6064 :Cloud: #Members field should be available in Member Form and removed from Supplier Form</t>
+  </si>
+  <si>
+    <t>TFS ID_44007:Test Case 8772 : Verify if member/member supervisor/Supplier/Supplier supervisor/Limited member can edit the primary account of a contact</t>
+  </si>
+  <si>
+    <t>7000509363</t>
+  </si>
+  <si>
+    <t>1000174081</t>
+  </si>
+  <si>
+    <t>2000394452</t>
+  </si>
+  <si>
+    <t>primaryAccountName</t>
+  </si>
+  <si>
+    <t>UserName3</t>
+  </si>
+  <si>
+    <t>UserName4</t>
+  </si>
+  <si>
+    <t>2000558743</t>
+  </si>
+  <si>
+    <t>2022_12_06_09_12_47</t>
+  </si>
+  <si>
+    <t>2000558744</t>
+  </si>
+  <si>
+    <t>2022_12_06_09_17_38</t>
+  </si>
+  <si>
+    <t>2000558745</t>
+  </si>
+  <si>
+    <t>2022_12_06_09_19_36</t>
+  </si>
+  <si>
+    <t>2000558746</t>
+  </si>
+  <si>
+    <t>2022_12_06_09_23_55</t>
+  </si>
+  <si>
+    <t>2022_12_06_09_27_57</t>
+  </si>
+  <si>
+    <t>2022_12_06_09_29_35</t>
+  </si>
+  <si>
+    <t>2000558748</t>
+  </si>
+  <si>
+    <t>2022_12_06_09_34_11</t>
+  </si>
+  <si>
+    <t>2022_12_06_09_38_27</t>
+  </si>
+  <si>
+    <t>2000558750</t>
+  </si>
+  <si>
+    <t>2022_12_06_09_41_33</t>
+  </si>
+  <si>
+    <t>2000558751</t>
+  </si>
+  <si>
+    <t>2022_12_06_09_45_35</t>
+  </si>
+  <si>
+    <t>2000558752</t>
+  </si>
+  <si>
+    <t>2022_12_06_09_48_49</t>
+  </si>
+  <si>
+    <t>2022_12_06_09_51_31</t>
+  </si>
+  <si>
+    <t>2022_12_06_09_56_12</t>
+  </si>
+  <si>
+    <t>2000558755</t>
+  </si>
+  <si>
+    <t>2022_12_06_09_58_23</t>
+  </si>
+  <si>
+    <t>2000558756</t>
+  </si>
+  <si>
+    <t>2022_12_06_10_01_50</t>
+  </si>
+  <si>
+    <t>2022_12_06_10_06_09</t>
+  </si>
+  <si>
+    <t>2022_12_07_08_32_56</t>
+  </si>
+  <si>
+    <t>2022_12_07_08_36_06</t>
+  </si>
+  <si>
+    <t>2022_12_07_08_36_57</t>
+  </si>
+  <si>
+    <t>2022_12_07_08_43_56</t>
+  </si>
+  <si>
+    <t>2000558763</t>
+  </si>
+  <si>
+    <t>338127555</t>
+  </si>
+  <si>
+    <t>ff2703874</t>
+  </si>
+  <si>
+    <t>2022_12_07_08_49_29</t>
+  </si>
+  <si>
+    <t>2022_12_07_08_50_37</t>
+  </si>
+  <si>
+    <t>2022_12_07_08_51_44</t>
+  </si>
+  <si>
+    <t>2022_12_07_08_52_52</t>
+  </si>
+  <si>
+    <t>2022_12_07_08_54_00</t>
+  </si>
+  <si>
+    <t>2022_12_07_08_55_07</t>
+  </si>
+  <si>
+    <t>2022_12_07_08_56_15</t>
+  </si>
+  <si>
+    <t>2022_12_07_08_57_23</t>
+  </si>
+  <si>
+    <t>2022_12_07_08_58_41</t>
+  </si>
+  <si>
+    <t>2022_12_07_09_00_09</t>
+  </si>
+  <si>
+    <t>2022_12_07_09_01_30</t>
+  </si>
+  <si>
+    <t>2022_12_07_09_02_37</t>
+  </si>
+  <si>
+    <t>2022_12_07_09_03_54</t>
+  </si>
+  <si>
+    <t>2022_12_07_09_05_15</t>
+  </si>
+  <si>
+    <t>2022_12_07_09_06_04</t>
+  </si>
+  <si>
+    <t>2022_12_07_09_07_26</t>
+  </si>
+  <si>
+    <t>2022_12_07_09_08_43</t>
+  </si>
+  <si>
+    <t>2022_12_07_09_10_00</t>
+  </si>
+  <si>
+    <t>2022_12_07_09_11_11</t>
+  </si>
+  <si>
+    <t>2022_12_07_09_12_15</t>
+  </si>
+  <si>
+    <t>2022_12_07_09_13_26</t>
+  </si>
+  <si>
+    <t>2022_12_07_09_16_45</t>
+  </si>
+  <si>
+    <t>2022_12_07_09_18_30</t>
   </si>
 </sst>
 </file>
@@ -2040,7 +2253,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2195,6 +2408,19 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2516,10 +2742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088699A3-39D2-44E6-8F71-47C2709580BF}">
-  <dimension ref="A1:J96"/>
+  <dimension ref="A1:J107"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2588,7 +2814,7 @@
         <v>427</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>523</v>
+        <v>595</v>
       </c>
       <c r="I2" s="45" t="s">
         <v>416</v>
@@ -2620,14 +2846,14 @@
         <v>427</v>
       </c>
       <c r="H3" t="s">
-        <v>525</v>
+        <v>597</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17">
         <v>3</v>
       </c>
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="94" t="s">
         <v>60</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -2646,7 +2872,7 @@
         <v>427</v>
       </c>
       <c r="H4" t="s">
-        <v>500</v>
+        <v>599</v>
       </c>
       <c r="J4" s="45" t="s">
         <v>425</v>
@@ -2675,7 +2901,7 @@
         <v>427</v>
       </c>
       <c r="H5" t="s">
-        <v>526</v>
+        <v>601</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -2705,7 +2931,7 @@
       <c r="A7" s="17">
         <v>6</v>
       </c>
-      <c r="B7" s="75" t="s">
+      <c r="B7" s="94" t="s">
         <v>71</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -2747,7 +2973,7 @@
         <v>427</v>
       </c>
       <c r="H8" t="s">
-        <v>501</v>
+        <v>605</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -2796,7 +3022,7 @@
         <v>427</v>
       </c>
       <c r="H10" t="s">
-        <v>502</v>
+        <v>608</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -2822,7 +3048,7 @@
         <v>427</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>527</v>
+        <v>610</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -2848,7 +3074,7 @@
         <v>427</v>
       </c>
       <c r="H12" t="s">
-        <v>503</v>
+        <v>612</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -2878,7 +3104,7 @@
       <c r="A14" s="17">
         <v>13</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="56" t="s">
         <v>361</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -2901,7 +3127,7 @@
       <c r="A15" s="17">
         <v>14</v>
       </c>
-      <c r="B15" s="71" t="s">
+      <c r="B15" s="93" t="s">
         <v>90</v>
       </c>
       <c r="C15" s="7" t="s">
@@ -2920,7 +3146,7 @@
         <v>427</v>
       </c>
       <c r="H15" t="s">
-        <v>504</v>
+        <v>616</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -2946,7 +3172,7 @@
         <v>427</v>
       </c>
       <c r="H16" t="s">
-        <v>505</v>
+        <v>618</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="60" customFormat="1" x14ac:dyDescent="0.25">
@@ -2957,7 +3183,7 @@
         <v>188</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D17" s="60" t="s">
         <v>8</v>
@@ -2966,10 +3192,10 @@
         <v>109</v>
       </c>
       <c r="F17" s="60" t="s">
-        <v>426</v>
+        <v>586</v>
       </c>
       <c r="G17" s="61" t="s">
-        <v>427</v>
+        <v>621</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -2980,7 +3206,7 @@
         <v>100</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D18" s="17" t="s">
         <v>8</v>
@@ -2989,10 +3215,10 @@
         <v>109</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>426</v>
+        <v>544</v>
       </c>
       <c r="G18" t="s">
-        <v>427</v>
+        <v>622</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -3003,7 +3229,7 @@
         <v>108</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>8</v>
@@ -3012,10 +3238,10 @@
         <v>109</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>426</v>
+        <v>586</v>
       </c>
       <c r="G19" t="s">
-        <v>427</v>
+        <v>623</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -3026,7 +3252,7 @@
         <v>362</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D20" s="17" t="s">
         <v>8</v>
@@ -3035,10 +3261,10 @@
         <v>61</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>426</v>
+        <v>586</v>
       </c>
       <c r="G20" t="s">
-        <v>427</v>
+        <v>624</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -3049,7 +3275,7 @@
         <v>346</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>8</v>
@@ -3058,13 +3284,13 @@
         <v>61</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>426</v>
+        <v>586</v>
       </c>
       <c r="G21" t="s">
-        <v>427</v>
+        <v>628</v>
       </c>
       <c r="H21" t="s">
-        <v>506</v>
+        <v>625</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -3075,7 +3301,7 @@
         <v>258</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D22" s="17" t="s">
         <v>8</v>
@@ -3084,13 +3310,13 @@
         <v>109</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>426</v>
+        <v>544</v>
       </c>
       <c r="G22" t="s">
-        <v>427</v>
+        <v>629</v>
       </c>
       <c r="H22" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -3101,7 +3327,7 @@
         <v>257</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>8</v>
@@ -3110,13 +3336,13 @@
         <v>109</v>
       </c>
       <c r="F23" s="17" t="s">
-        <v>426</v>
+        <v>544</v>
       </c>
       <c r="G23" t="s">
-        <v>427</v>
+        <v>630</v>
       </c>
       <c r="H23" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -3127,7 +3353,7 @@
         <v>247</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D24" s="17" t="s">
         <v>8</v>
@@ -3136,13 +3362,13 @@
         <v>109</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>426</v>
+        <v>544</v>
       </c>
       <c r="G24" t="s">
-        <v>427</v>
+        <v>631</v>
       </c>
       <c r="H24" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -3153,7 +3379,7 @@
         <v>259</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D25" s="17" t="s">
         <v>8</v>
@@ -3162,13 +3388,13 @@
         <v>109</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>426</v>
+        <v>544</v>
       </c>
       <c r="G25" t="s">
-        <v>427</v>
+        <v>632</v>
       </c>
       <c r="H25" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -3179,7 +3405,7 @@
         <v>260</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D26" s="17" t="s">
         <v>8</v>
@@ -3188,13 +3414,13 @@
         <v>109</v>
       </c>
       <c r="F26" s="17" t="s">
-        <v>426</v>
+        <v>544</v>
       </c>
       <c r="G26" t="s">
-        <v>427</v>
+        <v>633</v>
       </c>
       <c r="H26" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -3205,7 +3431,7 @@
         <v>261</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D27" s="17" t="s">
         <v>8</v>
@@ -3214,13 +3440,13 @@
         <v>109</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>426</v>
+        <v>544</v>
       </c>
       <c r="G27" t="s">
-        <v>427</v>
+        <v>634</v>
       </c>
       <c r="H27" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -3231,7 +3457,7 @@
         <v>265</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D28" s="17" t="s">
         <v>8</v>
@@ -3240,13 +3466,13 @@
         <v>109</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>426</v>
+        <v>544</v>
       </c>
       <c r="G28" t="s">
-        <v>427</v>
+        <v>635</v>
       </c>
       <c r="H28" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="60" customFormat="1" x14ac:dyDescent="0.25">
@@ -3295,7 +3521,7 @@
         <v>427</v>
       </c>
       <c r="H30" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.25">
@@ -3306,7 +3532,7 @@
         <v>50</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D31" s="64" t="s">
         <v>47</v>
@@ -3315,10 +3541,10 @@
         <v>61</v>
       </c>
       <c r="F31" s="64" t="s">
-        <v>426</v>
+        <v>586</v>
       </c>
       <c r="G31" s="64" t="s">
-        <v>427</v>
+        <v>636</v>
       </c>
       <c r="H31" s="64"/>
       <c r="I31" s="65"/>
@@ -3331,7 +3557,7 @@
         <v>126</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D32" s="64" t="s">
         <v>47</v>
@@ -3340,10 +3566,10 @@
         <v>109</v>
       </c>
       <c r="F32" s="67" t="s">
-        <v>426</v>
+        <v>586</v>
       </c>
       <c r="G32" s="64" t="s">
-        <v>427</v>
+        <v>637</v>
       </c>
       <c r="H32" s="64"/>
       <c r="I32" s="65"/>
@@ -3356,7 +3582,7 @@
         <v>131</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D33" s="64" t="s">
         <v>47</v>
@@ -3365,10 +3591,10 @@
         <v>109</v>
       </c>
       <c r="F33" s="64" t="s">
-        <v>426</v>
+        <v>586</v>
       </c>
       <c r="G33" s="64" t="s">
-        <v>427</v>
+        <v>638</v>
       </c>
       <c r="H33" s="64"/>
       <c r="I33" s="65"/>
@@ -3381,7 +3607,7 @@
         <v>138</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D34" s="64" t="s">
         <v>47</v>
@@ -3390,10 +3616,10 @@
         <v>109</v>
       </c>
       <c r="F34" s="67" t="s">
-        <v>426</v>
+        <v>586</v>
       </c>
       <c r="G34" s="64" t="s">
-        <v>427</v>
+        <v>639</v>
       </c>
       <c r="H34" s="64"/>
       <c r="I34" s="65"/>
@@ -3406,7 +3632,7 @@
         <v>143</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D35" s="64" t="s">
         <v>47</v>
@@ -3415,10 +3641,10 @@
         <v>109</v>
       </c>
       <c r="F35" s="67" t="s">
-        <v>426</v>
+        <v>586</v>
       </c>
       <c r="G35" s="64" t="s">
-        <v>427</v>
+        <v>640</v>
       </c>
       <c r="H35" s="64"/>
       <c r="I35" s="65"/>
@@ -3431,7 +3657,7 @@
         <v>148</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D36" s="64" t="s">
         <v>47</v>
@@ -3440,10 +3666,10 @@
         <v>109</v>
       </c>
       <c r="F36" s="64" t="s">
-        <v>426</v>
+        <v>586</v>
       </c>
       <c r="G36" s="64" t="s">
-        <v>427</v>
+        <v>641</v>
       </c>
       <c r="H36" s="64"/>
       <c r="I36" s="65"/>
@@ -3456,7 +3682,7 @@
         <v>152</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D37" s="64" t="s">
         <v>47</v>
@@ -3465,10 +3691,10 @@
         <v>61</v>
       </c>
       <c r="F37" s="64" t="s">
-        <v>426</v>
+        <v>586</v>
       </c>
       <c r="G37" s="64" t="s">
-        <v>427</v>
+        <v>642</v>
       </c>
       <c r="H37" s="64"/>
       <c r="I37" s="65"/>
@@ -3481,7 +3707,7 @@
         <v>157</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D38" s="64" t="s">
         <v>47</v>
@@ -3490,10 +3716,10 @@
         <v>61</v>
       </c>
       <c r="F38" s="64" t="s">
-        <v>426</v>
+        <v>586</v>
       </c>
       <c r="G38" s="64" t="s">
-        <v>427</v>
+        <v>643</v>
       </c>
       <c r="H38" s="64"/>
       <c r="I38" s="65"/>
@@ -3506,7 +3732,7 @@
         <v>160</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D39" s="64" t="s">
         <v>47</v>
@@ -3515,10 +3741,10 @@
         <v>109</v>
       </c>
       <c r="F39" s="64" t="s">
-        <v>426</v>
+        <v>586</v>
       </c>
       <c r="G39" s="64" t="s">
-        <v>427</v>
+        <v>644</v>
       </c>
       <c r="H39" s="64"/>
       <c r="I39" s="65"/>
@@ -3531,7 +3757,7 @@
         <v>163</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D40" s="64" t="s">
         <v>47</v>
@@ -3540,10 +3766,10 @@
         <v>109</v>
       </c>
       <c r="F40" s="64" t="s">
-        <v>426</v>
+        <v>586</v>
       </c>
       <c r="G40" s="64" t="s">
-        <v>427</v>
+        <v>645</v>
       </c>
       <c r="H40" s="64"/>
       <c r="I40" s="65"/>
@@ -3556,7 +3782,7 @@
         <v>168</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D41" s="64" t="s">
         <v>47</v>
@@ -3565,10 +3791,10 @@
         <v>109</v>
       </c>
       <c r="F41" s="64" t="s">
-        <v>426</v>
+        <v>586</v>
       </c>
       <c r="G41" s="64" t="s">
-        <v>427</v>
+        <v>646</v>
       </c>
       <c r="H41" s="64"/>
       <c r="I41" s="65"/>
@@ -3581,7 +3807,7 @@
         <v>175</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D42" s="64" t="s">
         <v>47</v>
@@ -3590,10 +3816,10 @@
         <v>109</v>
       </c>
       <c r="F42" s="64" t="s">
-        <v>426</v>
+        <v>586</v>
       </c>
       <c r="G42" s="64" t="s">
-        <v>427</v>
+        <v>647</v>
       </c>
       <c r="H42" s="64"/>
       <c r="I42" s="65"/>
@@ -3606,7 +3832,7 @@
         <v>182</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D43" s="64" t="s">
         <v>47</v>
@@ -3615,10 +3841,10 @@
         <v>61</v>
       </c>
       <c r="F43" s="64" t="s">
-        <v>426</v>
+        <v>586</v>
       </c>
       <c r="G43" s="64" t="s">
-        <v>427</v>
+        <v>648</v>
       </c>
       <c r="H43" s="64"/>
       <c r="I43" s="65"/>
@@ -3631,7 +3857,7 @@
         <v>375</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D44" s="64" t="s">
         <v>47</v>
@@ -3640,10 +3866,10 @@
         <v>61</v>
       </c>
       <c r="F44" s="64" t="s">
-        <v>426</v>
+        <v>586</v>
       </c>
       <c r="G44" s="64" t="s">
-        <v>427</v>
+        <v>649</v>
       </c>
       <c r="H44" s="64"/>
       <c r="I44" s="65"/>
@@ -3656,7 +3882,7 @@
         <v>267</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D45" s="64" t="s">
         <v>47</v>
@@ -3665,10 +3891,10 @@
         <v>61</v>
       </c>
       <c r="F45" s="64" t="s">
-        <v>426</v>
+        <v>586</v>
       </c>
       <c r="G45" s="64" t="s">
-        <v>427</v>
+        <v>650</v>
       </c>
       <c r="H45" s="64"/>
       <c r="I45" s="65"/>
@@ -3935,7 +4161,7 @@
         <v>427</v>
       </c>
       <c r="H55" t="s">
-        <v>559</v>
+        <v>549</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -4105,7 +4331,7 @@
         <v>427</v>
       </c>
       <c r="H62" t="s">
-        <v>560</v>
+        <v>550</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -4177,7 +4403,7 @@
         <v>427</v>
       </c>
       <c r="H65" t="s">
-        <v>561</v>
+        <v>551</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -4203,7 +4429,7 @@
         <v>427</v>
       </c>
       <c r="H66" t="s">
-        <v>562</v>
+        <v>552</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -4252,7 +4478,7 @@
         <v>427</v>
       </c>
       <c r="H68" t="s">
-        <v>563</v>
+        <v>553</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -4278,7 +4504,7 @@
         <v>427</v>
       </c>
       <c r="H69" t="s">
-        <v>564</v>
+        <v>554</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -4442,7 +4668,7 @@
         <v>427</v>
       </c>
       <c r="H76" t="s">
-        <v>565</v>
+        <v>555</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -4468,7 +4694,7 @@
         <v>427</v>
       </c>
       <c r="H77" t="s">
-        <v>566</v>
+        <v>556</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -4476,7 +4702,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="78" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="C78" s="7" t="s">
         <v>56</v>
@@ -4499,7 +4725,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="85" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="C79" s="7" t="s">
         <v>56</v>
@@ -4522,7 +4748,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="85" t="s">
-        <v>528</v>
+        <v>518</v>
       </c>
       <c r="C80" s="7" t="s">
         <v>56</v>
@@ -4540,7 +4766,7 @@
         <v>427</v>
       </c>
       <c r="H80" t="s">
-        <v>567</v>
+        <v>557</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4548,7 +4774,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="81" t="s">
-        <v>529</v>
+        <v>519</v>
       </c>
       <c r="C81" s="7" t="s">
         <v>56</v>
@@ -4571,7 +4797,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="78" t="s">
-        <v>532</v>
+        <v>522</v>
       </c>
       <c r="C82" s="7" t="s">
         <v>56</v>
@@ -4589,7 +4815,7 @@
         <v>427</v>
       </c>
       <c r="H82" t="s">
-        <v>568</v>
+        <v>558</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -4597,7 +4823,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="78" t="s">
-        <v>534</v>
+        <v>524</v>
       </c>
       <c r="C83" s="7" t="s">
         <v>56</v>
@@ -4620,7 +4846,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="78" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="C84" s="7" t="s">
         <v>56</v>
@@ -4638,7 +4864,7 @@
         <v>427</v>
       </c>
       <c r="H84" t="s">
-        <v>569</v>
+        <v>559</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -4646,7 +4872,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="78" t="s">
-        <v>540</v>
+        <v>530</v>
       </c>
       <c r="C85" s="7" t="s">
         <v>56</v>
@@ -4664,7 +4890,7 @@
         <v>427</v>
       </c>
       <c r="H85" t="s">
-        <v>570</v>
+        <v>560</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -4672,7 +4898,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="78" t="s">
-        <v>543</v>
+        <v>533</v>
       </c>
       <c r="C86" s="7" t="s">
         <v>56</v>
@@ -4695,7 +4921,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="78" t="s">
-        <v>544</v>
+        <v>534</v>
       </c>
       <c r="C87" s="7" t="s">
         <v>56</v>
@@ -4718,7 +4944,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="78" t="s">
-        <v>546</v>
+        <v>536</v>
       </c>
       <c r="C88" s="7" t="s">
         <v>56</v>
@@ -4741,7 +4967,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="84" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="C89" s="7" t="s">
         <v>56</v>
@@ -4759,7 +4985,7 @@
         <v>427</v>
       </c>
       <c r="H89" t="s">
-        <v>571</v>
+        <v>561</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -4767,7 +4993,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="78" t="s">
-        <v>549</v>
+        <v>539</v>
       </c>
       <c r="C90" s="7" t="s">
         <v>56</v>
@@ -4790,7 +5016,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="84" t="s">
-        <v>551</v>
+        <v>541</v>
       </c>
       <c r="C91" s="7" t="s">
         <v>56</v>
@@ -4808,7 +5034,7 @@
         <v>427</v>
       </c>
       <c r="H91" t="s">
-        <v>572</v>
+        <v>562</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -4816,7 +5042,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="84" t="s">
-        <v>553</v>
+        <v>543</v>
       </c>
       <c r="C92" s="7" t="s">
         <v>56</v>
@@ -4834,7 +5060,7 @@
         <v>427</v>
       </c>
       <c r="H92" t="s">
-        <v>573</v>
+        <v>563</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4842,7 +5068,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="81" t="s">
-        <v>555</v>
+        <v>545</v>
       </c>
       <c r="C93" s="7" t="s">
         <v>56</v>
@@ -4860,7 +5086,7 @@
         <v>427</v>
       </c>
       <c r="H93" t="s">
-        <v>574</v>
+        <v>564</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -4868,7 +5094,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="78" t="s">
-        <v>558</v>
+        <v>548</v>
       </c>
       <c r="C94" s="7" t="s">
         <v>56</v>
@@ -4891,7 +5117,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="86" t="s">
-        <v>555</v>
+        <v>545</v>
       </c>
       <c r="C95" s="7" t="s">
         <v>56</v>
@@ -4903,15 +5129,18 @@
         <v>109</v>
       </c>
       <c r="F95" s="17" t="s">
-        <v>554</v>
+        <v>544</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="7">
+        <v>95</v>
+      </c>
       <c r="B96" s="74" t="s">
-        <v>575</v>
+        <v>565</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D96" s="7" t="s">
         <v>47</v>
@@ -4920,10 +5149,263 @@
         <v>109</v>
       </c>
       <c r="F96" t="s">
+        <v>426</v>
+      </c>
+      <c r="G96" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" s="7">
+        <v>96</v>
+      </c>
+      <c r="B97" s="73" t="s">
+        <v>568</v>
+      </c>
+      <c r="C97" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D97" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E97" s="62" t="s">
+        <v>109</v>
+      </c>
+      <c r="F97" t="s">
+        <v>426</v>
+      </c>
+      <c r="G97" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="7">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>567</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D98" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E98" s="62" t="s">
+        <v>109</v>
+      </c>
+      <c r="F98" t="s">
+        <v>426</v>
+      </c>
+      <c r="G98" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="7">
+        <v>98</v>
+      </c>
+      <c r="B99" s="78" t="s">
+        <v>571</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D99" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E99" s="62" t="s">
+        <v>109</v>
+      </c>
+      <c r="F99" s="17" t="s">
+        <v>426</v>
+      </c>
+      <c r="G99" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A100" s="7">
+        <v>99</v>
+      </c>
+      <c r="B100" s="74" t="s">
+        <v>572</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D100" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E100" s="62" t="s">
+        <v>109</v>
+      </c>
+      <c r="F100" t="s">
+        <v>426</v>
+      </c>
+      <c r="G100" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A101" s="7">
+        <v>100</v>
+      </c>
+      <c r="B101" s="90" t="s">
+        <v>574</v>
+      </c>
+      <c r="C101" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D101" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E101" s="62" t="s">
+        <v>109</v>
+      </c>
+      <c r="F101" t="s">
+        <v>426</v>
+      </c>
+      <c r="G101" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A102" s="7">
+        <v>101</v>
+      </c>
+      <c r="B102" s="90" t="s">
         <v>578</v>
       </c>
-      <c r="G96" t="s">
+      <c r="C102" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D102" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E102" s="62" t="s">
+        <v>109</v>
+      </c>
+      <c r="F102" t="s">
+        <v>426</v>
+      </c>
+      <c r="G102" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="7">
+        <v>102</v>
+      </c>
+      <c r="B103" s="7" t="s">
         <v>579</v>
+      </c>
+      <c r="C103" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D103" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E103" s="62" t="s">
+        <v>109</v>
+      </c>
+      <c r="F103" t="s">
+        <v>426</v>
+      </c>
+      <c r="G103" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A104" s="7">
+        <v>103</v>
+      </c>
+      <c r="B104" s="91" t="s">
+        <v>580</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D104" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E104" s="62" t="s">
+        <v>109</v>
+      </c>
+      <c r="F104" t="s">
+        <v>426</v>
+      </c>
+      <c r="G104" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A105" s="7">
+        <v>104</v>
+      </c>
+      <c r="B105" s="92" t="s">
+        <v>585</v>
+      </c>
+      <c r="C105" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D105" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E105" s="62" t="s">
+        <v>109</v>
+      </c>
+      <c r="F105" t="s">
+        <v>426</v>
+      </c>
+      <c r="G105" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A106" s="7">
+        <v>105</v>
+      </c>
+      <c r="B106" s="92" t="s">
+        <v>587</v>
+      </c>
+      <c r="C106" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D106" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E106" s="62" t="s">
+        <v>109</v>
+      </c>
+      <c r="F106" t="s">
+        <v>426</v>
+      </c>
+      <c r="G106" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A107" s="7">
+        <v>106</v>
+      </c>
+      <c r="B107" s="92" t="s">
+        <v>588</v>
+      </c>
+      <c r="C107" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D107" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E107" s="62" t="s">
+        <v>109</v>
+      </c>
+      <c r="F107" t="s">
+        <v>426</v>
+      </c>
+      <c r="G107" t="s">
+        <v>427</v>
       </c>
     </row>
   </sheetData>
@@ -4939,10 +5421,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9856292-E718-4F44-A2EB-03A51CA4C0E1}">
-  <dimension ref="A1:EM71"/>
+  <dimension ref="A1:EM72"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="AH1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AN30" sqref="AN30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5045,7 +5527,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>539</v>
+        <v>529</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>1</v>
@@ -5363,7 +5845,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="2" spans="1:109" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:109" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22">
         <v>1</v>
       </c>
@@ -5546,7 +6028,7 @@
       <c r="DB2" s="22"/>
       <c r="DC2" s="22"/>
     </row>
-    <row r="3" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:109" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22">
         <v>2</v>
       </c>
@@ -5743,7 +6225,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="4" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:109" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22">
         <v>3</v>
       </c>
@@ -5904,7 +6386,7 @@
       <c r="DB4" s="27"/>
       <c r="DC4" s="27"/>
     </row>
-    <row r="5" spans="1:109" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:109" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="22">
         <v>4</v>
       </c>
@@ -6089,7 +6571,7 @@
       <c r="DB5" s="22"/>
       <c r="DC5" s="22"/>
     </row>
-    <row r="6" spans="1:109" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:109" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="22">
         <v>5</v>
       </c>
@@ -6274,7 +6756,7 @@
       <c r="DB6" s="22"/>
       <c r="DC6" s="22"/>
     </row>
-    <row r="7" spans="1:109" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:109" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22">
         <v>6</v>
       </c>
@@ -6453,7 +6935,7 @@
       <c r="DB7" s="22"/>
       <c r="DC7" s="22"/>
     </row>
-    <row r="8" spans="1:109" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:109" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29">
         <v>7</v>
       </c>
@@ -6634,7 +7116,7 @@
       <c r="DB8" s="29"/>
       <c r="DC8" s="29"/>
     </row>
-    <row r="9" spans="1:109" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:109" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29">
         <v>8</v>
       </c>
@@ -6813,7 +7295,7 @@
       <c r="DB9" s="29"/>
       <c r="DC9" s="29"/>
     </row>
-    <row r="10" spans="1:109" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:109" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22">
         <v>9</v>
       </c>
@@ -7002,7 +7484,7 @@
       <c r="DB10" s="22"/>
       <c r="DC10" s="22"/>
     </row>
-    <row r="11" spans="1:109" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:109" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22">
         <v>10</v>
       </c>
@@ -7191,7 +7673,7 @@
       <c r="DB11" s="22"/>
       <c r="DC11" s="22"/>
     </row>
-    <row r="12" spans="1:109" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:109" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22">
         <v>11</v>
       </c>
@@ -7374,7 +7856,7 @@
       <c r="DB12" s="22"/>
       <c r="DC12" s="22"/>
     </row>
-    <row r="13" spans="1:109" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:109" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22">
         <v>12</v>
       </c>
@@ -7561,7 +8043,7 @@
       <c r="DB13" s="22"/>
       <c r="DC13" s="22"/>
     </row>
-    <row r="14" spans="1:109" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:109" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22">
         <v>13</v>
       </c>
@@ -7744,7 +8226,7 @@
       <c r="DB14" s="22"/>
       <c r="DC14" s="22"/>
     </row>
-    <row r="15" spans="1:109" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:109" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22">
         <v>14</v>
       </c>
@@ -7927,7 +8409,7 @@
       <c r="DB15" s="22"/>
       <c r="DC15" s="22"/>
     </row>
-    <row r="16" spans="1:109" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:109" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22">
         <v>15</v>
       </c>
@@ -8116,7 +8598,7 @@
       <c r="DB16" s="22"/>
       <c r="DC16" s="22"/>
     </row>
-    <row r="17" spans="1:110" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:110" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22">
         <v>16</v>
       </c>
@@ -8299,7 +8781,7 @@
       <c r="DB17" s="22"/>
       <c r="DC17" s="22"/>
     </row>
-    <row r="18" spans="1:110" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:110" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="22">
         <v>17</v>
       </c>
@@ -8482,7 +8964,7 @@
       <c r="DB18" s="22"/>
       <c r="DC18" s="22"/>
     </row>
-    <row r="19" spans="1:110" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:110" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="22">
         <v>18</v>
       </c>
@@ -8659,7 +9141,7 @@
       <c r="DB19" s="27"/>
       <c r="DC19" s="27"/>
     </row>
-    <row r="20" spans="1:110" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:110" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="22">
         <v>19</v>
       </c>
@@ -8790,7 +9272,7 @@
       <c r="DB20" s="27"/>
       <c r="DC20" s="27"/>
     </row>
-    <row r="21" spans="1:110" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:110" s="13" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="29">
         <v>20</v>
       </c>
@@ -9177,10 +9659,10 @@
         <v>56</v>
       </c>
       <c r="CO22" s="14" t="s">
-        <v>508</v>
+        <v>627</v>
       </c>
       <c r="CP22" s="14" t="s">
-        <v>507</v>
+        <v>626</v>
       </c>
       <c r="CQ22" s="27" t="s">
         <v>56</v>
@@ -10144,7 +10626,7 @@
         <v>424</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="N30" s="22" t="s">
         <v>4</v>
@@ -10174,7 +10656,7 @@
         <v>23</v>
       </c>
       <c r="AB30" s="57" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="AC30" s="2" t="s">
         <v>84</v>
@@ -10229,7 +10711,7 @@
         <v>336</v>
       </c>
       <c r="DD30" s="57" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
     </row>
     <row r="31" spans="1:110" x14ac:dyDescent="0.25">
@@ -10976,7 +11458,7 @@
         <v>424</v>
       </c>
       <c r="F39" s="57" t="s">
-        <v>524</v>
+        <v>517</v>
       </c>
       <c r="G39" s="22"/>
       <c r="H39" s="22"/>
@@ -12819,7 +13301,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="C55" s="22" t="s">
         <v>27</v>
@@ -12829,7 +13311,7 @@
         <v>424</v>
       </c>
       <c r="F55" s="57" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
     </row>
     <row r="56" spans="1:143" x14ac:dyDescent="0.25">
@@ -12837,7 +13319,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="C56" s="22" t="s">
         <v>27</v>
@@ -12855,7 +13337,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>528</v>
+        <v>518</v>
       </c>
       <c r="C57" s="22" t="s">
         <v>27</v>
@@ -13014,7 +13496,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="73" t="s">
-        <v>529</v>
+        <v>519</v>
       </c>
       <c r="C58" s="22" t="s">
         <v>27</v>
@@ -13024,10 +13506,10 @@
         <v>424</v>
       </c>
       <c r="F58" s="57" t="s">
-        <v>530</v>
+        <v>520</v>
       </c>
       <c r="AE58" s="23" t="s">
-        <v>531</v>
+        <v>521</v>
       </c>
     </row>
     <row r="59" spans="1:143" x14ac:dyDescent="0.25">
@@ -13035,7 +13517,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>532</v>
+        <v>522</v>
       </c>
       <c r="C59" s="22" t="s">
         <v>27</v>
@@ -13049,7 +13531,7 @@
       <c r="H59" s="22"/>
       <c r="I59" s="22"/>
       <c r="J59" s="22" t="s">
-        <v>533</v>
+        <v>523</v>
       </c>
       <c r="K59" s="22"/>
       <c r="L59" s="22"/>
@@ -13229,7 +13711,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>534</v>
+        <v>524</v>
       </c>
       <c r="C60" s="22" t="s">
         <v>27</v>
@@ -13239,7 +13721,7 @@
         <v>424</v>
       </c>
       <c r="F60" s="57" t="s">
-        <v>535</v>
+        <v>525</v>
       </c>
     </row>
     <row r="61" spans="1:143" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -13247,7 +13729,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="C61" s="22" t="s">
         <v>27</v>
@@ -13259,13 +13741,13 @@
         <v>424</v>
       </c>
       <c r="F61" s="25" t="s">
-        <v>538</v>
+        <v>528</v>
       </c>
       <c r="G61" s="22"/>
       <c r="H61" s="22"/>
       <c r="I61" s="22"/>
       <c r="J61" s="22" t="s">
-        <v>537</v>
+        <v>527</v>
       </c>
       <c r="K61" s="22"/>
       <c r="L61" s="22"/>
@@ -13436,7 +13918,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>540</v>
+        <v>530</v>
       </c>
       <c r="C62" s="22" t="s">
         <v>83</v>
@@ -13445,10 +13927,10 @@
         <v>424</v>
       </c>
       <c r="F62" s="57" t="s">
-        <v>541</v>
+        <v>531</v>
       </c>
       <c r="J62" s="22" t="s">
-        <v>542</v>
+        <v>532</v>
       </c>
       <c r="K62" s="22"/>
       <c r="L62" s="22"/>
@@ -13649,7 +14131,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>543</v>
+        <v>533</v>
       </c>
       <c r="C63" s="22" t="s">
         <v>83</v>
@@ -13658,7 +14140,7 @@
         <v>424</v>
       </c>
       <c r="F63" s="57" t="s">
-        <v>541</v>
+        <v>531</v>
       </c>
       <c r="J63" s="22"/>
       <c r="K63" s="22"/>
@@ -13802,7 +14284,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>544</v>
+        <v>534</v>
       </c>
       <c r="C64" s="22" t="s">
         <v>83</v>
@@ -13811,7 +14293,7 @@
         <v>424</v>
       </c>
       <c r="F64" s="57" t="s">
-        <v>545</v>
+        <v>535</v>
       </c>
     </row>
     <row r="65" spans="1:123" x14ac:dyDescent="0.25">
@@ -13819,7 +14301,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>546</v>
+        <v>536</v>
       </c>
       <c r="C65" s="22" t="s">
         <v>83</v>
@@ -13828,7 +14310,7 @@
         <v>424</v>
       </c>
       <c r="F65" s="57" t="s">
-        <v>541</v>
+        <v>531</v>
       </c>
     </row>
     <row r="66" spans="1:123" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -13836,7 +14318,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="22" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="C66" s="22" t="s">
         <v>27</v>
@@ -13850,7 +14332,7 @@
       <c r="H66" s="22"/>
       <c r="I66" s="22"/>
       <c r="J66" s="22" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="K66" s="22"/>
       <c r="L66" s="22"/>
@@ -14019,7 +14501,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>549</v>
+        <v>539</v>
       </c>
       <c r="C67" s="22" t="s">
         <v>27</v>
@@ -14031,7 +14513,7 @@
         <v>424</v>
       </c>
       <c r="F67" s="57" t="s">
-        <v>550</v>
+        <v>540</v>
       </c>
     </row>
     <row r="68" spans="1:123" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -14039,7 +14521,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="22" t="s">
-        <v>551</v>
+        <v>541</v>
       </c>
       <c r="C68" s="22" t="s">
         <v>27</v>
@@ -14053,7 +14535,7 @@
       <c r="H68" s="22"/>
       <c r="I68" s="22"/>
       <c r="J68" s="22" t="s">
-        <v>552</v>
+        <v>542</v>
       </c>
       <c r="K68" s="22"/>
       <c r="L68" s="22"/>
@@ -14222,7 +14704,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="22" t="s">
-        <v>553</v>
+        <v>543</v>
       </c>
       <c r="C69" s="22" t="s">
         <v>83</v>
@@ -14236,7 +14718,7 @@
       <c r="H69" s="22"/>
       <c r="I69" s="22"/>
       <c r="J69" s="22" t="s">
-        <v>552</v>
+        <v>542</v>
       </c>
       <c r="K69" s="22"/>
       <c r="L69" s="22"/>
@@ -14405,7 +14887,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="73" t="s">
-        <v>555</v>
+        <v>545</v>
       </c>
       <c r="C70" s="22" t="s">
         <v>27</v>
@@ -14419,7 +14901,7 @@
       <c r="H70" s="22"/>
       <c r="I70" s="22"/>
       <c r="J70" s="22" t="s">
-        <v>556</v>
+        <v>546</v>
       </c>
       <c r="K70" s="22"/>
       <c r="L70" s="22"/>
@@ -14601,7 +15083,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>558</v>
+        <v>548</v>
       </c>
       <c r="C71" s="22" t="s">
         <v>27</v>
@@ -14610,8 +15092,26 @@
         <v>424</v>
       </c>
       <c r="F71" s="57" t="s">
-        <v>524</v>
-      </c>
+        <v>517</v>
+      </c>
+    </row>
+    <row r="72" spans="1:123" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>64</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>571</v>
+      </c>
+      <c r="C72" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="E72" s="22" t="s">
+        <v>424</v>
+      </c>
+      <c r="F72" s="57" t="s">
+        <v>531</v>
+      </c>
+      <c r="G72" s="57"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -14625,10 +15125,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D073B921-24DF-4F78-BD1E-1984D65F897D}">
-  <dimension ref="A1:BC18"/>
+  <dimension ref="A1:BJ28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14636,57 +15136,57 @@
     <col min="1" max="1" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="114.0" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="4" max="6" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="19.42578125" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="82.42578125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="24.5703125" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="34.85546875" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="31" max="33" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="34" max="34" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="35" max="36" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="4.140625" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" width="5.7109375" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="6.7109375" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="82.42578125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="34.85546875" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="33" max="35" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="37" max="38" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" width="4.140625" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" width="5.7109375" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" width="6.7109375" collapsed="true"/>
+    <col min="47" max="47" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="48" max="48" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="49" max="49" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
     <col min="50" max="50" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="51" max="51" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="51" max="51" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="52" max="52" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="53" max="53" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="54" max="54" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="55" max="55" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="56" max="56" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -14700,158 +15200,181 @@
         <v>414</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="BC1" s="1"/>
-    </row>
-    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BE1" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="BG1" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="BH1" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="BI1" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="BJ1" s="5" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="2" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
         <v>1</v>
       </c>
@@ -14862,50 +15385,50 @@
         <v>124</v>
       </c>
       <c r="D2" s="14"/>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="22" t="s">
         <v>424</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="H2" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14" t="s">
+      <c r="I2" s="14"/>
+      <c r="J2" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="K2" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14" t="s">
+      <c r="L2" s="14"/>
+      <c r="M2" s="14" t="s">
         <v>125</v>
-      </c>
-      <c r="L2" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" s="14" t="s">
-        <v>49</v>
       </c>
       <c r="N2" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
+      <c r="O2" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="P2" s="15" t="s">
+        <v>48</v>
+      </c>
       <c r="Q2" s="15"/>
-      <c r="R2" s="14" t="s">
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="S2" s="15" t="s">
+      <c r="U2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="T2" s="15"/>
-      <c r="U2" s="15"/>
       <c r="V2" s="15"/>
       <c r="W2" s="15"/>
       <c r="X2" s="15"/>
       <c r="Y2" s="15"/>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="14"/>
-      <c r="AB2" s="14"/>
+      <c r="AA2" s="15"/>
+      <c r="AB2" s="15"/>
       <c r="AC2" s="14"/>
       <c r="AD2" s="14"/>
       <c r="AE2" s="14"/>
@@ -14932,8 +15455,10 @@
       <c r="AZ2" s="14"/>
       <c r="BA2" s="14"/>
       <c r="BB2" s="14"/>
-    </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC2" s="14"/>
+      <c r="BD2" s="14"/>
+    </row>
+    <row r="3" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
         <v>2</v>
       </c>
@@ -14944,53 +15469,53 @@
         <v>124</v>
       </c>
       <c r="D3" s="14"/>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="22" t="s">
         <v>424</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="H3" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14" t="s">
+      <c r="I3" s="14"/>
+      <c r="J3" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="K3" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14" t="s">
+      <c r="L3" s="14"/>
+      <c r="M3" s="14" t="s">
         <v>127</v>
-      </c>
-      <c r="L3" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="M3" s="14" t="s">
-        <v>128</v>
       </c>
       <c r="N3" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
+      <c r="O3" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="P3" s="15" t="s">
+        <v>48</v>
+      </c>
       <c r="Q3" s="15"/>
-      <c r="R3" s="14" t="s">
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="S3" s="15" t="s">
+      <c r="U3" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="T3" s="15"/>
-      <c r="U3" s="15"/>
       <c r="V3" s="15"/>
       <c r="W3" s="15"/>
       <c r="X3" s="15"/>
       <c r="Y3" s="15"/>
       <c r="Z3" s="15"/>
-      <c r="AA3" s="15" t="s">
+      <c r="AA3" s="15"/>
+      <c r="AB3" s="15"/>
+      <c r="AC3" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="AB3" s="14"/>
-      <c r="AC3" s="14"/>
       <c r="AD3" s="14"/>
       <c r="AE3" s="14"/>
       <c r="AF3" s="14"/>
@@ -15016,8 +15541,10 @@
       <c r="AZ3" s="14"/>
       <c r="BA3" s="14"/>
       <c r="BB3" s="14"/>
-    </row>
-    <row r="4" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC3" s="14"/>
+      <c r="BD3" s="14"/>
+    </row>
+    <row r="4" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
         <v>3</v>
       </c>
@@ -15028,55 +15555,55 @@
         <v>124</v>
       </c>
       <c r="D4" s="14"/>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="22" t="s">
         <v>424</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="H4" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14" t="s">
+      <c r="I4" s="14"/>
+      <c r="J4" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="K4" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14" t="s">
+      <c r="L4" s="14"/>
+      <c r="M4" s="14" t="s">
         <v>132</v>
-      </c>
-      <c r="L4" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="M4" s="14" t="s">
-        <v>134</v>
       </c>
       <c r="N4" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
+      <c r="O4" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="P4" s="15" t="s">
+        <v>133</v>
+      </c>
       <c r="Q4" s="15"/>
-      <c r="R4" s="14" t="s">
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="S4" s="15" t="s">
+      <c r="U4" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="T4" s="15" t="s">
+      <c r="V4" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="U4" s="15"/>
-      <c r="V4" s="15"/>
       <c r="W4" s="15"/>
       <c r="X4" s="15"/>
       <c r="Y4" s="15"/>
-      <c r="Z4" s="15" t="s">
+      <c r="Z4" s="15"/>
+      <c r="AA4" s="15"/>
+      <c r="AB4" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="AA4" s="15"/>
-      <c r="AB4" s="14"/>
-      <c r="AC4" s="14"/>
+      <c r="AC4" s="15"/>
       <c r="AD4" s="14"/>
       <c r="AE4" s="14"/>
       <c r="AF4" s="14"/>
@@ -15102,8 +15629,10 @@
       <c r="AZ4" s="14"/>
       <c r="BA4" s="14"/>
       <c r="BB4" s="14"/>
-    </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC4" s="14"/>
+      <c r="BD4" s="14"/>
+    </row>
+    <row r="5" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
         <v>4</v>
       </c>
@@ -15114,50 +15643,50 @@
         <v>139</v>
       </c>
       <c r="D5" s="14"/>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="22" t="s">
         <v>424</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="H5" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14" t="s">
+      <c r="I5" s="14"/>
+      <c r="J5" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="K5" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14" t="s">
+      <c r="L5" s="14"/>
+      <c r="M5" s="14" t="s">
         <v>140</v>
-      </c>
-      <c r="L5" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="M5" s="14" t="s">
-        <v>141</v>
       </c>
       <c r="N5" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
+      <c r="O5" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="P5" s="15" t="s">
+        <v>133</v>
+      </c>
       <c r="Q5" s="15"/>
-      <c r="R5" s="14" t="s">
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="S5" s="15" t="s">
+      <c r="U5" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="T5" s="15"/>
-      <c r="U5" s="15"/>
       <c r="V5" s="15"/>
       <c r="W5" s="15"/>
       <c r="X5" s="15"/>
       <c r="Y5" s="15"/>
       <c r="Z5" s="15"/>
-      <c r="AA5" s="14"/>
-      <c r="AB5" s="14"/>
+      <c r="AA5" s="15"/>
+      <c r="AB5" s="15"/>
       <c r="AC5" s="14"/>
       <c r="AD5" s="14"/>
       <c r="AE5" s="14"/>
@@ -15184,8 +15713,10 @@
       <c r="AZ5" s="14"/>
       <c r="BA5" s="14"/>
       <c r="BB5" s="14"/>
-    </row>
-    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC5" s="14"/>
+      <c r="BD5" s="14"/>
+    </row>
+    <row r="6" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>5</v>
       </c>
@@ -15196,58 +15727,58 @@
         <v>139</v>
       </c>
       <c r="D6" s="14"/>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="22" t="s">
         <v>424</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="H6" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14" t="s">
+      <c r="I6" s="14"/>
+      <c r="J6" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="K6" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14" t="s">
+      <c r="L6" s="14"/>
+      <c r="M6" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="L6" s="15" t="s">
+      <c r="N6" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="M6" s="14" t="s">
+      <c r="O6" s="14" t="s">
         <v>128</v>
-      </c>
-      <c r="N6" s="41" t="s">
-        <v>187</v>
-      </c>
-      <c r="O6" s="15" t="s">
-        <v>145</v>
       </c>
       <c r="P6" s="41" t="s">
         <v>187</v>
       </c>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="14" t="s">
+      <c r="Q6" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="R6" s="41" t="s">
+        <v>187</v>
+      </c>
+      <c r="S6" s="15"/>
+      <c r="T6" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="S6" s="15" t="s">
+      <c r="U6" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="T6" s="15"/>
-      <c r="U6" s="15"/>
       <c r="V6" s="15"/>
       <c r="W6" s="15"/>
       <c r="X6" s="15"/>
       <c r="Y6" s="15"/>
       <c r="Z6" s="15"/>
-      <c r="AA6" s="14"/>
-      <c r="AB6" s="14" t="s">
+      <c r="AA6" s="15"/>
+      <c r="AB6" s="15"/>
+      <c r="AC6" s="14"/>
+      <c r="AD6" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="AC6" s="14"/>
-      <c r="AD6" s="14"/>
       <c r="AE6" s="14"/>
       <c r="AF6" s="14"/>
       <c r="AG6" s="14"/>
@@ -15272,8 +15803,10 @@
       <c r="AZ6" s="14"/>
       <c r="BA6" s="14"/>
       <c r="BB6" s="14"/>
-    </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC6" s="14"/>
+      <c r="BD6" s="14"/>
+    </row>
+    <row r="7" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
         <v>6</v>
       </c>
@@ -15284,58 +15817,58 @@
         <v>124</v>
       </c>
       <c r="D7" s="14"/>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="22" t="s">
         <v>424</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="H7" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14" t="s">
+      <c r="I7" s="14"/>
+      <c r="J7" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="K7" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14" t="s">
+      <c r="L7" s="14"/>
+      <c r="M7" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="L7" s="15" t="s">
+      <c r="N7" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="M7" s="14" t="s">
+      <c r="O7" s="14" t="s">
         <v>141</v>
-      </c>
-      <c r="N7" s="41" t="s">
-        <v>187</v>
-      </c>
-      <c r="O7" s="15" t="s">
-        <v>145</v>
       </c>
       <c r="P7" s="41" t="s">
         <v>187</v>
       </c>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="14" t="s">
+      <c r="Q7" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="R7" s="41" t="s">
+        <v>187</v>
+      </c>
+      <c r="S7" s="15"/>
+      <c r="T7" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="S7" s="15" t="s">
+      <c r="U7" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="T7" s="15"/>
-      <c r="U7" s="15"/>
       <c r="V7" s="15"/>
       <c r="W7" s="15"/>
       <c r="X7" s="15"/>
       <c r="Y7" s="15"/>
       <c r="Z7" s="15"/>
-      <c r="AA7" s="14"/>
-      <c r="AB7" s="14" t="s">
+      <c r="AA7" s="15"/>
+      <c r="AB7" s="15"/>
+      <c r="AC7" s="14"/>
+      <c r="AD7" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="AC7" s="14"/>
-      <c r="AD7" s="14"/>
       <c r="AE7" s="14"/>
       <c r="AF7" s="14"/>
       <c r="AG7" s="14"/>
@@ -15360,8 +15893,10 @@
       <c r="AZ7" s="14"/>
       <c r="BA7" s="14"/>
       <c r="BB7" s="14"/>
-    </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC7" s="14"/>
+      <c r="BD7" s="14"/>
+    </row>
+    <row r="8" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
         <v>7</v>
       </c>
@@ -15372,47 +15907,47 @@
         <v>124</v>
       </c>
       <c r="D8" s="14"/>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="22" t="s">
         <v>424</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="H8" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14" t="s">
+      <c r="I8" s="14"/>
+      <c r="J8" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="I8" s="14" t="s">
+      <c r="K8" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14" t="s">
+      <c r="L8" s="14"/>
+      <c r="M8" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="L8" s="15" t="s">
+      <c r="N8" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="M8" s="14"/>
-      <c r="N8" s="41" t="s">
+      <c r="O8" s="14"/>
+      <c r="P8" s="41" t="s">
         <v>187</v>
       </c>
-      <c r="O8" s="14"/>
-      <c r="P8" s="41"/>
       <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="15"/>
+      <c r="R8" s="41"/>
+      <c r="S8" s="14"/>
       <c r="T8" s="14"/>
-      <c r="U8" s="16" t="s">
+      <c r="U8" s="15"/>
+      <c r="V8" s="14"/>
+      <c r="W8" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="V8" s="16"/>
-      <c r="W8" s="16"/>
       <c r="X8" s="16"/>
-      <c r="Y8" s="14" t="s">
+      <c r="Y8" s="16"/>
+      <c r="Z8" s="16"/>
+      <c r="AA8" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="Z8" s="14"/>
-      <c r="AA8" s="14"/>
       <c r="AB8" s="14"/>
       <c r="AC8" s="14"/>
       <c r="AD8" s="14"/>
@@ -15440,8 +15975,10 @@
       <c r="AZ8" s="14"/>
       <c r="BA8" s="14"/>
       <c r="BB8" s="14"/>
-    </row>
-    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC8" s="14"/>
+      <c r="BD8" s="14"/>
+    </row>
+    <row r="9" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
         <v>8</v>
       </c>
@@ -15452,62 +15989,62 @@
         <v>124</v>
       </c>
       <c r="D9" s="14"/>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="22" t="s">
         <v>424</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="H9" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14" t="s">
+      <c r="I9" s="14"/>
+      <c r="J9" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="K9" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14" t="s">
+      <c r="L9" s="14"/>
+      <c r="M9" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="L9" s="42">
+      <c r="N9" s="42">
         <v>44201</v>
       </c>
-      <c r="M9" s="14" t="s">
+      <c r="O9" s="14" t="s">
         <v>134</v>
-      </c>
-      <c r="N9" s="41" t="s">
-        <v>162</v>
-      </c>
-      <c r="O9" s="15" t="s">
-        <v>145</v>
       </c>
       <c r="P9" s="41" t="s">
         <v>162</v>
       </c>
-      <c r="Q9" s="14" t="s">
+      <c r="Q9" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="R9" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="S9" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="R9" s="14" t="s">
+      <c r="T9" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="S9" s="15" t="s">
+      <c r="U9" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="T9" s="14"/>
-      <c r="U9" s="16"/>
-      <c r="V9" s="15" t="s">
+      <c r="V9" s="14"/>
+      <c r="W9" s="16"/>
+      <c r="X9" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="W9" s="15"/>
-      <c r="X9" s="15"/>
-      <c r="Y9" s="14"/>
-      <c r="Z9" s="14"/>
+      <c r="Y9" s="15"/>
+      <c r="Z9" s="15"/>
       <c r="AA9" s="14"/>
-      <c r="AB9" s="14" t="s">
+      <c r="AB9" s="14"/>
+      <c r="AC9" s="14"/>
+      <c r="AD9" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="AC9" s="14"/>
-      <c r="AD9" s="14"/>
       <c r="AE9" s="14"/>
       <c r="AF9" s="14"/>
       <c r="AG9" s="14"/>
@@ -15532,8 +16069,10 @@
       <c r="AZ9" s="14"/>
       <c r="BA9" s="14"/>
       <c r="BB9" s="14"/>
-    </row>
-    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC9" s="14"/>
+      <c r="BD9" s="14"/>
+    </row>
+    <row r="10" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
         <v>9</v>
       </c>
@@ -15544,51 +16083,51 @@
         <v>124</v>
       </c>
       <c r="D10" s="14"/>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="22" t="s">
         <v>424</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="H10" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14" t="s">
+      <c r="I10" s="14"/>
+      <c r="J10" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="I10" s="14" t="s">
+      <c r="K10" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14" t="s">
+      <c r="L10" s="14"/>
+      <c r="M10" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="L10" s="15" t="s">
+      <c r="N10" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="M10" s="14"/>
-      <c r="N10" s="41" t="s">
+      <c r="O10" s="14"/>
+      <c r="P10" s="41" t="s">
         <v>162</v>
       </c>
-      <c r="O10" s="16"/>
-      <c r="P10" s="41"/>
-      <c r="Q10" s="14" t="s">
+      <c r="Q10" s="16"/>
+      <c r="R10" s="41"/>
+      <c r="S10" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="R10" s="14"/>
-      <c r="S10" s="15"/>
       <c r="T10" s="14"/>
-      <c r="U10" s="16" t="s">
+      <c r="U10" s="15"/>
+      <c r="V10" s="14"/>
+      <c r="W10" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="V10" s="15" t="s">
+      <c r="X10" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="W10" s="16"/>
-      <c r="X10" s="16"/>
-      <c r="Y10" s="14" t="s">
+      <c r="Y10" s="16"/>
+      <c r="Z10" s="16"/>
+      <c r="AA10" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="Z10" s="14"/>
-      <c r="AA10" s="14"/>
       <c r="AB10" s="14"/>
       <c r="AC10" s="14"/>
       <c r="AD10" s="14"/>
@@ -15616,8 +16155,10 @@
       <c r="AZ10" s="14"/>
       <c r="BA10" s="14"/>
       <c r="BB10" s="14"/>
-    </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC10" s="14"/>
+      <c r="BD10" s="14"/>
+    </row>
+    <row r="11" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
         <v>10</v>
       </c>
@@ -15628,47 +16169,47 @@
         <v>124</v>
       </c>
       <c r="D11" s="14"/>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="22" t="s">
         <v>424</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="H11" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14" t="s">
+      <c r="I11" s="14"/>
+      <c r="J11" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="I11" s="14" t="s">
+      <c r="K11" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14" t="s">
+      <c r="L11" s="14"/>
+      <c r="M11" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="L11" s="42"/>
-      <c r="M11" s="14"/>
       <c r="N11" s="42"/>
-      <c r="O11" s="15"/>
+      <c r="O11" s="14"/>
       <c r="P11" s="42"/>
-      <c r="Q11" s="14" t="s">
+      <c r="Q11" s="15"/>
+      <c r="R11" s="42"/>
+      <c r="S11" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="R11" s="14"/>
-      <c r="S11" s="15"/>
       <c r="T11" s="14"/>
-      <c r="U11" s="16" t="s">
+      <c r="U11" s="15"/>
+      <c r="V11" s="14"/>
+      <c r="W11" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="V11" s="15" t="s">
+      <c r="X11" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="W11" s="15"/>
-      <c r="X11" s="15"/>
-      <c r="Y11" s="14" t="s">
+      <c r="Y11" s="15"/>
+      <c r="Z11" s="15"/>
+      <c r="AA11" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="Z11" s="14"/>
-      <c r="AA11" s="14"/>
       <c r="AB11" s="14"/>
       <c r="AC11" s="14"/>
       <c r="AD11" s="14"/>
@@ -15696,8 +16237,10 @@
       <c r="AZ11" s="14"/>
       <c r="BA11" s="14"/>
       <c r="BB11" s="14"/>
-    </row>
-    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC11" s="14"/>
+      <c r="BD11" s="14"/>
+    </row>
+    <row r="12" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
         <v>11</v>
       </c>
@@ -15708,53 +16251,53 @@
         <v>124</v>
       </c>
       <c r="D12" s="14"/>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="22" t="s">
         <v>424</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="H12" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14" t="s">
+      <c r="I12" s="14"/>
+      <c r="J12" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="I12" s="14" t="s">
+      <c r="K12" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="J12" s="14" t="s">
+      <c r="L12" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="K12" s="14" t="s">
+      <c r="M12" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
       <c r="N12" s="14"/>
       <c r="O12" s="14"/>
       <c r="P12" s="14"/>
       <c r="Q12" s="14"/>
-      <c r="R12" s="14" t="s">
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="S12" s="15" t="s">
+      <c r="U12" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="T12" s="14"/>
-      <c r="U12" s="16" t="s">
+      <c r="V12" s="14"/>
+      <c r="W12" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="V12" s="16" t="s">
+      <c r="X12" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="W12" s="16"/>
-      <c r="X12" s="16" t="s">
+      <c r="Y12" s="16"/>
+      <c r="Z12" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="Y12" s="14" t="s">
+      <c r="AA12" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="Z12" s="14"/>
-      <c r="AA12" s="14"/>
       <c r="AB12" s="14"/>
       <c r="AC12" s="14"/>
       <c r="AD12" s="14"/>
@@ -15782,8 +16325,10 @@
       <c r="AZ12" s="14"/>
       <c r="BA12" s="14"/>
       <c r="BB12" s="14"/>
-    </row>
-    <row r="13" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC12" s="14"/>
+      <c r="BD12" s="14"/>
+    </row>
+    <row r="13" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
         <v>12</v>
       </c>
@@ -15796,55 +16341,55 @@
       <c r="D13" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="22" t="s">
         <v>424</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="H13" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14" t="s">
+      <c r="I13" s="14"/>
+      <c r="J13" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="I13" s="14" t="s">
+      <c r="K13" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="J13" s="14" t="s">
+      <c r="L13" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="K13" s="14" t="s">
+      <c r="M13" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
       <c r="N13" s="14"/>
       <c r="O13" s="14"/>
       <c r="P13" s="14"/>
       <c r="Q13" s="14"/>
-      <c r="R13" s="14" t="s">
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="S13" s="15" t="s">
+      <c r="U13" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="T13" s="14"/>
-      <c r="U13" s="16" t="s">
+      <c r="V13" s="14"/>
+      <c r="W13" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="V13" s="16" t="s">
+      <c r="X13" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="W13" s="16" t="s">
+      <c r="Y13" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="X13" s="16" t="s">
+      <c r="Z13" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="Y13" s="14" t="s">
+      <c r="AA13" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="Z13" s="14"/>
-      <c r="AA13" s="14"/>
       <c r="AB13" s="14"/>
       <c r="AC13" s="14"/>
       <c r="AD13" s="14"/>
@@ -15872,8 +16417,10 @@
       <c r="AZ13" s="14"/>
       <c r="BA13" s="14"/>
       <c r="BB13" s="14"/>
-    </row>
-    <row r="14" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC13" s="14"/>
+      <c r="BD13" s="14"/>
+    </row>
+    <row r="14" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A14" s="14">
         <v>13</v>
       </c>
@@ -15884,53 +16431,53 @@
         <v>124</v>
       </c>
       <c r="D14" s="14"/>
-      <c r="E14" s="22" t="s">
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="22" t="s">
         <v>424</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="H14" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14" t="s">
+      <c r="I14" s="14"/>
+      <c r="J14" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="K14" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="J14" s="14" t="s">
+      <c r="L14" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="K14" s="14" t="s">
+      <c r="M14" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
       <c r="N14" s="14"/>
       <c r="O14" s="14"/>
       <c r="P14" s="14"/>
       <c r="Q14" s="14"/>
-      <c r="R14" s="14" t="s">
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="S14" s="15" t="s">
+      <c r="U14" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="T14" s="14"/>
-      <c r="U14" s="16" t="s">
+      <c r="V14" s="14"/>
+      <c r="W14" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="V14" s="16" t="s">
+      <c r="X14" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="W14" s="16"/>
-      <c r="X14" s="16" t="s">
+      <c r="Y14" s="16"/>
+      <c r="Z14" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="Y14" s="14" t="s">
+      <c r="AA14" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="Z14" s="14"/>
-      <c r="AA14" s="14"/>
       <c r="AB14" s="14"/>
       <c r="AC14" s="14"/>
       <c r="AD14" s="14"/>
@@ -15958,8 +16505,10 @@
       <c r="AZ14" s="14"/>
       <c r="BA14" s="14"/>
       <c r="BB14" s="14"/>
-    </row>
-    <row r="15" spans="1:55" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BC14" s="14"/>
+      <c r="BD14" s="14"/>
+    </row>
+    <row r="15" spans="1:62" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="35">
         <v>14</v>
       </c>
@@ -15970,136 +16519,138 @@
         <v>124</v>
       </c>
       <c r="D15" s="35"/>
-      <c r="E15" s="22" t="s">
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="22" t="s">
         <v>424</v>
       </c>
-      <c r="F15" s="35" t="s">
+      <c r="H15" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35" t="s">
+      <c r="I15" s="35"/>
+      <c r="J15" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="I15" s="35" t="s">
+      <c r="K15" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="J15" s="35" t="s">
+      <c r="L15" s="35" t="s">
         <v>169</v>
       </c>
-      <c r="K15" s="35" t="s">
+      <c r="M15" s="35" t="s">
         <v>268</v>
       </c>
-      <c r="L15" s="37" t="s">
+      <c r="N15" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="M15" s="35" t="s">
+      <c r="O15" s="35" t="s">
         <v>134</v>
-      </c>
-      <c r="N15" s="31" t="s">
-        <v>162</v>
-      </c>
-      <c r="O15" s="37" t="s">
-        <v>145</v>
       </c>
       <c r="P15" s="31" t="s">
         <v>162</v>
       </c>
-      <c r="Q15" s="35" t="s">
+      <c r="Q15" s="37" t="s">
+        <v>145</v>
+      </c>
+      <c r="R15" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="S15" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="R15" s="35" t="s">
+      <c r="T15" s="35" t="s">
         <v>183</v>
       </c>
-      <c r="S15" s="37" t="s">
+      <c r="U15" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="T15" s="37" t="s">
+      <c r="V15" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="U15" s="35"/>
-      <c r="V15" s="35"/>
-      <c r="W15" s="43" t="s">
+      <c r="W15" s="35"/>
+      <c r="X15" s="35"/>
+      <c r="Y15" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="X15" s="43" t="s">
+      <c r="Z15" s="43" t="s">
         <v>169</v>
       </c>
-      <c r="Y15" s="35"/>
-      <c r="Z15" s="35"/>
       <c r="AA15" s="35"/>
-      <c r="AB15" s="35" t="s">
+      <c r="AB15" s="35"/>
+      <c r="AC15" s="35"/>
+      <c r="AD15" s="35" t="s">
         <v>147</v>
       </c>
-      <c r="AC15" s="35" t="s">
+      <c r="AE15" s="35" t="s">
         <v>147</v>
       </c>
-      <c r="AD15" s="35"/>
-      <c r="AE15" s="35"/>
       <c r="AF15" s="35"/>
       <c r="AG15" s="35"/>
       <c r="AH15" s="35"/>
-      <c r="AI15" s="35" t="s">
+      <c r="AI15" s="35"/>
+      <c r="AJ15" s="35"/>
+      <c r="AK15" s="35" t="s">
         <v>278</v>
       </c>
-      <c r="AJ15" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="AK15" s="44" t="s">
+      <c r="AL15" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM15" s="44" t="s">
         <v>221</v>
       </c>
-      <c r="AL15" s="35" t="s">
+      <c r="AN15" s="35" t="s">
         <v>228</v>
       </c>
-      <c r="AM15" s="35" t="s">
+      <c r="AO15" s="35" t="s">
         <v>279</v>
       </c>
-      <c r="AN15" s="35" t="s">
+      <c r="AP15" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="AO15" s="35" t="s">
+      <c r="AQ15" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="AP15" s="35" t="s">
+      <c r="AR15" s="35" t="s">
         <v>238</v>
       </c>
-      <c r="AQ15" s="35" t="s">
+      <c r="AS15" s="35" t="s">
         <v>239</v>
       </c>
-      <c r="AR15" s="35" t="s">
+      <c r="AT15" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="AS15" s="43" t="s">
+      <c r="AU15" s="43" t="s">
         <v>244</v>
       </c>
-      <c r="AT15" s="43" t="s">
+      <c r="AV15" s="43" t="s">
         <v>243</v>
       </c>
-      <c r="AU15" s="45" t="s">
+      <c r="AW15" s="45" t="s">
         <v>241</v>
       </c>
-      <c r="AV15" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="AW15" s="35" t="s">
-        <v>56</v>
-      </c>
       <c r="AX15" s="35" t="s">
         <v>56</v>
       </c>
       <c r="AY15" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="AZ15" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="BA15" s="35" t="s">
         <v>280</v>
       </c>
-      <c r="AZ15" s="46" t="s">
+      <c r="BB15" s="46" t="s">
         <v>284</v>
       </c>
-      <c r="BA15" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="BB15" s="35" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC15" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="BD15" s="35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
         <v>15</v>
       </c>
@@ -16110,51 +16661,51 @@
         <v>124</v>
       </c>
       <c r="D16" s="14"/>
-      <c r="E16" s="22" t="s">
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="22" t="s">
         <v>424</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="H16" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="I16" s="14" t="s">
         <v>263</v>
       </c>
-      <c r="H16" s="14" t="s">
+      <c r="J16" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="I16" s="14" t="s">
+      <c r="K16" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="J16" s="14" t="s">
+      <c r="L16" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="K16" s="14" t="s">
+      <c r="M16" s="14" t="s">
         <v>372</v>
       </c>
-      <c r="L16" s="23" t="s">
-        <v>345</v>
-      </c>
-      <c r="M16" s="14" t="s">
+      <c r="N16" s="23" t="s">
+        <v>345</v>
+      </c>
+      <c r="O16" s="14" t="s">
         <v>134</v>
-      </c>
-      <c r="N16" s="23" t="s">
-        <v>385</v>
-      </c>
-      <c r="O16" s="16" t="s">
-        <v>377</v>
       </c>
       <c r="P16" s="23" t="s">
         <v>385</v>
       </c>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14" t="s">
+      <c r="Q16" s="16" t="s">
+        <v>377</v>
+      </c>
+      <c r="R16" s="23" t="s">
+        <v>385</v>
+      </c>
+      <c r="S16" s="14"/>
+      <c r="T16" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="S16" s="15" t="s">
+      <c r="U16" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="T16" s="14"/>
-      <c r="U16" s="14"/>
       <c r="V16" s="14"/>
       <c r="W16" s="14"/>
       <c r="X16" s="14"/>
@@ -16163,23 +16714,23 @@
       <c r="AA16" s="14"/>
       <c r="AB16" s="14"/>
       <c r="AC16" s="14"/>
-      <c r="AD16" s="23" t="s">
+      <c r="AD16" s="14"/>
+      <c r="AE16" s="14"/>
+      <c r="AF16" s="23" t="s">
         <v>384</v>
       </c>
-      <c r="AE16" s="48" t="s">
+      <c r="AG16" s="48" t="s">
         <v>334</v>
       </c>
-      <c r="AF16" s="48" t="s">
+      <c r="AH16" s="48" t="s">
         <v>336</v>
       </c>
-      <c r="AG16" s="23" t="s">
+      <c r="AI16" s="23" t="s">
         <v>405</v>
       </c>
-      <c r="AH16" s="48" t="s">
+      <c r="AJ16" s="48" t="s">
         <v>379</v>
       </c>
-      <c r="AI16" s="14"/>
-      <c r="AJ16" s="14"/>
       <c r="AK16" s="14"/>
       <c r="AL16" s="14"/>
       <c r="AM16" s="14"/>
@@ -16198,70 +16749,72 @@
       <c r="AZ16" s="14"/>
       <c r="BA16" s="14"/>
       <c r="BB16" s="14"/>
-    </row>
-    <row r="17" spans="1:54" ht="30" x14ac:dyDescent="0.25">
+      <c r="BC16" s="14"/>
+      <c r="BD16" s="14"/>
+    </row>
+    <row r="17" spans="1:62" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="77">
         <v>16</v>
       </c>
       <c r="B17" s="73" t="s">
-        <v>555</v>
+        <v>545</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>139</v>
       </c>
       <c r="D17" s="14"/>
-      <c r="E17" s="22" t="s">
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="22" t="s">
         <v>424</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="H17" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14" t="s">
+      <c r="I17" s="14"/>
+      <c r="J17" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="I17" s="14" t="s">
+      <c r="K17" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="J17" s="14"/>
-      <c r="K17" s="22" t="s">
-        <v>557</v>
-      </c>
-      <c r="L17" s="15" t="s">
+      <c r="L17" s="14"/>
+      <c r="M17" s="22" t="s">
+        <v>547</v>
+      </c>
+      <c r="N17" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="M17" s="14" t="s">
+      <c r="O17" s="14" t="s">
         <v>128</v>
-      </c>
-      <c r="N17" s="41" t="s">
-        <v>187</v>
-      </c>
-      <c r="O17" s="15" t="s">
-        <v>145</v>
       </c>
       <c r="P17" s="41" t="s">
         <v>187</v>
       </c>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="14" t="s">
+      <c r="Q17" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="R17" s="41" t="s">
+        <v>187</v>
+      </c>
+      <c r="S17" s="15"/>
+      <c r="T17" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="S17" s="15" t="s">
+      <c r="U17" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="T17" s="15"/>
-      <c r="U17" s="15"/>
       <c r="V17" s="15"/>
       <c r="W17" s="15"/>
       <c r="X17" s="15"/>
       <c r="Y17" s="15"/>
       <c r="Z17" s="15"/>
-      <c r="AA17" s="14"/>
-      <c r="AB17" s="14" t="s">
+      <c r="AA17" s="15"/>
+      <c r="AB17" s="15"/>
+      <c r="AC17" s="14"/>
+      <c r="AD17" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="AC17" s="14"/>
-      <c r="AD17" s="14"/>
       <c r="AE17" s="14"/>
       <c r="AF17" s="14"/>
       <c r="AG17" s="14"/>
@@ -16286,65 +16839,67 @@
       <c r="AZ17" s="14"/>
       <c r="BA17" s="14"/>
       <c r="BB17" s="14"/>
-    </row>
-    <row r="18" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="BC17" s="14"/>
+      <c r="BD17" s="14"/>
+    </row>
+    <row r="18" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A18" s="14">
         <v>17</v>
       </c>
       <c r="B18" s="74" t="s">
-        <v>575</v>
+        <v>565</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>124</v>
       </c>
       <c r="D18" s="14"/>
-      <c r="E18" s="22" t="s">
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="22" t="s">
         <v>424</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="H18" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14" t="s">
+      <c r="I18" s="14"/>
+      <c r="J18" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="I18" s="14" t="s">
+      <c r="K18" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="J18" s="14" t="s">
+      <c r="L18" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="K18" s="14" t="s">
+      <c r="M18" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
       <c r="N18" s="14"/>
       <c r="O18" s="14"/>
       <c r="P18" s="14"/>
       <c r="Q18" s="14"/>
-      <c r="R18" s="14" t="s">
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="S18" s="15" t="s">
+      <c r="U18" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="T18" s="14"/>
-      <c r="U18" s="16" t="s">
-        <v>576</v>
-      </c>
-      <c r="V18" s="16" t="s">
+      <c r="V18" s="14"/>
+      <c r="W18" s="16" t="s">
+        <v>566</v>
+      </c>
+      <c r="X18" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="W18" s="16"/>
-      <c r="X18" s="16" t="s">
+      <c r="Y18" s="16"/>
+      <c r="Z18" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="Y18" s="14" t="s">
+      <c r="AA18" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="Z18" s="14"/>
-      <c r="AA18" s="14"/>
       <c r="AB18" s="14"/>
       <c r="AC18" s="14"/>
       <c r="AD18" s="14"/>
@@ -16372,14 +16927,474 @@
       <c r="AZ18" s="14"/>
       <c r="BA18" s="14"/>
       <c r="BB18" s="14"/>
+      <c r="BC18" s="14"/>
+      <c r="BD18" s="14"/>
+    </row>
+    <row r="19" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A19" s="77">
+        <v>18</v>
+      </c>
+      <c r="B19" s="73" t="s">
+        <v>568</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="22" t="s">
+        <v>424</v>
+      </c>
+      <c r="W19" s="88" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="20" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A20" s="77">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>567</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="22" t="s">
+        <v>424</v>
+      </c>
+      <c r="W20" s="88" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="21" spans="1:62" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="77">
+        <v>20</v>
+      </c>
+      <c r="B21" s="74" t="s">
+        <v>572</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="22" t="s">
+        <v>424</v>
+      </c>
+      <c r="W21" s="89" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="22" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A22" s="77">
+        <v>21</v>
+      </c>
+      <c r="B22" s="90" t="s">
+        <v>574</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="22" t="s">
+        <v>424</v>
+      </c>
+      <c r="W22" s="89" t="s">
+        <v>573</v>
+      </c>
+      <c r="BE22" t="s">
+        <v>576</v>
+      </c>
+      <c r="BF22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:62" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="14">
+        <v>22</v>
+      </c>
+      <c r="B23" s="90" t="s">
+        <v>578</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="22" t="s">
+        <v>424</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I23" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="J23" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="K23" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="L23" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="M23" s="14" t="s">
+        <v>582</v>
+      </c>
+      <c r="N23" s="23" t="s">
+        <v>345</v>
+      </c>
+      <c r="O23" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="P23" s="23" t="s">
+        <v>385</v>
+      </c>
+      <c r="Q23" s="16" t="s">
+        <v>377</v>
+      </c>
+      <c r="R23" s="23" t="s">
+        <v>385</v>
+      </c>
+      <c r="S23" s="14"/>
+      <c r="T23" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="U23" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="V23" s="14"/>
+      <c r="W23" s="14"/>
+      <c r="X23" s="14"/>
+      <c r="Y23" s="14"/>
+      <c r="Z23" s="14"/>
+      <c r="AA23" s="14"/>
+      <c r="AB23" s="14"/>
+      <c r="AC23" s="14"/>
+      <c r="AD23" s="14"/>
+      <c r="AE23" s="14"/>
+      <c r="AF23" s="23" t="s">
+        <v>384</v>
+      </c>
+      <c r="AG23" s="48" t="s">
+        <v>334</v>
+      </c>
+      <c r="AH23" s="48" t="s">
+        <v>336</v>
+      </c>
+      <c r="AI23" s="23" t="s">
+        <v>405</v>
+      </c>
+      <c r="AJ23" s="48" t="s">
+        <v>379</v>
+      </c>
+      <c r="AK23" s="14"/>
+      <c r="AL23" s="14"/>
+      <c r="AM23" s="14"/>
+      <c r="AN23" s="14"/>
+      <c r="AO23" s="14"/>
+      <c r="AP23" s="14"/>
+      <c r="AQ23" s="14"/>
+      <c r="AR23" s="14"/>
+      <c r="AS23" s="14"/>
+      <c r="AT23" s="14"/>
+      <c r="AU23" s="14"/>
+      <c r="AV23" s="14"/>
+      <c r="AW23" s="14"/>
+      <c r="AX23" s="14"/>
+      <c r="AY23" s="14"/>
+      <c r="AZ23" s="14"/>
+      <c r="BA23" s="14"/>
+      <c r="BB23" s="14"/>
+      <c r="BC23" s="14"/>
+      <c r="BD23" s="14"/>
+    </row>
+    <row r="24" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A24" s="14">
+        <v>23</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>579</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="22" t="s">
+        <v>424</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="J24" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="K24" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="L24" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="M24" s="14" t="s">
+        <v>581</v>
+      </c>
+      <c r="N24" s="23" t="s">
+        <v>345</v>
+      </c>
+      <c r="O24" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="P24" s="23" t="s">
+        <v>385</v>
+      </c>
+      <c r="Q24" s="16" t="s">
+        <v>377</v>
+      </c>
+      <c r="R24" s="23" t="s">
+        <v>385</v>
+      </c>
+      <c r="S24" s="14"/>
+      <c r="T24" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="U24" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="V24" s="14"/>
+      <c r="W24" s="14"/>
+      <c r="X24" s="14"/>
+      <c r="Y24" s="14"/>
+      <c r="Z24" s="14"/>
+      <c r="AA24" s="14"/>
+      <c r="AB24" s="14"/>
+      <c r="AC24" s="14"/>
+      <c r="AD24" s="14"/>
+      <c r="AE24" s="14"/>
+      <c r="AF24" s="23" t="s">
+        <v>384</v>
+      </c>
+      <c r="AG24" s="48" t="s">
+        <v>334</v>
+      </c>
+      <c r="AH24" s="48" t="s">
+        <v>336</v>
+      </c>
+      <c r="AI24" s="23" t="s">
+        <v>405</v>
+      </c>
+      <c r="AJ24" s="48" t="s">
+        <v>379</v>
+      </c>
+      <c r="AK24" s="14"/>
+      <c r="AL24" s="14"/>
+      <c r="AM24" s="14"/>
+      <c r="AN24" s="14"/>
+      <c r="AO24" s="14"/>
+      <c r="AP24" s="14"/>
+      <c r="AQ24" s="14"/>
+      <c r="AR24" s="14"/>
+      <c r="AS24" s="14"/>
+      <c r="AT24" s="14"/>
+      <c r="AU24" s="14"/>
+      <c r="AV24" s="14"/>
+      <c r="AW24" s="14"/>
+      <c r="AX24" s="14"/>
+      <c r="AY24" s="14"/>
+      <c r="AZ24" s="14"/>
+      <c r="BA24" s="14"/>
+      <c r="BB24" s="14"/>
+      <c r="BC24" s="14"/>
+      <c r="BD24" s="14"/>
+    </row>
+    <row r="25" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A25" s="14">
+        <v>24</v>
+      </c>
+      <c r="B25" s="91" t="s">
+        <v>580</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="22" t="s">
+        <v>424</v>
+      </c>
+      <c r="H25" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="K25" s="14"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="14" t="s">
+        <v>584</v>
+      </c>
+      <c r="N25" s="23" t="s">
+        <v>345</v>
+      </c>
+      <c r="O25" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="P25" s="23" t="s">
+        <v>385</v>
+      </c>
+      <c r="Q25" s="16" t="s">
+        <v>583</v>
+      </c>
+      <c r="R25" s="23" t="s">
+        <v>385</v>
+      </c>
+      <c r="S25" s="14"/>
+      <c r="T25" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="U25" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="V25" s="14"/>
+      <c r="W25" s="14"/>
+      <c r="X25" s="14"/>
+      <c r="Y25" s="14"/>
+      <c r="Z25" s="14"/>
+      <c r="AA25" s="14"/>
+      <c r="AB25" s="14"/>
+      <c r="AC25" s="14"/>
+      <c r="AD25" s="14"/>
+      <c r="AE25" s="14"/>
+      <c r="AF25" s="23" t="s">
+        <v>384</v>
+      </c>
+      <c r="AG25" s="48" t="s">
+        <v>334</v>
+      </c>
+      <c r="AH25" s="48" t="s">
+        <v>336</v>
+      </c>
+      <c r="AI25" s="23" t="s">
+        <v>405</v>
+      </c>
+      <c r="AJ25" s="48" t="s">
+        <v>379</v>
+      </c>
+      <c r="AK25" s="14"/>
+      <c r="AL25" s="14"/>
+      <c r="AM25" s="14"/>
+      <c r="AN25" s="14"/>
+      <c r="AO25" s="14"/>
+      <c r="AP25" s="14"/>
+      <c r="AQ25" s="14"/>
+      <c r="AR25" s="14"/>
+      <c r="AS25" s="14"/>
+      <c r="AT25" s="14"/>
+      <c r="AU25" s="14"/>
+      <c r="AV25" s="14"/>
+      <c r="AW25" s="14"/>
+      <c r="AX25" s="14"/>
+      <c r="AY25" s="14"/>
+      <c r="AZ25" s="14"/>
+      <c r="BA25" s="14"/>
+      <c r="BB25" s="14"/>
+      <c r="BC25" s="14"/>
+      <c r="BD25" s="14"/>
+    </row>
+    <row r="26" spans="1:62" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="77">
+        <v>25</v>
+      </c>
+      <c r="B26" s="92" t="s">
+        <v>585</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="22" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="27" spans="1:62" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="77">
+        <v>26</v>
+      </c>
+      <c r="B27" s="92" t="s">
+        <v>587</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="22" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="28" spans="1:62" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="77">
+        <v>27</v>
+      </c>
+      <c r="B28" s="92" t="s">
+        <v>588</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G28" s="22" t="s">
+        <v>424</v>
+      </c>
+      <c r="BG28" s="88" t="s">
+        <v>589</v>
+      </c>
+      <c r="BH28" s="88" t="s">
+        <v>590</v>
+      </c>
+      <c r="BI28" s="88" t="s">
+        <v>591</v>
+      </c>
+      <c r="BJ28" t="s">
+        <v>351</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AU15" r:id="rId1" xr:uid="{8A19EDCF-BD59-40A9-B1BB-CA280508B1BC}"/>
-    <hyperlink ref="K16" r:id="rId2" display="http://10.32.6.121:8080/tfs/MSDynamics/MSDynamicsCRM/_workitems/edit/5906" xr:uid="{887959FD-2E54-4DD2-BB21-81D978BEC156}"/>
+    <hyperlink ref="AW15" r:id="rId1" xr:uid="{8A19EDCF-BD59-40A9-B1BB-CA280508B1BC}"/>
+    <hyperlink ref="M16" r:id="rId2" display="http://10.32.6.121:8080/tfs/MSDynamics/MSDynamicsCRM/_workitems/edit/5906" xr:uid="{887959FD-2E54-4DD2-BB21-81D978BEC156}"/>
+    <hyperlink ref="M23" r:id="rId3" display="http://10.32.6.121:8080/tfs/MSDynamics/MSDynamicsCRM/_workitems/edit/5906" xr:uid="{E3FE4A80-D9D3-4FB5-9132-9AE3BFF8AC5D}"/>
+    <hyperlink ref="M24" r:id="rId4" display="http://10.32.6.121:8080/tfs/MSDynamics/MSDynamicsCRM/_workitems/edit/5906" xr:uid="{E1024793-1A08-448B-BAB6-ED90CB1C51E7}"/>
+    <hyperlink ref="M25" r:id="rId5" display="http://10.32.6.121:8080/tfs/MSDynamics/MSDynamicsCRM/_workitems/edit/5906" xr:uid="{7B93BD04-A8BD-4A83-931A-B737C30F0AD7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -16387,8 +17402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A51C67A-098B-49A1-9024-B5BC951889FA}">
   <dimension ref="A1:AF11"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17004,6 +18019,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -17012,7 +18036,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006150CD2B74865543AE839454BD4B5DC6" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a2ee5e546ec1836f671c2a05bfe6bfc8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0be14d6d-d8a1-45f7-9f98-2db40f8691c4" xmlns:ns3="567c5c99-f8da-409a-bc28-51b94ad9a241" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e7ff770c31624934d8e1a633c6fbe95" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -17246,16 +18270,17 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB0B3A61-2E64-4CE7-BDD4-6ECB945D22FD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E980A1B9-8C22-45F7-8344-5E520FA354EB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -17263,7 +18288,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64F77A26-17A6-43DF-A115-F9EC24E62EB0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17281,14 +18306,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB0B3A61-2E64-4CE7-BDD4-6ECB945D22FD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Password update and S49 Smoke RUn
</commit_message>
<xml_diff>
--- a/data/CRM_Testdata.xlsx
+++ b/data/CRM_Testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\fahmed2\git\Dynamics-CRM-Stage\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8658E2C-470F-47E4-9CFD-055D8AADCC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583B04C9-39BC-452F-BE89-4CBEF257C181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="599" xr2:uid="{442E3441-3F3C-4A77-BB17-E93CAE512719}"/>
   </bookViews>
@@ -2216,9 +2216,6 @@
     <t>Create Member without error</t>
   </si>
   <si>
-    <t>Premier@2023</t>
-  </si>
-  <si>
     <t>2000568635</t>
   </si>
   <si>
@@ -2388,6 +2385,9 @@
   </si>
   <si>
     <t>2023_04_05_10_09_33</t>
+  </si>
+  <si>
+    <t>Premier@2023a</t>
   </si>
 </sst>
 </file>
@@ -3274,7 +3274,7 @@
   <dimension ref="A1:J126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3337,13 +3337,13 @@
         <v>61</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="I2" s="43" t="s">
         <v>407</v>
@@ -3375,7 +3375,7 @@
         <v>416</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="J3" s="73"/>
     </row>
@@ -3402,7 +3402,7 @@
         <v>416</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="J4" s="72" t="s">
         <v>414</v>
@@ -3431,7 +3431,7 @@
         <v>416</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="J5" s="73"/>
     </row>
@@ -3506,7 +3506,7 @@
         <v>416</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="J8" s="73"/>
     </row>
@@ -3557,7 +3557,7 @@
         <v>416</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="J10" s="73"/>
     </row>
@@ -3584,7 +3584,7 @@
         <v>416</v>
       </c>
       <c r="H11" s="34" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="J11" s="73"/>
     </row>
@@ -3611,7 +3611,7 @@
         <v>416</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="J12" s="73"/>
     </row>
@@ -3686,7 +3686,7 @@
         <v>416</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="J15" s="73"/>
     </row>
@@ -3713,7 +3713,7 @@
         <v>416</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="J16" s="73"/>
     </row>
@@ -3836,7 +3836,7 @@
         <v>416</v>
       </c>
       <c r="H21" s="77" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J21" s="75"/>
     </row>
@@ -3863,7 +3863,7 @@
         <v>416</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="J22" s="73"/>
     </row>
@@ -3890,7 +3890,7 @@
         <v>416</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="J23" s="73"/>
     </row>
@@ -3917,7 +3917,7 @@
         <v>416</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="J24" s="73"/>
     </row>
@@ -3944,7 +3944,7 @@
         <v>416</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="J25" s="73"/>
     </row>
@@ -3971,7 +3971,7 @@
         <v>416</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="J26" s="73"/>
     </row>
@@ -3998,7 +3998,7 @@
         <v>416</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="J27" s="73"/>
     </row>
@@ -4474,7 +4474,7 @@
         <v>416</v>
       </c>
       <c r="H46" s="62" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="I46" s="62"/>
     </row>
@@ -4501,7 +4501,7 @@
         <v>416</v>
       </c>
       <c r="H47" s="62" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="I47" s="62"/>
     </row>
@@ -4528,7 +4528,7 @@
         <v>416</v>
       </c>
       <c r="H48" s="62" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I48" s="62"/>
     </row>
@@ -4555,7 +4555,7 @@
         <v>416</v>
       </c>
       <c r="H49" s="62" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="I49" s="62"/>
     </row>
@@ -4582,7 +4582,7 @@
         <v>416</v>
       </c>
       <c r="H50" s="62" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="I50" s="62"/>
     </row>
@@ -4659,7 +4659,7 @@
         <v>416</v>
       </c>
       <c r="H53" s="62" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="I53" s="62"/>
     </row>
@@ -4686,7 +4686,7 @@
         <v>416</v>
       </c>
       <c r="H54" s="61" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="I54" s="61"/>
     </row>
@@ -4713,7 +4713,7 @@
         <v>416</v>
       </c>
       <c r="H55" s="13" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I55" s="34"/>
     </row>
@@ -4790,7 +4790,7 @@
         <v>416</v>
       </c>
       <c r="H58" s="13" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="I58" s="34"/>
     </row>
@@ -4892,7 +4892,7 @@
         <v>416</v>
       </c>
       <c r="H62" s="13" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="I62" s="34"/>
     </row>
@@ -4969,7 +4969,7 @@
         <v>416</v>
       </c>
       <c r="H65" s="13" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="I65" s="34"/>
     </row>
@@ -4996,7 +4996,7 @@
         <v>416</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="I66" s="34"/>
     </row>
@@ -5048,7 +5048,7 @@
         <v>416</v>
       </c>
       <c r="H68" s="13" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="I68" s="34"/>
     </row>
@@ -5075,7 +5075,7 @@
         <v>416</v>
       </c>
       <c r="H69" s="13" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="I69" s="34"/>
     </row>
@@ -5252,7 +5252,7 @@
         <v>416</v>
       </c>
       <c r="H76" s="13" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="I76" s="34"/>
     </row>
@@ -5279,7 +5279,7 @@
         <v>416</v>
       </c>
       <c r="H77" s="13" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="I77" s="34"/>
     </row>
@@ -5406,7 +5406,7 @@
         <v>416</v>
       </c>
       <c r="H82" s="13" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="I82" s="34"/>
     </row>
@@ -5458,7 +5458,7 @@
         <v>416</v>
       </c>
       <c r="H84" s="13" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="I84" s="34"/>
     </row>
@@ -5485,7 +5485,7 @@
         <v>416</v>
       </c>
       <c r="H85" s="13" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I85" s="34"/>
     </row>
@@ -5587,7 +5587,7 @@
         <v>416</v>
       </c>
       <c r="H89" s="13" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="I89" s="34"/>
     </row>
@@ -5639,7 +5639,7 @@
         <v>416</v>
       </c>
       <c r="H91" s="13" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="I91" s="34"/>
     </row>
@@ -5666,7 +5666,7 @@
         <v>416</v>
       </c>
       <c r="H92" s="13" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="I92" s="34"/>
     </row>
@@ -5693,7 +5693,7 @@
         <v>416</v>
       </c>
       <c r="H93" s="13" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="I93" s="34"/>
     </row>
@@ -6068,7 +6068,7 @@
         <v>416</v>
       </c>
       <c r="H108" s="13" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="J108" s="73"/>
     </row>
@@ -6120,7 +6120,7 @@
         <v>416</v>
       </c>
       <c r="H110" s="13" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="J110" s="73"/>
     </row>
@@ -6147,7 +6147,7 @@
         <v>416</v>
       </c>
       <c r="H111" s="13" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="J111" s="73"/>
     </row>
@@ -6518,8 +6518,8 @@
   <dimension ref="A1:EP90"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6966,7 +6966,7 @@
       </c>
       <c r="D2" s="21"/>
       <c r="E2" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F2" s="21"/>
       <c r="G2" s="21"/>
@@ -7155,7 +7155,7 @@
       </c>
       <c r="D3" s="21"/>
       <c r="E3" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F3" s="26"/>
       <c r="G3" s="26"/>
@@ -7358,7 +7358,7 @@
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F4" s="29" t="s">
         <v>408</v>
@@ -7525,7 +7525,7 @@
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
@@ -7716,7 +7716,7 @@
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="21"/>
@@ -7907,7 +7907,7 @@
       </c>
       <c r="D7" s="21"/>
       <c r="E7" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
@@ -8092,7 +8092,7 @@
       </c>
       <c r="D8" s="28"/>
       <c r="E8" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F8" s="28"/>
       <c r="G8" s="28"/>
@@ -8279,7 +8279,7 @@
       </c>
       <c r="D9" s="28"/>
       <c r="E9" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
@@ -8464,7 +8464,7 @@
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
@@ -8659,7 +8659,7 @@
       </c>
       <c r="D11" s="21"/>
       <c r="E11" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
@@ -8854,7 +8854,7 @@
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
@@ -9043,7 +9043,7 @@
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="21"/>
@@ -9236,7 +9236,7 @@
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
@@ -9425,7 +9425,7 @@
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="21"/>
@@ -9614,7 +9614,7 @@
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="21"/>
@@ -9809,7 +9809,7 @@
       </c>
       <c r="D17" s="21"/>
       <c r="E17" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="21"/>
@@ -9998,7 +9998,7 @@
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="21"/>
@@ -10187,7 +10187,7 @@
       </c>
       <c r="D19" s="21"/>
       <c r="E19" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F19" s="21"/>
       <c r="G19" s="21"/>
@@ -10370,7 +10370,7 @@
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F20" s="21"/>
       <c r="G20" s="21"/>
@@ -10507,7 +10507,7 @@
       </c>
       <c r="D21" s="34"/>
       <c r="E21" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F21" s="35" t="s">
         <v>409</v>
@@ -10658,7 +10658,7 @@
       </c>
       <c r="D22" s="13"/>
       <c r="E22" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F22" s="26"/>
       <c r="G22" s="26"/>
@@ -10893,10 +10893,10 @@
         <v>56</v>
       </c>
       <c r="CR22" s="13" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="CS22" s="13" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="CT22" s="26" t="s">
         <v>56</v>
@@ -11739,7 +11739,7 @@
       </c>
       <c r="D29" s="13"/>
       <c r="E29" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F29" s="26"/>
       <c r="G29" s="26"/>
@@ -11890,7 +11890,7 @@
       </c>
       <c r="D30" s="21"/>
       <c r="E30" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>479</v>
@@ -11995,7 +11995,7 @@
       </c>
       <c r="D31" s="21"/>
       <c r="E31" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="DG31" s="26"/>
       <c r="DH31" s="26"/>
@@ -12013,7 +12013,7 @@
       </c>
       <c r="D32" s="21"/>
       <c r="E32" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="L32" s="21" t="s">
         <v>419</v>
@@ -12198,7 +12198,7 @@
       </c>
       <c r="D33" s="21"/>
       <c r="E33" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F33" s="49" t="s">
         <v>425</v>
@@ -12342,7 +12342,7 @@
       </c>
       <c r="D34" s="21"/>
       <c r="E34" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F34" s="49" t="s">
         <v>425</v>
@@ -12481,7 +12481,7 @@
       </c>
       <c r="D35" s="21"/>
       <c r="E35" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F35" s="24" t="s">
         <v>430</v>
@@ -12676,7 +12676,7 @@
       </c>
       <c r="D36" s="21"/>
       <c r="E36" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F36" s="49" t="s">
         <v>434</v>
@@ -12700,7 +12700,7 @@
       </c>
       <c r="D37" s="21"/>
       <c r="E37" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F37" s="49" t="s">
         <v>425</v>
@@ -12727,7 +12727,7 @@
       </c>
       <c r="D38" s="21"/>
       <c r="E38" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F38" s="49" t="s">
         <v>438</v>
@@ -12751,7 +12751,7 @@
       </c>
       <c r="D39" s="21"/>
       <c r="E39" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F39" s="49" t="s">
         <v>483</v>
@@ -12965,7 +12965,7 @@
         <v>27</v>
       </c>
       <c r="E40" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F40" s="49" t="s">
         <v>438</v>
@@ -12989,7 +12989,7 @@
       </c>
       <c r="D41" s="21"/>
       <c r="E41" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F41" s="21"/>
       <c r="G41" s="21"/>
@@ -13186,7 +13186,7 @@
       </c>
       <c r="D42" s="21"/>
       <c r="E42" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F42" s="26"/>
       <c r="G42" s="26"/>
@@ -13204,7 +13204,7 @@
         <v>4</v>
       </c>
       <c r="Q42" s="22" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="R42" s="23" t="s">
         <v>339</v>
@@ -13233,17 +13233,17 @@
         <v>29</v>
       </c>
       <c r="AF42" s="22" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="AG42" s="22" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="AH42" s="26"/>
       <c r="AI42" s="21" t="s">
         <v>401</v>
       </c>
       <c r="AJ42" s="22" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="AK42" s="26"/>
       <c r="AL42" s="21" t="s">
@@ -13256,7 +13256,7 @@
         <v>36</v>
       </c>
       <c r="AO42" s="22" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="AP42" s="22" t="s">
         <v>76</v>
@@ -13265,7 +13265,7 @@
         <v>76</v>
       </c>
       <c r="AR42" s="22" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="AS42" s="26"/>
       <c r="AT42" s="26"/>
@@ -13343,10 +13343,10 @@
         <v>326</v>
       </c>
       <c r="CX42" s="22" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="CY42" s="22" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="CZ42" s="23" t="s">
         <v>255</v>
@@ -13362,7 +13362,7 @@
         <v>76</v>
       </c>
       <c r="DE42" s="22" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="DF42" s="88" t="s">
         <v>356</v>
@@ -13383,7 +13383,7 @@
       </c>
       <c r="D43" s="21"/>
       <c r="E43" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F43" s="21"/>
       <c r="G43" s="21"/>
@@ -13430,7 +13430,7 @@
         <v>23</v>
       </c>
       <c r="AD43" s="24" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="AE43" s="21" t="s">
         <v>29</v>
@@ -13564,7 +13564,7 @@
       </c>
       <c r="D44" s="21"/>
       <c r="E44" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="DG44" s="26"/>
       <c r="DH44" s="26"/>
@@ -13582,7 +13582,7 @@
       </c>
       <c r="D45" s="21"/>
       <c r="E45" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F45" s="21"/>
       <c r="G45" s="21"/>
@@ -13629,7 +13629,7 @@
         <v>23</v>
       </c>
       <c r="AD45" s="24" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="AE45" s="21" t="s">
         <v>29</v>
@@ -13766,7 +13766,7 @@
       </c>
       <c r="D46" s="21"/>
       <c r="E46" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F46" s="21"/>
       <c r="G46" s="21"/>
@@ -13815,7 +13815,7 @@
         <v>23</v>
       </c>
       <c r="AD46" s="24" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="AE46" s="21" t="s">
         <v>29</v>
@@ -13955,7 +13955,7 @@
       </c>
       <c r="D47" s="21"/>
       <c r="E47" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F47" s="49" t="s">
         <v>460</v>
@@ -13987,7 +13987,7 @@
       </c>
       <c r="D48" s="21"/>
       <c r="E48" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F48" s="49" t="s">
         <v>460</v>
@@ -14008,7 +14008,7 @@
       </c>
       <c r="D49" s="21"/>
       <c r="E49" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F49" s="49" t="s">
         <v>460</v>
@@ -14029,7 +14029,7 @@
       </c>
       <c r="D50" s="21"/>
       <c r="E50" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F50" s="49"/>
       <c r="DG50" s="26"/>
@@ -14050,7 +14050,7 @@
       </c>
       <c r="D51" s="21"/>
       <c r="E51" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F51" s="49" t="s">
         <v>470</v>
@@ -14074,7 +14074,7 @@
       </c>
       <c r="D52" s="21"/>
       <c r="E52" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F52" s="26"/>
       <c r="G52" s="26"/>
@@ -14277,7 +14277,7 @@
       </c>
       <c r="D53" s="21"/>
       <c r="E53" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F53" s="21"/>
       <c r="G53" s="21"/>
@@ -14474,7 +14474,7 @@
       </c>
       <c r="D54" s="21"/>
       <c r="E54" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F54" s="24" t="s">
         <v>475</v>
@@ -14664,7 +14664,7 @@
       </c>
       <c r="D55" s="21"/>
       <c r="E55" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F55" s="49" t="s">
         <v>478</v>
@@ -14685,7 +14685,7 @@
       </c>
       <c r="D56" s="21"/>
       <c r="E56" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F56" s="49" t="s">
         <v>475</v>
@@ -14706,7 +14706,7 @@
       </c>
       <c r="D57" s="21"/>
       <c r="E57" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F57" s="49" t="s">
         <v>475</v>
@@ -14869,7 +14869,7 @@
       </c>
       <c r="D58" s="21"/>
       <c r="E58" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F58" s="49" t="s">
         <v>486</v>
@@ -14893,7 +14893,7 @@
       </c>
       <c r="D59" s="21"/>
       <c r="E59" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F59" s="21"/>
       <c r="G59" s="21"/>
@@ -15093,7 +15093,7 @@
       </c>
       <c r="D60" s="21"/>
       <c r="E60" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F60" s="49" t="s">
         <v>491</v>
@@ -15116,7 +15116,7 @@
         <v>83</v>
       </c>
       <c r="E61" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F61" s="24" t="s">
         <v>494</v>
@@ -15308,7 +15308,7 @@
         <v>83</v>
       </c>
       <c r="E62" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F62" s="49" t="s">
         <v>497</v>
@@ -15522,7 +15522,7 @@
         <v>83</v>
       </c>
       <c r="E63" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F63" s="49" t="s">
         <v>497</v>
@@ -15676,7 +15676,7 @@
         <v>83</v>
       </c>
       <c r="E64" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F64" s="49" t="s">
         <v>501</v>
@@ -15696,7 +15696,7 @@
         <v>83</v>
       </c>
       <c r="E65" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F65" s="49" t="s">
         <v>497</v>
@@ -15717,7 +15717,7 @@
       </c>
       <c r="D66" s="21"/>
       <c r="E66" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F66" s="21"/>
       <c r="G66" s="21"/>
@@ -15908,7 +15908,7 @@
         <v>83</v>
       </c>
       <c r="E67" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F67" s="49" t="s">
         <v>506</v>
@@ -15929,7 +15929,7 @@
       </c>
       <c r="D68" s="21"/>
       <c r="E68" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F68" s="21"/>
       <c r="G68" s="21"/>
@@ -16118,7 +16118,7 @@
       </c>
       <c r="D69" s="21"/>
       <c r="E69" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F69" s="21"/>
       <c r="G69" s="21"/>
@@ -16307,7 +16307,7 @@
       </c>
       <c r="D70" s="21"/>
       <c r="E70" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F70" s="21"/>
       <c r="G70" s="21"/>
@@ -16505,7 +16505,7 @@
         <v>27</v>
       </c>
       <c r="E71" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F71" s="49" t="s">
         <v>483</v>
@@ -16525,7 +16525,7 @@
         <v>83</v>
       </c>
       <c r="E72" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F72" s="49" t="s">
         <v>497</v>
@@ -16547,7 +16547,7 @@
       </c>
       <c r="D73" s="28"/>
       <c r="E73" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F73" s="28"/>
       <c r="G73" s="28"/>
@@ -16734,7 +16734,7 @@
       </c>
       <c r="D74" s="26"/>
       <c r="E74" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F74" s="39" t="s">
         <v>560</v>
@@ -16894,7 +16894,7 @@
       </c>
       <c r="D75" s="28"/>
       <c r="E75" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F75" s="28"/>
       <c r="G75" s="28"/>
@@ -17075,7 +17075,7 @@
       </c>
       <c r="D76" s="28"/>
       <c r="E76" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F76" s="28"/>
       <c r="G76" s="28"/>
@@ -17248,7 +17248,7 @@
       </c>
       <c r="D77" s="28"/>
       <c r="E77" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F77" s="28"/>
       <c r="G77" s="28"/>
@@ -17413,7 +17413,7 @@
       </c>
       <c r="D78" s="21"/>
       <c r="E78" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F78" s="21"/>
       <c r="G78" s="21"/>
@@ -17594,7 +17594,7 @@
       </c>
       <c r="D79" s="21"/>
       <c r="E79" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F79" s="21"/>
       <c r="G79" s="21"/>
@@ -17775,7 +17775,7 @@
       </c>
       <c r="D80" s="21"/>
       <c r="E80" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F80" s="21"/>
       <c r="G80" s="21"/>
@@ -17902,7 +17902,7 @@
       </c>
       <c r="D81" s="21"/>
       <c r="E81" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F81" s="21"/>
       <c r="G81" s="21"/>
@@ -18029,7 +18029,7 @@
       </c>
       <c r="D82" s="21"/>
       <c r="E82" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F82" s="21"/>
       <c r="G82" s="21"/>
@@ -18194,7 +18194,7 @@
       </c>
       <c r="D83" s="21"/>
       <c r="E83" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F83" s="21"/>
       <c r="G83" s="21"/>
@@ -18363,7 +18363,7 @@
       </c>
       <c r="D84" s="21"/>
       <c r="E84" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F84" s="21"/>
       <c r="G84" s="21"/>
@@ -18506,7 +18506,7 @@
       </c>
       <c r="D85" s="21"/>
       <c r="E85" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F85" s="21"/>
       <c r="G85" s="21"/>
@@ -18675,7 +18675,7 @@
       </c>
       <c r="D86" s="21"/>
       <c r="E86" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F86" s="24" t="s">
         <v>612</v>
@@ -18812,7 +18812,7 @@
       </c>
       <c r="D87" s="21"/>
       <c r="E87" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F87" s="24" t="s">
         <v>619</v>
@@ -18947,10 +18947,10 @@
       </c>
       <c r="D88" s="21"/>
       <c r="E88" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F88" s="24" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="G88" s="24"/>
       <c r="H88" s="24"/>
@@ -19080,7 +19080,7 @@
       </c>
       <c r="D89" s="21"/>
       <c r="E89" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F89" s="24" t="s">
         <v>635</v>
@@ -19251,7 +19251,7 @@
       </c>
       <c r="D90" s="21"/>
       <c r="E90" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="F90" s="21"/>
       <c r="G90" s="21"/>
@@ -19443,8 +19443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D073B921-24DF-4F78-BD1E-1984D65F897D}">
   <dimension ref="A1:BL29"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="X16" sqref="X16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19706,7 +19706,7 @@
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="H2" s="13" t="s">
         <v>46</v>
@@ -19798,7 +19798,7 @@
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
       <c r="G3" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="H3" s="13" t="s">
         <v>46</v>
@@ -19892,7 +19892,7 @@
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="G4" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="H4" s="13" t="s">
         <v>46</v>
@@ -19988,7 +19988,7 @@
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
       <c r="G5" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="H5" s="13" t="s">
         <v>46</v>
@@ -20080,7 +20080,7 @@
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
       <c r="G6" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="H6" s="13" t="s">
         <v>46</v>
@@ -20178,7 +20178,7 @@
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
       <c r="G7" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="H7" s="13" t="s">
         <v>46</v>
@@ -20276,7 +20276,7 @@
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
       <c r="G8" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="H8" s="13" t="s">
         <v>46</v>
@@ -20366,7 +20366,7 @@
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
       <c r="G9" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="H9" s="13" t="s">
         <v>46</v>
@@ -20468,7 +20468,7 @@
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
       <c r="G10" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="H10" s="13" t="s">
         <v>46</v>
@@ -20562,7 +20562,7 @@
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
       <c r="G11" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="H11" s="13" t="s">
         <v>46</v>
@@ -20652,7 +20652,7 @@
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
       <c r="G12" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="H12" s="13" t="s">
         <v>46</v>
@@ -20684,17 +20684,17 @@
       </c>
       <c r="V12" s="13"/>
       <c r="W12" s="15" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="X12" s="15" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="Y12" s="15"/>
       <c r="Z12" s="15" t="s">
         <v>169</v>
       </c>
       <c r="AA12" s="13" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="AB12" s="13"/>
       <c r="AC12" s="13"/>
@@ -20750,7 +20750,7 @@
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
       <c r="G13" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="H13" s="13" t="s">
         <v>46</v>
@@ -20782,10 +20782,10 @@
       </c>
       <c r="V13" s="13"/>
       <c r="W13" s="15" t="s">
+        <v>687</v>
+      </c>
+      <c r="X13" s="15" t="s">
         <v>688</v>
-      </c>
-      <c r="X13" s="15" t="s">
-        <v>689</v>
       </c>
       <c r="Y13" s="15" t="s">
         <v>21</v>
@@ -20794,7 +20794,7 @@
         <v>175</v>
       </c>
       <c r="AA13" s="13" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="AB13" s="13"/>
       <c r="AC13" s="13"/>
@@ -20848,7 +20848,7 @@
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
       <c r="G14" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="H14" s="13" t="s">
         <v>46</v>
@@ -20944,7 +20944,7 @@
       <c r="E15" s="34"/>
       <c r="F15" s="34"/>
       <c r="G15" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="H15" s="34" t="s">
         <v>46</v>
@@ -21094,7 +21094,7 @@
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
       <c r="G16" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="H16" s="13" t="s">
         <v>46</v>
@@ -21204,7 +21204,7 @@
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
       <c r="G17" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="H17" s="13" t="s">
         <v>46</v>
@@ -21302,7 +21302,7 @@
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
       <c r="G18" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="H18" s="13" t="s">
         <v>46</v>
@@ -21398,7 +21398,7 @@
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
       <c r="G19" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="W19" s="57" t="s">
         <v>519</v>
@@ -21426,7 +21426,7 @@
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="W20" s="57" t="s">
         <v>520</v>
@@ -21454,7 +21454,7 @@
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
       <c r="G21" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="W21" s="57" t="s">
         <v>523</v>
@@ -21482,7 +21482,7 @@
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
       <c r="G22" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="W22" s="57" t="s">
         <v>523</v>
@@ -21514,7 +21514,7 @@
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
       <c r="G23" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="H23" s="13" t="s">
         <v>46</v>
@@ -21624,7 +21624,7 @@
       <c r="E24" s="13"/>
       <c r="F24" s="13"/>
       <c r="G24" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="H24" s="13" t="s">
         <v>46</v>
@@ -21734,7 +21734,7 @@
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
       <c r="G25" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="H25" s="13" t="s">
         <v>46</v>
@@ -21838,7 +21838,7 @@
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
       <c r="G26" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="M26" t="s">
         <v>571</v>
@@ -21866,7 +21866,7 @@
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
       <c r="G27" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="BE27" s="13"/>
       <c r="BF27" s="13"/>
@@ -21897,7 +21897,7 @@
         <v>27</v>
       </c>
       <c r="G28" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="BE28" s="13"/>
       <c r="BF28" s="13"/>
@@ -21930,7 +21930,7 @@
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
       <c r="G29" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="H29" s="13" t="s">
         <v>576</v>
@@ -22022,7 +22022,7 @@
   <dimension ref="A1:V10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22118,7 +22118,7 @@
         <v>27</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="E2" s="21"/>
       <c r="F2" s="13" t="s">
@@ -22159,7 +22159,7 @@
         <v>27</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="E3" s="21"/>
       <c r="F3" s="13" t="s">
@@ -22209,7 +22209,7 @@
         <v>27</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="E4" s="21"/>
       <c r="F4" s="13" t="s">
@@ -22256,7 +22256,7 @@
         <v>27</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="E5" s="21"/>
       <c r="F5" s="13" t="s">
@@ -22297,7 +22297,7 @@
         <v>27</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="E6" s="21"/>
       <c r="F6" s="13" t="s">
@@ -22338,7 +22338,7 @@
         <v>27</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="E7" s="47" t="s">
         <v>322</v>
@@ -22369,7 +22369,7 @@
         <v>27</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="E8" s="47" t="s">
         <v>322</v>
@@ -22400,7 +22400,7 @@
         <v>83</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13" t="s">
@@ -22447,7 +22447,7 @@
         <v>27</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>640</v>
+        <v>697</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13" t="s">
@@ -22497,15 +22497,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006150CD2B74865543AE839454BD4B5DC6" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a2ee5e546ec1836f671c2a05bfe6bfc8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0be14d6d-d8a1-45f7-9f98-2db40f8691c4" xmlns:ns3="567c5c99-f8da-409a-bc28-51b94ad9a241" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e7ff770c31624934d8e1a633c6fbe95" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -22739,6 +22730,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E980A1B9-8C22-45F7-8344-5E520FA354EB}">
   <ds:schemaRefs>
@@ -22748,16 +22748,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB0B3A61-2E64-4CE7-BDD4-6ECB945D22FD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64F77A26-17A6-43DF-A115-F9EC24E62EB0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -22775,4 +22765,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB0B3A61-2E64-4CE7-BDD4-6ECB945D22FD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>